<commit_message>
Partial addition to regular hero data.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13014" windowHeight="10610" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13014" windowHeight="10610"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="LUT" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">attributes!$A$1:$B$119</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">attributes!$A$1:$B$124</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="310">
   <si>
     <t>attributes</t>
   </si>
@@ -716,6 +716,249 @@
   </si>
   <si>
     <t>remove_debuffs_probability</t>
+  </si>
+  <si>
+    <t>cooldown_decrease_on_regular_attack_amount</t>
+  </si>
+  <si>
+    <t>cooldown_decrease_on_counter_attack_amount</t>
+  </si>
+  <si>
+    <t>cooldown_decrease_on_speed_attack_amount</t>
+  </si>
+  <si>
+    <t>evan_6_0</t>
+  </si>
+  <si>
+    <t>Multi Slash</t>
+  </si>
+  <si>
+    <t>Imperator Evan</t>
+  </si>
+  <si>
+    <t>Shield of Order</t>
+  </si>
+  <si>
+    <t>Volition</t>
+  </si>
+  <si>
+    <t>karin_6_0</t>
+  </si>
+  <si>
+    <t>Saint Karin</t>
+  </si>
+  <si>
+    <t>Heal</t>
+  </si>
+  <si>
+    <t>Resurrect</t>
+  </si>
+  <si>
+    <t>Blessing Resurrection</t>
+  </si>
+  <si>
+    <t>yuri_6_0</t>
+  </si>
+  <si>
+    <t>Explorer Yuri</t>
+  </si>
+  <si>
+    <t>Spirit Drain</t>
+  </si>
+  <si>
+    <t>Magic Orb</t>
+  </si>
+  <si>
+    <t>Fox Charm</t>
+  </si>
+  <si>
+    <t>stat_damage_output_increase_turns</t>
+  </si>
+  <si>
+    <t>stat_damage_output_increase_probability</t>
+  </si>
+  <si>
+    <t>li_6_0</t>
+  </si>
+  <si>
+    <t>Furious Monk  Li</t>
+  </si>
+  <si>
+    <t>Penta Palm</t>
+  </si>
+  <si>
+    <t>Iron Physique</t>
+  </si>
+  <si>
+    <t>Sign of Revenge</t>
+  </si>
+  <si>
+    <t>yui_6_0</t>
+  </si>
+  <si>
+    <t>Maestro Yui</t>
+  </si>
+  <si>
+    <t>Blessed Melody</t>
+  </si>
+  <si>
+    <t>Battle Melody</t>
+  </si>
+  <si>
+    <t>Battle Maestro</t>
+  </si>
+  <si>
+    <t>jupy_6_0</t>
+  </si>
+  <si>
+    <t>Piercing Arrow Jupy</t>
+  </si>
+  <si>
+    <t>Multi Shot</t>
+  </si>
+  <si>
+    <t>Sniping Stance</t>
+  </si>
+  <si>
+    <t>massively</t>
+  </si>
+  <si>
+    <t>Hawk Eye</t>
+  </si>
+  <si>
+    <t>hellenia_6_0</t>
+  </si>
+  <si>
+    <t>Flame Comet Hellenia</t>
+  </si>
+  <si>
+    <t>Celestial Light</t>
+  </si>
+  <si>
+    <t>Celestial Shield</t>
+  </si>
+  <si>
+    <t>stat_block_rate_decrease_turns</t>
+  </si>
+  <si>
+    <t>stat_block_rate_increase_turns</t>
+  </si>
+  <si>
+    <t>Valkyrie's Potential</t>
+  </si>
+  <si>
+    <t>stat_incoming_damage_decrease_probability</t>
+  </si>
+  <si>
+    <t>heavenia_6_0</t>
+  </si>
+  <si>
+    <t>Blue Meteor Heavenia</t>
+  </si>
+  <si>
+    <t>Judgment Sword</t>
+  </si>
+  <si>
+    <t>Ferocious Strike</t>
+  </si>
+  <si>
+    <t>Mana Capture</t>
+  </si>
+  <si>
+    <t>snipper_6_0</t>
+  </si>
+  <si>
+    <t>Veteran Hunter Snipper</t>
+  </si>
+  <si>
+    <t>Wild Shot</t>
+  </si>
+  <si>
+    <t>Death Sentence</t>
+  </si>
+  <si>
+    <t>Hunting Technique</t>
+  </si>
+  <si>
+    <t>ariel_6_0</t>
+  </si>
+  <si>
+    <t>Blessing of Light Ariel</t>
+  </si>
+  <si>
+    <t>Judgment of Light</t>
+  </si>
+  <si>
+    <t>Bright Light</t>
+  </si>
+  <si>
+    <t>buff_removal_probability</t>
+  </si>
+  <si>
+    <t>Blessing of God</t>
+  </si>
+  <si>
+    <t>stat_critical_rate_increase_probability</t>
+  </si>
+  <si>
+    <t>evan_6_1</t>
+  </si>
+  <si>
+    <t>evan_6_2</t>
+  </si>
+  <si>
+    <t>karin_6_1</t>
+  </si>
+  <si>
+    <t>karin_6_2</t>
+  </si>
+  <si>
+    <t>yuri_6_1</t>
+  </si>
+  <si>
+    <t>yuri_6_2</t>
+  </si>
+  <si>
+    <t>li_6_1</t>
+  </si>
+  <si>
+    <t>li_6_2</t>
+  </si>
+  <si>
+    <t>yui_6_1</t>
+  </si>
+  <si>
+    <t>yui_6_2</t>
+  </si>
+  <si>
+    <t>jupy_6_1</t>
+  </si>
+  <si>
+    <t>jupy_6_2</t>
+  </si>
+  <si>
+    <t>hellenia_6_1</t>
+  </si>
+  <si>
+    <t>hellenia_6_2</t>
+  </si>
+  <si>
+    <t>heavenia_6_1</t>
+  </si>
+  <si>
+    <t>heavenia_6_2</t>
+  </si>
+  <si>
+    <t>snipper_6_1</t>
+  </si>
+  <si>
+    <t>snipper_6_2</t>
+  </si>
+  <si>
+    <t>ariel_6_1</t>
+  </si>
+  <si>
+    <t>ariel_6_2</t>
   </si>
 </sst>
 </file>
@@ -1040,10 +1283,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:Y55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1637,6 +1880,24 @@
       <c r="J13">
         <v>25</v>
       </c>
+      <c r="K13" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="L13" t="s">
+        <v>117</v>
+      </c>
+      <c r="M13" t="s">
+        <v>226</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="O13" t="s">
+        <v>117</v>
+      </c>
+      <c r="P13" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -2059,6 +2320,963 @@
       </c>
       <c r="G25">
         <v>50</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I25" t="s">
+        <v>164</v>
+      </c>
+      <c r="J25" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>232</v>
+      </c>
+      <c r="B26" t="s">
+        <v>234</v>
+      </c>
+      <c r="C26" t="s">
+        <v>233</v>
+      </c>
+      <c r="D26">
+        <v>64</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F26" t="s">
+        <v>221</v>
+      </c>
+      <c r="G26">
+        <v>180</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I26" t="s">
+        <v>221</v>
+      </c>
+      <c r="J26">
+        <v>2</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L26" t="s">
+        <v>221</v>
+      </c>
+      <c r="M26" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>290</v>
+      </c>
+      <c r="B27" t="s">
+        <v>234</v>
+      </c>
+      <c r="C27" t="s">
+        <v>235</v>
+      </c>
+      <c r="D27">
+        <v>90</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F27" t="s">
+        <v>114</v>
+      </c>
+      <c r="G27">
+        <v>50</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I27" t="s">
+        <v>114</v>
+      </c>
+      <c r="J27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>291</v>
+      </c>
+      <c r="B28" t="s">
+        <v>234</v>
+      </c>
+      <c r="C28" t="s">
+        <v>236</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F28" t="s">
+        <v>117</v>
+      </c>
+      <c r="G28">
+        <v>50</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I28" t="s">
+        <v>117</v>
+      </c>
+      <c r="J28" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>237</v>
+      </c>
+      <c r="B29" t="s">
+        <v>238</v>
+      </c>
+      <c r="C29" t="s">
+        <v>239</v>
+      </c>
+      <c r="D29">
+        <v>58</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>116</v>
+      </c>
+      <c r="G29">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>292</v>
+      </c>
+      <c r="B30" t="s">
+        <v>238</v>
+      </c>
+      <c r="C30" t="s">
+        <v>240</v>
+      </c>
+      <c r="D30">
+        <v>140</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" t="s">
+        <v>116</v>
+      </c>
+      <c r="G30">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>293</v>
+      </c>
+      <c r="B31" t="s">
+        <v>238</v>
+      </c>
+      <c r="C31" t="s">
+        <v>241</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" t="s">
+        <v>117</v>
+      </c>
+      <c r="G31">
+        <v>5</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" t="s">
+        <v>114</v>
+      </c>
+      <c r="J31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>242</v>
+      </c>
+      <c r="B32" t="s">
+        <v>243</v>
+      </c>
+      <c r="C32" t="s">
+        <v>244</v>
+      </c>
+      <c r="D32">
+        <v>70</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F32" t="s">
+        <v>221</v>
+      </c>
+      <c r="G32">
+        <v>180</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I32" t="s">
+        <v>114</v>
+      </c>
+      <c r="J32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>294</v>
+      </c>
+      <c r="B33" t="s">
+        <v>243</v>
+      </c>
+      <c r="C33" t="s">
+        <v>245</v>
+      </c>
+      <c r="D33">
+        <v>70</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F33" t="s">
+        <v>164</v>
+      </c>
+      <c r="G33">
+        <v>80</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I33" t="s">
+        <v>164</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L33" t="s">
+        <v>164</v>
+      </c>
+      <c r="M33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>295</v>
+      </c>
+      <c r="B34" t="s">
+        <v>243</v>
+      </c>
+      <c r="C34" t="s">
+        <v>246</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" t="s">
+        <v>164</v>
+      </c>
+      <c r="G34">
+        <v>40</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I34" t="s">
+        <v>164</v>
+      </c>
+      <c r="J34" t="s">
+        <v>162</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L34" t="s">
+        <v>164</v>
+      </c>
+      <c r="M34" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>249</v>
+      </c>
+      <c r="B35" t="s">
+        <v>250</v>
+      </c>
+      <c r="C35" t="s">
+        <v>251</v>
+      </c>
+      <c r="D35">
+        <v>72</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F35" t="s">
+        <v>221</v>
+      </c>
+      <c r="G35">
+        <v>180</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I35" t="s">
+        <v>221</v>
+      </c>
+      <c r="J35">
+        <v>2</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L35" t="s">
+        <v>221</v>
+      </c>
+      <c r="M35" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>296</v>
+      </c>
+      <c r="B36" t="s">
+        <v>250</v>
+      </c>
+      <c r="C36" t="s">
+        <v>252</v>
+      </c>
+      <c r="D36">
+        <v>110</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" t="s">
+        <v>114</v>
+      </c>
+      <c r="G36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>297</v>
+      </c>
+      <c r="B37" t="s">
+        <v>250</v>
+      </c>
+      <c r="C37" t="s">
+        <v>253</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" t="s">
+        <v>114</v>
+      </c>
+      <c r="G37" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>254</v>
+      </c>
+      <c r="B38" t="s">
+        <v>255</v>
+      </c>
+      <c r="C38" t="s">
+        <v>256</v>
+      </c>
+      <c r="D38">
+        <v>82</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" t="s">
+        <v>117</v>
+      </c>
+      <c r="G38">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>298</v>
+      </c>
+      <c r="B39" t="s">
+        <v>255</v>
+      </c>
+      <c r="C39" t="s">
+        <v>257</v>
+      </c>
+      <c r="D39">
+        <v>142</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39" t="s">
+        <v>117</v>
+      </c>
+      <c r="G39">
+        <v>30</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I39" t="s">
+        <v>117</v>
+      </c>
+      <c r="J39">
+        <v>10</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L39" t="s">
+        <v>117</v>
+      </c>
+      <c r="M39">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>299</v>
+      </c>
+      <c r="B40" t="s">
+        <v>255</v>
+      </c>
+      <c r="C40" t="s">
+        <v>258</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="s">
+        <v>117</v>
+      </c>
+      <c r="G40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>259</v>
+      </c>
+      <c r="B41" t="s">
+        <v>260</v>
+      </c>
+      <c r="C41" t="s">
+        <v>261</v>
+      </c>
+      <c r="D41">
+        <v>74</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F41" t="s">
+        <v>221</v>
+      </c>
+      <c r="G41">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>300</v>
+      </c>
+      <c r="B42" t="s">
+        <v>260</v>
+      </c>
+      <c r="C42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D42">
+        <v>50</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F42" t="s">
+        <v>114</v>
+      </c>
+      <c r="G42" t="s">
+        <v>263</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I42" t="s">
+        <v>114</v>
+      </c>
+      <c r="J42">
+        <v>3</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L42" t="s">
+        <v>114</v>
+      </c>
+      <c r="M42" t="s">
+        <v>263</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O42" t="s">
+        <v>114</v>
+      </c>
+      <c r="P42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>301</v>
+      </c>
+      <c r="B43" t="s">
+        <v>260</v>
+      </c>
+      <c r="C43" t="s">
+        <v>264</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F43" t="s">
+        <v>117</v>
+      </c>
+      <c r="G43">
+        <v>50</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I43" t="s">
+        <v>117</v>
+      </c>
+      <c r="J43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>265</v>
+      </c>
+      <c r="B44" t="s">
+        <v>266</v>
+      </c>
+      <c r="C44" t="s">
+        <v>267</v>
+      </c>
+      <c r="D44">
+        <v>80</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F44" t="s">
+        <v>164</v>
+      </c>
+      <c r="G44">
+        <v>80</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I44" t="s">
+        <v>114</v>
+      </c>
+      <c r="J44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>302</v>
+      </c>
+      <c r="B45" t="s">
+        <v>266</v>
+      </c>
+      <c r="C45" t="s">
+        <v>268</v>
+      </c>
+      <c r="D45">
+        <v>85</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F45" t="s">
+        <v>114</v>
+      </c>
+      <c r="G45" t="s">
+        <v>162</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="I45" t="s">
+        <v>114</v>
+      </c>
+      <c r="J45">
+        <v>2</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L45" t="s">
+        <v>164</v>
+      </c>
+      <c r="M45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>303</v>
+      </c>
+      <c r="B46" t="s">
+        <v>266</v>
+      </c>
+      <c r="C46" t="s">
+        <v>271</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F46" t="s">
+        <v>117</v>
+      </c>
+      <c r="G46">
+        <v>30</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I46" t="s">
+        <v>114</v>
+      </c>
+      <c r="J46">
+        <v>40</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L46" t="s">
+        <v>114</v>
+      </c>
+      <c r="M46" t="s">
+        <v>226</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="O46" t="s">
+        <v>114</v>
+      </c>
+      <c r="P46" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>273</v>
+      </c>
+      <c r="B47" t="s">
+        <v>274</v>
+      </c>
+      <c r="C47" t="s">
+        <v>275</v>
+      </c>
+      <c r="D47">
+        <v>70</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F47" t="s">
+        <v>164</v>
+      </c>
+      <c r="G47">
+        <v>80</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I47" t="s">
+        <v>164</v>
+      </c>
+      <c r="J47">
+        <v>2</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L47" t="s">
+        <v>164</v>
+      </c>
+      <c r="M47" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>304</v>
+      </c>
+      <c r="B48" t="s">
+        <v>274</v>
+      </c>
+      <c r="C48" t="s">
+        <v>276</v>
+      </c>
+      <c r="D48">
+        <v>80</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F48" t="s">
+        <v>221</v>
+      </c>
+      <c r="G48">
+        <v>180</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="I48" t="s">
+        <v>221</v>
+      </c>
+      <c r="J48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>305</v>
+      </c>
+      <c r="B49" t="s">
+        <v>274</v>
+      </c>
+      <c r="C49" t="s">
+        <v>277</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" t="s">
+        <v>114</v>
+      </c>
+      <c r="G49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>278</v>
+      </c>
+      <c r="B50" t="s">
+        <v>279</v>
+      </c>
+      <c r="C50" t="s">
+        <v>280</v>
+      </c>
+      <c r="D50">
+        <v>82</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F50" t="s">
+        <v>164</v>
+      </c>
+      <c r="G50">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>306</v>
+      </c>
+      <c r="B51" t="s">
+        <v>279</v>
+      </c>
+      <c r="C51" t="s">
+        <v>281</v>
+      </c>
+      <c r="D51">
+        <v>62</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F51" t="s">
+        <v>221</v>
+      </c>
+      <c r="G51">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>307</v>
+      </c>
+      <c r="B52" t="s">
+        <v>279</v>
+      </c>
+      <c r="C52" t="s">
+        <v>282</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" t="s">
+        <v>114</v>
+      </c>
+      <c r="G52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>283</v>
+      </c>
+      <c r="B53" t="s">
+        <v>284</v>
+      </c>
+      <c r="C53" t="s">
+        <v>285</v>
+      </c>
+      <c r="D53">
+        <v>80</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F53" t="s">
+        <v>164</v>
+      </c>
+      <c r="G53">
+        <v>80</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I53" t="s">
+        <v>164</v>
+      </c>
+      <c r="J53">
+        <v>2</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L53" t="s">
+        <v>164</v>
+      </c>
+      <c r="M53" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>308</v>
+      </c>
+      <c r="B54" t="s">
+        <v>284</v>
+      </c>
+      <c r="C54" t="s">
+        <v>286</v>
+      </c>
+      <c r="D54">
+        <v>110</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F54" t="s">
+        <v>164</v>
+      </c>
+      <c r="G54">
+        <v>80</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="I54" t="s">
+        <v>164</v>
+      </c>
+      <c r="J54" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>309</v>
+      </c>
+      <c r="B55" t="s">
+        <v>284</v>
+      </c>
+      <c r="C55" t="s">
+        <v>288</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F55" t="s">
+        <v>117</v>
+      </c>
+      <c r="G55">
+        <v>50</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I55" t="s">
+        <v>117</v>
+      </c>
+      <c r="J55" t="s">
+        <v>226</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L55" t="s">
+        <v>117</v>
+      </c>
+      <c r="M55" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2082,7 +3300,37 @@
           <x14:formula1>
             <xm:f>attributes!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>K9:K1048576</xm:sqref>
+          <xm:sqref>N9:N1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>N2:N7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q2:Q1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>K2:K7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>W2:W1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -2094,37 +3342,7 @@
           <x14:formula1>
             <xm:f>attributes!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>W2:W1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>K2:K7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>Q2:Q1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>N2:N7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>N9:N1048576</xm:sqref>
+          <xm:sqref>K9:K1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2134,10 +3352,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B120"/>
+  <dimension ref="A1:B130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -2226,41 +3444,41 @@
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>287</v>
       </c>
       <c r="B11" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>230</v>
       </c>
       <c r="B12" t="s">
-        <v>154</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>229</v>
       </c>
       <c r="B13" t="s">
-        <v>154</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>231</v>
       </c>
       <c r="B14" t="s">
-        <v>154</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
         <v>154</v>
@@ -2268,7 +3486,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
         <v>154</v>
@@ -2276,47 +3494,47 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>192</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>193</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>192</v>
       </c>
       <c r="B21" t="s">
-        <v>151</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
         <v>151</v>
@@ -2324,7 +3542,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>151</v>
@@ -2332,7 +3550,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>193</v>
       </c>
       <c r="B24" t="s">
         <v>151</v>
@@ -2340,7 +3558,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
         <v>151</v>
@@ -2348,7 +3566,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
         <v>151</v>
@@ -2356,7 +3574,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
         <v>151</v>
@@ -2364,7 +3582,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s">
         <v>151</v>
@@ -2372,47 +3590,47 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B29" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>152</v>
@@ -2420,7 +3638,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>152</v>
@@ -2428,7 +3646,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>152</v>
@@ -2436,7 +3654,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B37" t="s">
         <v>152</v>
@@ -2444,7 +3662,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B38" t="s">
         <v>152</v>
@@ -2452,7 +3670,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B39" t="s">
         <v>152</v>
@@ -2460,7 +3678,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
         <v>152</v>
@@ -2468,7 +3686,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B41" t="s">
         <v>152</v>
@@ -2476,7 +3694,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B42" t="s">
         <v>152</v>
@@ -2484,7 +3702,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B43" t="s">
         <v>152</v>
@@ -2492,7 +3710,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B44" t="s">
         <v>152</v>
@@ -2500,7 +3718,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B45" t="s">
         <v>152</v>
@@ -2508,7 +3726,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B46" t="s">
         <v>152</v>
@@ -2516,7 +3734,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B47" t="s">
         <v>152</v>
@@ -2524,7 +3742,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="B48" t="s">
         <v>152</v>
@@ -2532,7 +3750,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>152</v>
@@ -2540,7 +3758,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="B50" t="s">
         <v>152</v>
@@ -2548,7 +3766,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>152</v>
@@ -2556,7 +3774,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="B52" t="s">
         <v>152</v>
@@ -2564,7 +3782,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="B53" t="s">
         <v>152</v>
@@ -2572,7 +3790,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="B54" t="s">
         <v>152</v>
@@ -2580,7 +3798,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="B55" t="s">
         <v>152</v>
@@ -2588,7 +3806,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B56" t="s">
         <v>152</v>
@@ -2596,7 +3814,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B57" t="s">
         <v>152</v>
@@ -2604,7 +3822,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B58" t="s">
         <v>152</v>
@@ -2612,7 +3830,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B59" t="s">
         <v>152</v>
@@ -2620,7 +3838,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B60" t="s">
         <v>152</v>
@@ -2628,7 +3846,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B61" t="s">
         <v>152</v>
@@ -2636,7 +3854,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B62" t="s">
         <v>152</v>
@@ -2644,7 +3862,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B63" t="s">
         <v>152</v>
@@ -2652,79 +3870,79 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="B64" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>194</v>
+        <v>97</v>
       </c>
       <c r="B65" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>227</v>
+        <v>98</v>
       </c>
       <c r="B66" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>228</v>
+        <v>99</v>
       </c>
       <c r="B67" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B68" t="s">
-        <v>6</v>
+        <v>195</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>5</v>
+        <v>194</v>
       </c>
       <c r="B69" t="s">
-        <v>2</v>
+        <v>195</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>156</v>
+        <v>227</v>
       </c>
       <c r="B70" t="s">
-        <v>2</v>
+        <v>195</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>157</v>
+        <v>228</v>
       </c>
       <c r="B71" t="s">
-        <v>2</v>
+        <v>195</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B72" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B73" t="s">
         <v>2</v>
@@ -2732,47 +3950,47 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="B74" t="s">
-        <v>195</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>55</v>
+        <v>157</v>
       </c>
       <c r="B75" t="s">
-        <v>155</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="B76" t="s">
-        <v>155</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="B77" t="s">
-        <v>155</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>51</v>
+        <v>171</v>
       </c>
       <c r="B78" t="s">
-        <v>155</v>
+        <v>195</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B79" t="s">
         <v>155</v>
@@ -2780,7 +3998,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B80" t="s">
         <v>155</v>
@@ -2788,7 +4006,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>58</v>
+        <v>269</v>
       </c>
       <c r="B81" t="s">
         <v>155</v>
@@ -2796,7 +4014,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>54</v>
+        <v>270</v>
       </c>
       <c r="B82" t="s">
         <v>155</v>
@@ -2804,7 +4022,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="B83" t="s">
         <v>155</v>
@@ -2812,7 +4030,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B84" t="s">
         <v>155</v>
@@ -2820,7 +4038,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B85" t="s">
         <v>155</v>
@@ -2828,7 +4046,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B86" t="s">
         <v>155</v>
@@ -2836,7 +4054,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="B87" t="s">
         <v>155</v>
@@ -2844,7 +4062,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>161</v>
+        <v>54</v>
       </c>
       <c r="B88" t="s">
         <v>155</v>
@@ -2852,7 +4070,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>160</v>
+        <v>75</v>
       </c>
       <c r="B89" t="s">
         <v>155</v>
@@ -2860,7 +4078,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>62</v>
+        <v>289</v>
       </c>
       <c r="B90" t="s">
         <v>155</v>
@@ -2868,7 +4086,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B91" t="s">
         <v>155</v>
@@ -2876,7 +4094,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B92" t="s">
         <v>155</v>
@@ -2884,7 +4102,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B93" t="s">
         <v>155</v>
@@ -2892,7 +4110,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B94" t="s">
         <v>155</v>
@@ -2900,7 +4118,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>65</v>
+        <v>248</v>
       </c>
       <c r="B95" t="s">
         <v>155</v>
@@ -2908,7 +4126,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>66</v>
+        <v>247</v>
       </c>
       <c r="B96" t="s">
         <v>155</v>
@@ -2916,7 +4134,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="B97" t="s">
         <v>155</v>
@@ -2924,7 +4142,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="B98" t="s">
         <v>155</v>
@@ -2932,7 +4150,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="B99" t="s">
         <v>155</v>
@@ -2940,7 +4158,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="B100" t="s">
         <v>155</v>
@@ -2948,7 +4166,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="B101" t="s">
         <v>155</v>
@@ -2956,7 +4174,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="B102" t="s">
         <v>155</v>
@@ -2964,7 +4182,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="B103" t="s">
         <v>155</v>
@@ -2972,15 +4190,15 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>108</v>
+        <v>159</v>
       </c>
       <c r="B104" t="s">
-        <v>155</v>
+        <v>195</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="B105" t="s">
         <v>155</v>
@@ -2988,7 +4206,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="B106" t="s">
         <v>155</v>
@@ -2996,7 +4214,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="B107" t="s">
         <v>155</v>
@@ -3004,7 +4222,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>82</v>
+        <v>272</v>
       </c>
       <c r="B108" t="s">
         <v>155</v>
@@ -3012,7 +4230,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="B109" t="s">
         <v>155</v>
@@ -3020,7 +4238,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>84</v>
+        <v>161</v>
       </c>
       <c r="B110" t="s">
         <v>155</v>
@@ -3028,7 +4246,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>67</v>
+        <v>160</v>
       </c>
       <c r="B111" t="s">
         <v>155</v>
@@ -3036,7 +4254,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="B112" t="s">
         <v>155</v>
@@ -3044,7 +4262,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="B113" t="s">
         <v>155</v>
@@ -3052,7 +4270,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="B114" t="s">
         <v>155</v>
@@ -3060,7 +4278,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="B115" t="s">
         <v>155</v>
@@ -3068,7 +4286,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B116" t="s">
         <v>155</v>
@@ -3076,7 +4294,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B117" t="s">
         <v>155</v>
@@ -3084,32 +4302,112 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="B118" t="s">
-        <v>195</v>
+        <v>155</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="B119" t="s">
-        <v>195</v>
+        <v>155</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>159</v>
+        <v>83</v>
       </c>
       <c r="B120" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>84</v>
+      </c>
+      <c r="B121" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>67</v>
+      </c>
+      <c r="B122" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>68</v>
+      </c>
+      <c r="B123" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>69</v>
+      </c>
+      <c r="B124" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>85</v>
+      </c>
+      <c r="B125" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>86</v>
+      </c>
+      <c r="B126" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>87</v>
+      </c>
+      <c r="B127" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>88</v>
+      </c>
+      <c r="B128" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>21</v>
+      </c>
+      <c r="B129" t="s">
         <v>195</v>
       </c>
     </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>17</v>
+      </c>
+      <c r="B130" t="s">
+        <v>195</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B119">
-    <sortState ref="A2:C123">
-      <sortCondition ref="A1:A123"/>
+  <autoFilter ref="A1:B124">
+    <sortState ref="A2:B125">
+      <sortCondition ref="A1:A119"/>
     </sortState>
   </autoFilter>
   <sortState ref="A2:B121">

</xml_diff>

<commit_message>
Cleaned up displace_bst_column() code.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13014" windowHeight="10610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13014" windowHeight="10610" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -1285,7 +1285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
@@ -3354,8 +3354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B130"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3374,263 +3374,263 @@
     </row>
     <row r="2" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>223</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>287</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>230</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>229</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>231</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>192</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B23" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>193</v>
+        <v>89</v>
       </c>
       <c r="B24" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="B25" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="B26" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="B27" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>100</v>
       </c>
       <c r="B29" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>95</v>
       </c>
       <c r="B31" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>96</v>
       </c>
       <c r="B32" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="B33" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="B34" t="s">
         <v>152</v>
@@ -3638,7 +3638,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="B35" t="s">
         <v>152</v>
@@ -3646,258 +3646,258 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>137</v>
       </c>
       <c r="B36" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="B38" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>136</v>
       </c>
       <c r="B40" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B41" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="B42" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>287</v>
       </c>
       <c r="B43" t="s">
-        <v>152</v>
+        <v>195</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B44" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B48" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="B49" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B50" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="B51" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>71</v>
+        <v>193</v>
       </c>
       <c r="B52" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="B53" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="B54" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>73</v>
+        <v>14</v>
       </c>
       <c r="B55" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
       <c r="B56" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>90</v>
+        <v>23</v>
       </c>
       <c r="B57" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="B58" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>92</v>
+        <v>19</v>
       </c>
       <c r="B59" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>93</v>
+        <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="B61" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>94</v>
+        <v>12</v>
       </c>
       <c r="B62" t="s">
-        <v>152</v>
+        <v>195</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>95</v>
+        <v>223</v>
       </c>
       <c r="B63" t="s">
-        <v>152</v>
+        <v>195</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>96</v>
+        <v>230</v>
       </c>
       <c r="B64" t="s">
-        <v>152</v>
+        <v>195</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>97</v>
+        <v>229</v>
       </c>
       <c r="B65" t="s">
-        <v>152</v>
+        <v>195</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>98</v>
+        <v>231</v>
       </c>
       <c r="B66" t="s">
-        <v>152</v>
+        <v>195</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>99</v>
+        <v>192</v>
       </c>
       <c r="B67" t="s">
-        <v>152</v>
+        <v>195</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -3934,47 +3934,47 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="B72" t="s">
-        <v>6</v>
+        <v>195</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>5</v>
+        <v>159</v>
       </c>
       <c r="B73" t="s">
-        <v>2</v>
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>156</v>
+        <v>21</v>
       </c>
       <c r="B74" t="s">
-        <v>2</v>
+        <v>195</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>157</v>
+        <v>17</v>
       </c>
       <c r="B75" t="s">
-        <v>2</v>
+        <v>195</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B76" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B77" t="s">
         <v>2</v>
@@ -3982,39 +3982,39 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="B78" t="s">
-        <v>195</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>55</v>
+        <v>157</v>
       </c>
       <c r="B79" t="s">
-        <v>155</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="B80" t="s">
-        <v>155</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>269</v>
+        <v>9</v>
       </c>
       <c r="B81" t="s">
-        <v>155</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>270</v>
+        <v>55</v>
       </c>
       <c r="B82" t="s">
         <v>155</v>
@@ -4022,7 +4022,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B83" t="s">
         <v>155</v>
@@ -4030,7 +4030,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>51</v>
+        <v>269</v>
       </c>
       <c r="B84" t="s">
         <v>155</v>
@@ -4038,7 +4038,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>56</v>
+        <v>270</v>
       </c>
       <c r="B85" t="s">
         <v>155</v>
@@ -4046,7 +4046,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B86" t="s">
         <v>155</v>
@@ -4054,7 +4054,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B87" t="s">
         <v>155</v>
@@ -4062,7 +4062,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B88" t="s">
         <v>155</v>
@@ -4070,7 +4070,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B89" t="s">
         <v>155</v>
@@ -4078,7 +4078,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>289</v>
+        <v>58</v>
       </c>
       <c r="B90" t="s">
         <v>155</v>
@@ -4086,7 +4086,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B91" t="s">
         <v>155</v>
@@ -4094,7 +4094,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B92" t="s">
         <v>155</v>
@@ -4102,7 +4102,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>61</v>
+        <v>289</v>
       </c>
       <c r="B93" t="s">
         <v>155</v>
@@ -4110,7 +4110,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="B94" t="s">
         <v>155</v>
@@ -4118,7 +4118,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>248</v>
+        <v>60</v>
       </c>
       <c r="B95" t="s">
         <v>155</v>
@@ -4126,7 +4126,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>247</v>
+        <v>61</v>
       </c>
       <c r="B96" t="s">
         <v>155</v>
@@ -4134,7 +4134,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="B97" t="s">
         <v>155</v>
@@ -4142,7 +4142,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>63</v>
+        <v>248</v>
       </c>
       <c r="B98" t="s">
         <v>155</v>
@@ -4150,7 +4150,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>64</v>
+        <v>247</v>
       </c>
       <c r="B99" t="s">
         <v>155</v>
@@ -4158,7 +4158,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B100" t="s">
         <v>155</v>
@@ -4166,7 +4166,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B101" t="s">
         <v>155</v>
@@ -4174,7 +4174,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B102" t="s">
         <v>155</v>
@@ -4182,7 +4182,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B103" t="s">
         <v>155</v>
@@ -4190,15 +4190,15 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>159</v>
+        <v>78</v>
       </c>
       <c r="B104" t="s">
-        <v>195</v>
+        <v>155</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="B105" t="s">
         <v>155</v>
@@ -4206,7 +4206,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="B106" t="s">
         <v>155</v>
@@ -4214,7 +4214,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B107" t="s">
         <v>155</v>
@@ -4222,7 +4222,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>272</v>
+        <v>103</v>
       </c>
       <c r="B108" t="s">
         <v>155</v>
@@ -4230,7 +4230,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B109" t="s">
         <v>155</v>
@@ -4238,7 +4238,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>161</v>
+        <v>272</v>
       </c>
       <c r="B110" t="s">
         <v>155</v>
@@ -4246,7 +4246,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>160</v>
+        <v>102</v>
       </c>
       <c r="B111" t="s">
         <v>155</v>
@@ -4254,7 +4254,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>105</v>
+        <v>161</v>
       </c>
       <c r="B112" t="s">
         <v>155</v>
@@ -4262,7 +4262,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>106</v>
+        <v>160</v>
       </c>
       <c r="B113" t="s">
         <v>155</v>
@@ -4270,7 +4270,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B114" t="s">
         <v>155</v>
@@ -4278,7 +4278,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B115" t="s">
         <v>155</v>
@@ -4286,7 +4286,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="B116" t="s">
         <v>155</v>
@@ -4294,7 +4294,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="B117" t="s">
         <v>155</v>
@@ -4302,7 +4302,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B118" t="s">
         <v>155</v>
@@ -4310,7 +4310,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B119" t="s">
         <v>155</v>
@@ -4318,7 +4318,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B120" t="s">
         <v>155</v>
@@ -4326,7 +4326,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B121" t="s">
         <v>155</v>
@@ -4334,7 +4334,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="B122" t="s">
         <v>155</v>
@@ -4342,7 +4342,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="B123" t="s">
         <v>155</v>
@@ -4350,7 +4350,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B124" t="s">
         <v>155</v>
@@ -4358,7 +4358,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="B125" t="s">
         <v>155</v>
@@ -4366,7 +4366,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B126" t="s">
         <v>155</v>
@@ -4374,7 +4374,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B127" t="s">
         <v>155</v>
@@ -4382,7 +4382,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B128" t="s">
         <v>155</v>
@@ -4390,24 +4390,24 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="B129" t="s">
-        <v>195</v>
+        <v>155</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="B130" t="s">
-        <v>195</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B124">
-    <sortState ref="A2:B125">
-      <sortCondition ref="A1:A119"/>
+    <sortState ref="A2:B130">
+      <sortCondition ref="B1:B124"/>
     </sortState>
   </autoFilter>
   <sortState ref="A2:B121">

</xml_diff>

<commit_message>
Added Sun Wukong, updated Yuri's skills.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -17,7 +17,7 @@
     <sheet name="LUT" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">attributes!$A$1:$B$129</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">attributes!$A$1:$B$130</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$AE$107</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1765" uniqueCount="598">
   <si>
     <t>attributes</t>
   </si>
@@ -1791,6 +1791,39 @@
   </si>
   <si>
     <t>heal_magic_attack_turns</t>
+  </si>
+  <si>
+    <t>wukong_6_0</t>
+  </si>
+  <si>
+    <t>Enlightened Warrior SunWukong</t>
+  </si>
+  <si>
+    <t>Jumbo Pole</t>
+  </si>
+  <si>
+    <t>attack_magical_with_piercing_probability</t>
+  </si>
+  <si>
+    <t>Split Image Strike</t>
+  </si>
+  <si>
+    <t>Final Avatar</t>
+  </si>
+  <si>
+    <t>summon_avatars_amount</t>
+  </si>
+  <si>
+    <t>summon_avatars_turns</t>
+  </si>
+  <si>
+    <t>summon_avatars_stat_original_fraction</t>
+  </si>
+  <si>
+    <t>wukong_6_1</t>
+  </si>
+  <si>
+    <t>wukong_6_2</t>
   </si>
 </sst>
 </file>
@@ -2115,10 +2148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE169"/>
+  <dimension ref="A1:AE172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H165" sqref="H165"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3362,6 +3395,15 @@
       <c r="G32">
         <v>180</v>
       </c>
+      <c r="H32" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="I32" t="s">
+        <v>202</v>
+      </c>
+      <c r="J32">
+        <v>100</v>
+      </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -7723,7 +7765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>559</v>
       </c>
@@ -7764,7 +7806,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>560</v>
       </c>
@@ -7787,7 +7829,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>564</v>
       </c>
@@ -7828,7 +7870,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>565</v>
       </c>
@@ -7860,7 +7902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>569</v>
       </c>
@@ -7901,7 +7943,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>570</v>
       </c>
@@ -7933,7 +7975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>574</v>
       </c>
@@ -7983,7 +8025,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>575</v>
       </c>
@@ -8033,7 +8075,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>576</v>
       </c>
@@ -8060,6 +8102,126 @@
       </c>
       <c r="J169">
         <v>100</v>
+      </c>
+    </row>
+    <row r="170" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>587</v>
+      </c>
+      <c r="B170" t="s">
+        <v>588</v>
+      </c>
+      <c r="C170" t="s">
+        <v>589</v>
+      </c>
+      <c r="D170">
+        <v>66</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F170" t="s">
+        <v>202</v>
+      </c>
+      <c r="G170">
+        <v>230</v>
+      </c>
+      <c r="H170" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="I170" t="s">
+        <v>202</v>
+      </c>
+      <c r="J170">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="171" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>596</v>
+      </c>
+      <c r="B171" t="s">
+        <v>588</v>
+      </c>
+      <c r="C171" t="s">
+        <v>591</v>
+      </c>
+      <c r="D171">
+        <v>80</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F171" t="s">
+        <v>102</v>
+      </c>
+      <c r="G171">
+        <v>150</v>
+      </c>
+      <c r="H171" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I171" t="s">
+        <v>102</v>
+      </c>
+      <c r="J171">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="172" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>597</v>
+      </c>
+      <c r="B172" t="s">
+        <v>588</v>
+      </c>
+      <c r="C172" t="s">
+        <v>592</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F172" t="s">
+        <v>97</v>
+      </c>
+      <c r="G172">
+        <v>50</v>
+      </c>
+      <c r="H172" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="I172" t="s">
+        <v>97</v>
+      </c>
+      <c r="J172">
+        <v>80</v>
+      </c>
+      <c r="K172" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="L172" t="s">
+        <v>97</v>
+      </c>
+      <c r="M172">
+        <v>4</v>
+      </c>
+      <c r="N172" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="O172" t="s">
+        <v>97</v>
+      </c>
+      <c r="P172">
+        <v>60</v>
+      </c>
+      <c r="Q172" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="R172" t="s">
+        <v>97</v>
+      </c>
+      <c r="S172">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -8562,11 +8724,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B135"/>
+  <dimension ref="A1:B139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B140" sqref="B140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -8593,7 +8755,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>583</v>
       </c>
       <c r="B3" t="s">
         <v>136</v>
@@ -8601,7 +8763,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>422</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>136</v>
@@ -8609,7 +8771,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>590</v>
       </c>
       <c r="B5" t="s">
         <v>136</v>
@@ -8617,7 +8779,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>422</v>
       </c>
       <c r="B6" t="s">
         <v>136</v>
@@ -8625,7 +8787,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>136</v>
@@ -8633,7 +8795,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>136</v>
@@ -8641,7 +8803,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>582</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
         <v>136</v>
@@ -8649,7 +8811,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B10" t="s">
         <v>136</v>
@@ -8657,15 +8819,15 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>176</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>204</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>176</v>
@@ -8673,23 +8835,23 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B13" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B14" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B15" t="s">
         <v>176</v>
@@ -8697,15 +8859,15 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>425</v>
+        <v>212</v>
       </c>
       <c r="B16" t="s">
-        <v>137</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B17" t="s">
         <v>137</v>
@@ -8713,7 +8875,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B18" t="s">
         <v>137</v>
@@ -8721,7 +8883,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>585</v>
+        <v>423</v>
       </c>
       <c r="B19" t="s">
         <v>137</v>
@@ -8737,31 +8899,31 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>584</v>
       </c>
       <c r="B21" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>173</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>134</v>
@@ -8769,7 +8931,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>174</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
         <v>134</v>
@@ -8777,7 +8939,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>174</v>
       </c>
       <c r="B26" t="s">
         <v>134</v>
@@ -8785,7 +8947,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
         <v>134</v>
@@ -8793,7 +8955,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
         <v>134</v>
@@ -8801,7 +8963,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s">
         <v>134</v>
@@ -8809,7 +8971,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B30" t="s">
         <v>134</v>
@@ -8817,7 +8979,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
         <v>134</v>
@@ -8825,7 +8987,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
         <v>134</v>
@@ -8833,31 +8995,31 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B33" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>424</v>
+        <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>424</v>
       </c>
       <c r="B36" t="s">
         <v>135</v>
@@ -8865,7 +9027,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B37" t="s">
         <v>135</v>
@@ -8873,7 +9035,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" t="s">
         <v>135</v>
@@ -8881,7 +9043,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B39" t="s">
         <v>135</v>
@@ -8889,7 +9051,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B40" t="s">
         <v>135</v>
@@ -8897,7 +9059,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B41" t="s">
         <v>135</v>
@@ -8905,7 +9067,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>288</v>
+        <v>27</v>
       </c>
       <c r="B42" t="s">
         <v>135</v>
@@ -8913,7 +9075,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B43" t="s">
         <v>135</v>
@@ -8921,7 +9083,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>28</v>
+        <v>287</v>
       </c>
       <c r="B44" t="s">
         <v>135</v>
@@ -8929,7 +9091,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B45" t="s">
         <v>135</v>
@@ -8937,7 +9099,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>290</v>
+        <v>29</v>
       </c>
       <c r="B46" t="s">
         <v>135</v>
@@ -8945,7 +9107,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B47" t="s">
         <v>135</v>
@@ -8953,7 +9115,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>30</v>
+        <v>289</v>
       </c>
       <c r="B48" t="s">
         <v>135</v>
@@ -8961,7 +9123,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B49" t="s">
         <v>135</v>
@@ -8969,7 +9131,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B50" t="s">
         <v>135</v>
@@ -8977,7 +9139,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B51" t="s">
         <v>135</v>
@@ -8985,7 +9147,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B52" t="s">
         <v>135</v>
@@ -8993,7 +9155,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="B53" t="s">
         <v>135</v>
@@ -9001,7 +9163,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B54" t="s">
         <v>135</v>
@@ -9009,7 +9171,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B55" t="s">
         <v>135</v>
@@ -9017,7 +9179,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B56" t="s">
         <v>135</v>
@@ -9025,7 +9187,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B57" t="s">
         <v>135</v>
@@ -9033,7 +9195,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B58" t="s">
         <v>135</v>
@@ -9041,7 +9203,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B59" t="s">
         <v>135</v>
@@ -9049,7 +9211,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B60" t="s">
         <v>135</v>
@@ -9057,7 +9219,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B61" t="s">
         <v>135</v>
@@ -9065,7 +9227,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>426</v>
+        <v>78</v>
       </c>
       <c r="B62" t="s">
         <v>135</v>
@@ -9073,7 +9235,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>79</v>
+        <v>426</v>
       </c>
       <c r="B63" t="s">
         <v>135</v>
@@ -9081,7 +9243,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B64" t="s">
         <v>135</v>
@@ -9089,7 +9251,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B65" t="s">
         <v>135</v>
@@ -9097,7 +9259,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B66" t="s">
         <v>135</v>
@@ -9105,7 +9267,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>306</v>
+        <v>82</v>
       </c>
       <c r="B67" t="s">
         <v>135</v>
@@ -9113,7 +9275,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B68" t="s">
         <v>135</v>
@@ -9121,7 +9283,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>83</v>
+        <v>305</v>
       </c>
       <c r="B69" t="s">
         <v>135</v>
@@ -9129,7 +9291,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B70" t="s">
         <v>135</v>
@@ -9137,15 +9299,15 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="B71" t="s">
-        <v>176</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>175</v>
+        <v>3</v>
       </c>
       <c r="B72" t="s">
         <v>176</v>
@@ -9153,7 +9315,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>208</v>
+        <v>175</v>
       </c>
       <c r="B73" t="s">
         <v>176</v>
@@ -9161,7 +9323,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B74" t="s">
         <v>176</v>
@@ -9169,15 +9331,15 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>363</v>
+        <v>209</v>
       </c>
       <c r="B75" t="s">
-        <v>2</v>
+        <v>176</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B76" t="s">
         <v>2</v>
@@ -9185,7 +9347,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>139</v>
+        <v>362</v>
       </c>
       <c r="B77" t="s">
         <v>2</v>
@@ -9193,7 +9355,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>581</v>
+        <v>139</v>
       </c>
       <c r="B78" t="s">
         <v>2</v>
@@ -9201,7 +9363,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>5</v>
+        <v>581</v>
       </c>
       <c r="B79" t="s">
         <v>2</v>
@@ -9209,7 +9371,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B80" t="s">
         <v>2</v>
@@ -9217,23 +9379,23 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>152</v>
+        <v>4</v>
       </c>
       <c r="B81" t="s">
-        <v>176</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>42</v>
+        <v>152</v>
       </c>
       <c r="B82" t="s">
-        <v>138</v>
+        <v>176</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>381</v>
+        <v>42</v>
       </c>
       <c r="B83" t="s">
         <v>138</v>
@@ -9241,7 +9403,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>249</v>
+        <v>381</v>
       </c>
       <c r="B84" t="s">
         <v>138</v>
@@ -9249,7 +9411,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>39</v>
+        <v>249</v>
       </c>
       <c r="B85" t="s">
         <v>138</v>
@@ -9257,7 +9419,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>250</v>
+        <v>39</v>
       </c>
       <c r="B86" t="s">
         <v>138</v>
@@ -9265,7 +9427,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>40</v>
+        <v>250</v>
       </c>
       <c r="B87" t="s">
         <v>138</v>
@@ -9273,7 +9435,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>336</v>
+        <v>40</v>
       </c>
       <c r="B88" t="s">
         <v>138</v>
@@ -9281,7 +9443,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B89" t="s">
         <v>138</v>
@@ -9289,7 +9451,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>38</v>
+        <v>338</v>
       </c>
       <c r="B90" t="s">
         <v>138</v>
@@ -9297,7 +9459,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>337</v>
+        <v>38</v>
       </c>
       <c r="B91" t="s">
         <v>138</v>
@@ -9305,7 +9467,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>43</v>
+        <v>337</v>
       </c>
       <c r="B92" t="s">
         <v>138</v>
@@ -9313,7 +9475,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B93" t="s">
         <v>138</v>
@@ -9321,7 +9483,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B94" t="s">
         <v>138</v>
@@ -9329,7 +9491,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B95" t="s">
         <v>138</v>
@@ -9337,7 +9499,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B96" t="s">
         <v>138</v>
@@ -9345,7 +9507,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B97" t="s">
         <v>138</v>
@@ -9353,7 +9515,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B98" t="s">
         <v>138</v>
@@ -9361,7 +9523,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B99" t="s">
         <v>138</v>
@@ -9369,7 +9531,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B100" t="s">
         <v>138</v>
@@ -9377,7 +9539,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>228</v>
+        <v>62</v>
       </c>
       <c r="B101" t="s">
         <v>138</v>
@@ -9385,7 +9547,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>49</v>
+        <v>228</v>
       </c>
       <c r="B102" t="s">
         <v>138</v>
@@ -9393,7 +9555,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B103" t="s">
         <v>138</v>
@@ -9401,7 +9563,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B104" t="s">
         <v>138</v>
@@ -9409,7 +9571,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B105" t="s">
         <v>138</v>
@@ -9417,7 +9579,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B106" t="s">
         <v>138</v>
@@ -9425,7 +9587,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B107" t="s">
         <v>138</v>
@@ -9433,7 +9595,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B108" t="s">
         <v>138</v>
@@ -9441,23 +9603,23 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>141</v>
+        <v>53</v>
       </c>
       <c r="B109" t="s">
-        <v>176</v>
+        <v>138</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>85</v>
+        <v>141</v>
       </c>
       <c r="B110" t="s">
-        <v>138</v>
+        <v>176</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>464</v>
+        <v>85</v>
       </c>
       <c r="B111" t="s">
         <v>138</v>
@@ -9465,7 +9627,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>86</v>
+        <v>464</v>
       </c>
       <c r="B112" t="s">
         <v>138</v>
@@ -9473,7 +9635,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B113" t="s">
         <v>138</v>
@@ -9481,7 +9643,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>143</v>
+        <v>87</v>
       </c>
       <c r="B114" t="s">
         <v>138</v>
@@ -9489,7 +9651,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>366</v>
+        <v>143</v>
       </c>
       <c r="B115" t="s">
         <v>138</v>
@@ -9497,7 +9659,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>142</v>
+        <v>366</v>
       </c>
       <c r="B116" t="s">
         <v>138</v>
@@ -9505,7 +9667,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>88</v>
+        <v>142</v>
       </c>
       <c r="B117" t="s">
         <v>138</v>
@@ -9513,7 +9675,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B118" t="s">
         <v>138</v>
@@ -9521,7 +9683,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B119" t="s">
         <v>138</v>
@@ -9529,7 +9691,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B120" t="s">
         <v>138</v>
@@ -9537,7 +9699,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="B121" t="s">
         <v>138</v>
@@ -9545,7 +9707,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B122" t="s">
         <v>138</v>
@@ -9553,7 +9715,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B123" t="s">
         <v>138</v>
@@ -9561,7 +9723,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B124" t="s">
         <v>138</v>
@@ -9569,7 +9731,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B125" t="s">
         <v>138</v>
@@ -9577,7 +9739,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B126" t="s">
         <v>138</v>
@@ -9585,7 +9747,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="B127" t="s">
         <v>138</v>
@@ -9593,7 +9755,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B128" t="s">
         <v>138</v>
@@ -9601,7 +9763,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B129" t="s">
         <v>138</v>
@@ -9609,7 +9771,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B130" t="s">
         <v>138</v>
@@ -9617,7 +9779,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>449</v>
+        <v>71</v>
       </c>
       <c r="B131" t="s">
         <v>138</v>
@@ -9625,7 +9787,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>72</v>
+        <v>449</v>
       </c>
       <c r="B132" t="s">
         <v>138</v>
@@ -9633,7 +9795,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B133" t="s">
         <v>138</v>
@@ -9641,24 +9803,56 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="B134" t="s">
-        <v>176</v>
+        <v>138</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>12</v>
+        <v>593</v>
       </c>
       <c r="B135" t="s">
         <v>176</v>
       </c>
     </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>595</v>
+      </c>
+      <c r="B136" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>594</v>
+      </c>
+      <c r="B137" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>15</v>
+      </c>
+      <c r="B138" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>12</v>
+      </c>
+      <c r="B139" t="s">
+        <v>176</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B129">
-    <sortState ref="A2:B134">
-      <sortCondition ref="A1:A128"/>
+  <autoFilter ref="A1:B130">
+    <sortState ref="A2:B139">
+      <sortCondition ref="A1:A130"/>
     </sortState>
   </autoFilter>
   <sortState ref="A2:B121">

</xml_diff>

<commit_message>
Work on modifier titling.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -1157,9 +1157,6 @@
     <t>ming_ming_6_2</t>
   </si>
   <si>
-    <t>Sprout's Friend Ming Ming</t>
-  </si>
-  <si>
     <t>Flight of the Bumblebee</t>
   </si>
   <si>
@@ -2361,6 +2358,9 @@
   </si>
   <si>
     <t>Contract With Demon (Baron)</t>
+  </si>
+  <si>
+    <t>Sprout's Friend MingMing</t>
   </si>
 </sst>
 </file>
@@ -2687,8 +2687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE246"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I240" sqref="I240"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3172,7 +3172,7 @@
         <v>206</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="O10" t="s">
         <v>96</v>
@@ -3604,7 +3604,7 @@
         <v>167</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F22" t="s">
         <v>99</v>
@@ -3797,7 +3797,7 @@
         <v>50</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>141</v>
+        <v>86</v>
       </c>
       <c r="I27" t="s">
         <v>96</v>
@@ -3849,7 +3849,7 @@
         <v>58</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F29" t="s">
         <v>98</v>
@@ -3872,7 +3872,7 @@
         <v>140</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F30" t="s">
         <v>98</v>
@@ -3901,7 +3901,7 @@
         <v>5</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="I31" t="s">
         <v>96</v>
@@ -4119,7 +4119,7 @@
         <v>82</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F38" t="s">
         <v>99</v>
@@ -4142,7 +4142,7 @@
         <v>142</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F39" t="s">
         <v>99</v>
@@ -4518,7 +4518,7 @@
         <v>85</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I50" t="s">
         <v>145</v>
@@ -4722,7 +4722,7 @@
         <v>62</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F56" t="s">
         <v>98</v>
@@ -4745,7 +4745,7 @@
         <v>82</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F57" t="s">
         <v>99</v>
@@ -4917,7 +4917,7 @@
         <v>82</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F62" t="s">
         <v>99</v>
@@ -5481,7 +5481,7 @@
         <v>345</v>
       </c>
       <c r="B77" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C77" t="s">
         <v>346</v>
@@ -5522,7 +5522,7 @@
         <v>347</v>
       </c>
       <c r="B78" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C78" t="s">
         <v>349</v>
@@ -5554,7 +5554,7 @@
         <v>348</v>
       </c>
       <c r="B79" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C79" t="s">
         <v>350</v>
@@ -5744,7 +5744,7 @@
         <v>120</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F84" t="s">
         <v>99</v>
@@ -5770,7 +5770,7 @@
         <v>359</v>
       </c>
       <c r="C85" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>140</v>
@@ -5929,10 +5929,10 @@
         <v>372</v>
       </c>
       <c r="B88" t="s">
+        <v>776</v>
+      </c>
+      <c r="C88" t="s">
         <v>375</v>
-      </c>
-      <c r="C88" t="s">
-        <v>376</v>
       </c>
       <c r="D88">
         <v>80</v>
@@ -5970,10 +5970,10 @@
         <v>373</v>
       </c>
       <c r="B89" t="s">
-        <v>375</v>
+        <v>776</v>
       </c>
       <c r="C89" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D89">
         <v>80</v>
@@ -5988,7 +5988,7 @@
         <v>80</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I89" t="s">
         <v>145</v>
@@ -6002,10 +6002,10 @@
         <v>374</v>
       </c>
       <c r="B90" t="s">
-        <v>375</v>
+        <v>776</v>
       </c>
       <c r="C90" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>38</v>
@@ -6040,13 +6040,13 @@
     </row>
     <row r="91" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>379</v>
+      </c>
+      <c r="B91" t="s">
+        <v>381</v>
+      </c>
+      <c r="C91" t="s">
         <v>380</v>
-      </c>
-      <c r="B91" t="s">
-        <v>382</v>
-      </c>
-      <c r="C91" t="s">
-        <v>381</v>
       </c>
       <c r="D91">
         <v>65</v>
@@ -6076,18 +6076,18 @@
         <v>201</v>
       </c>
       <c r="M91" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="92" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B92" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C92" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D92">
         <v>72</v>
@@ -6113,13 +6113,13 @@
     </row>
     <row r="93" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B93" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C93" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>12</v>
@@ -6163,13 +6163,13 @@
     </row>
     <row r="94" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B94" t="s">
+        <v>389</v>
+      </c>
+      <c r="C94" t="s">
         <v>390</v>
-      </c>
-      <c r="C94" t="s">
-        <v>391</v>
       </c>
       <c r="D94">
         <v>105</v>
@@ -6195,13 +6195,13 @@
     </row>
     <row r="95" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B95" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C95" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D95">
         <v>80</v>
@@ -6227,13 +6227,13 @@
     </row>
     <row r="96" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>388</v>
+      </c>
+      <c r="B96" t="s">
         <v>389</v>
       </c>
-      <c r="B96" t="s">
-        <v>390</v>
-      </c>
       <c r="C96" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>14</v>
@@ -6265,13 +6265,13 @@
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B97" t="s">
+        <v>396</v>
+      </c>
+      <c r="C97" t="s">
         <v>397</v>
-      </c>
-      <c r="C97" t="s">
-        <v>398</v>
       </c>
       <c r="D97">
         <v>90</v>
@@ -6297,13 +6297,13 @@
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B98" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C98" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D98">
         <v>74</v>
@@ -6320,13 +6320,13 @@
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>395</v>
+      </c>
+      <c r="B99" t="s">
         <v>396</v>
       </c>
-      <c r="B99" t="s">
-        <v>397</v>
-      </c>
       <c r="C99" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>53</v>
@@ -6358,13 +6358,13 @@
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B100" t="s">
+        <v>402</v>
+      </c>
+      <c r="C100" t="s">
         <v>403</v>
-      </c>
-      <c r="C100" t="s">
-        <v>404</v>
       </c>
       <c r="D100">
         <v>36</v>
@@ -6381,13 +6381,13 @@
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>401</v>
+      </c>
+      <c r="B101" t="s">
         <v>402</v>
       </c>
-      <c r="B101" t="s">
-        <v>403</v>
-      </c>
       <c r="C101" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>40</v>
@@ -6419,13 +6419,13 @@
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B102" t="s">
+        <v>408</v>
+      </c>
+      <c r="C102" t="s">
         <v>409</v>
-      </c>
-      <c r="C102" t="s">
-        <v>410</v>
       </c>
       <c r="D102">
         <v>74</v>
@@ -6442,13 +6442,13 @@
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B103" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C103" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D103">
         <v>150</v>
@@ -6465,13 +6465,13 @@
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>407</v>
+      </c>
+      <c r="B104" t="s">
         <v>408</v>
       </c>
-      <c r="B104" t="s">
-        <v>409</v>
-      </c>
       <c r="C104" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>8</v>
@@ -6485,13 +6485,13 @@
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B105" t="s">
+        <v>415</v>
+      </c>
+      <c r="C105" t="s">
         <v>416</v>
-      </c>
-      <c r="C105" t="s">
-        <v>417</v>
       </c>
       <c r="D105">
         <v>85</v>
@@ -6526,13 +6526,13 @@
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B106" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C106" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D106">
         <v>100</v>
@@ -6558,13 +6558,13 @@
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>414</v>
+      </c>
+      <c r="B107" t="s">
         <v>415</v>
       </c>
-      <c r="B107" t="s">
-        <v>416</v>
-      </c>
       <c r="C107" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>14</v>
@@ -6578,13 +6578,13 @@
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>424</v>
+      </c>
+      <c r="B108" t="s">
         <v>425</v>
       </c>
-      <c r="B108" t="s">
+      <c r="C108" t="s">
         <v>426</v>
-      </c>
-      <c r="C108" t="s">
-        <v>427</v>
       </c>
       <c r="D108">
         <v>72</v>
@@ -6619,13 +6619,13 @@
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B109" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C109" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D109">
         <v>70</v>
@@ -6642,13 +6642,13 @@
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B110" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C110" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>56</v>
@@ -6671,13 +6671,13 @@
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B111" t="s">
+        <v>434</v>
+      </c>
+      <c r="C111" t="s">
         <v>435</v>
-      </c>
-      <c r="C111" t="s">
-        <v>436</v>
       </c>
       <c r="D111">
         <v>48</v>
@@ -6712,13 +6712,13 @@
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B112" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C112" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D112">
         <v>102</v>
@@ -6747,16 +6747,16 @@
     </row>
     <row r="113" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>433</v>
+      </c>
+      <c r="B113" t="s">
         <v>434</v>
       </c>
-      <c r="B113" t="s">
-        <v>435</v>
-      </c>
       <c r="C113" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F113" t="s">
         <v>201</v>
@@ -6785,13 +6785,13 @@
     </row>
     <row r="114" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B114" t="s">
+        <v>441</v>
+      </c>
+      <c r="C114" t="s">
         <v>442</v>
-      </c>
-      <c r="C114" t="s">
-        <v>443</v>
       </c>
       <c r="D114">
         <v>80</v>
@@ -6826,13 +6826,13 @@
     </row>
     <row r="115" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B115" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C115" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D115">
         <v>120</v>
@@ -6849,16 +6849,16 @@
     </row>
     <row r="116" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>440</v>
+      </c>
+      <c r="B116" t="s">
         <v>441</v>
       </c>
-      <c r="B116" t="s">
-        <v>442</v>
-      </c>
       <c r="C116" t="s">
+        <v>444</v>
+      </c>
+      <c r="E116" s="1" t="s">
         <v>445</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>446</v>
       </c>
       <c r="F116" t="s">
         <v>96</v>
@@ -6896,19 +6896,19 @@
     </row>
     <row r="117" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>446</v>
+      </c>
+      <c r="B117" t="s">
         <v>447</v>
       </c>
-      <c r="B117" t="s">
-        <v>448</v>
-      </c>
       <c r="C117" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D117">
         <v>100</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F117" t="s">
         <v>99</v>
@@ -6917,7 +6917,7 @@
         <v>60</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I117" t="s">
         <v>99</v>
@@ -6928,13 +6928,13 @@
     </row>
     <row r="118" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B118" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C118" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D118">
         <v>102</v>
@@ -6960,13 +6960,13 @@
     </row>
     <row r="119" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B119" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C119" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>53</v>
@@ -7025,13 +7025,13 @@
     </row>
     <row r="120" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
+        <v>453</v>
+      </c>
+      <c r="B120" t="s">
         <v>454</v>
       </c>
-      <c r="B120" t="s">
-        <v>455</v>
-      </c>
       <c r="C120" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D120">
         <v>72</v>
@@ -7075,13 +7075,13 @@
     </row>
     <row r="121" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B121" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C121" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D121">
         <v>82</v>
@@ -7125,16 +7125,16 @@
     </row>
     <row r="122" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B122" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C122" t="s">
+        <v>459</v>
+      </c>
+      <c r="E122" s="1" t="s">
         <v>460</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>461</v>
       </c>
       <c r="F122" t="s">
         <v>99</v>
@@ -7145,13 +7145,13 @@
     </row>
     <row r="123" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B123" t="s">
+        <v>464</v>
+      </c>
+      <c r="C123" t="s">
         <v>465</v>
-      </c>
-      <c r="C123" t="s">
-        <v>466</v>
       </c>
       <c r="D123">
         <v>90</v>
@@ -7177,13 +7177,13 @@
     </row>
     <row r="124" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B124" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C124" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D124">
         <v>85</v>
@@ -7198,7 +7198,7 @@
         <v>80</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I124" t="s">
         <v>145</v>
@@ -7227,13 +7227,13 @@
     </row>
     <row r="125" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
+        <v>463</v>
+      </c>
+      <c r="B125" t="s">
         <v>464</v>
       </c>
-      <c r="B125" t="s">
-        <v>465</v>
-      </c>
       <c r="C125" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>12</v>
@@ -7254,7 +7254,7 @@
         <v>206</v>
       </c>
       <c r="K125" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="L125" t="s">
         <v>96</v>
@@ -7274,13 +7274,13 @@
     </row>
     <row r="126" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B126" t="s">
+        <v>469</v>
+      </c>
+      <c r="C126" t="s">
         <v>470</v>
-      </c>
-      <c r="C126" t="s">
-        <v>471</v>
       </c>
       <c r="D126">
         <v>44</v>
@@ -7297,19 +7297,19 @@
     </row>
     <row r="127" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
+        <v>468</v>
+      </c>
+      <c r="B127" t="s">
         <v>469</v>
       </c>
-      <c r="B127" t="s">
-        <v>470</v>
-      </c>
       <c r="C127" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D127">
         <v>132</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F127" t="s">
         <v>96</v>
@@ -7320,13 +7320,13 @@
     </row>
     <row r="128" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B128" t="s">
+        <v>474</v>
+      </c>
+      <c r="C128" t="s">
         <v>475</v>
-      </c>
-      <c r="C128" t="s">
-        <v>476</v>
       </c>
       <c r="D128">
         <v>44</v>
@@ -7343,13 +7343,13 @@
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
+        <v>473</v>
+      </c>
+      <c r="B129" t="s">
         <v>474</v>
       </c>
-      <c r="B129" t="s">
-        <v>475</v>
-      </c>
       <c r="C129" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D129">
         <v>54</v>
@@ -7366,13 +7366,13 @@
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B130" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C130" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D130">
         <v>44</v>
@@ -7389,13 +7389,13 @@
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
+        <v>478</v>
+      </c>
+      <c r="B131" t="s">
         <v>479</v>
       </c>
-      <c r="B131" t="s">
+      <c r="C131" t="s">
         <v>480</v>
-      </c>
-      <c r="C131" t="s">
-        <v>481</v>
       </c>
       <c r="D131">
         <v>54</v>
@@ -7421,13 +7421,13 @@
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B132" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C132" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D132">
         <v>48</v>
@@ -7444,19 +7444,19 @@
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B133" t="s">
+        <v>484</v>
+      </c>
+      <c r="C133" t="s">
         <v>485</v>
-      </c>
-      <c r="C133" t="s">
-        <v>486</v>
       </c>
       <c r="D133">
         <v>58</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F133" t="s">
         <v>96</v>
@@ -7467,16 +7467,16 @@
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
+        <v>483</v>
+      </c>
+      <c r="B134" t="s">
         <v>484</v>
       </c>
-      <c r="B134" t="s">
-        <v>485</v>
-      </c>
       <c r="C134" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F134" t="s">
         <v>96</v>
@@ -7487,13 +7487,13 @@
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B135" t="s">
+        <v>489</v>
+      </c>
+      <c r="C135" t="s">
         <v>490</v>
-      </c>
-      <c r="C135" t="s">
-        <v>491</v>
       </c>
       <c r="D135">
         <v>44</v>
@@ -7510,13 +7510,13 @@
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>488</v>
+      </c>
+      <c r="B136" t="s">
         <v>489</v>
       </c>
-      <c r="B136" t="s">
-        <v>490</v>
-      </c>
       <c r="C136" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D136">
         <v>54</v>
@@ -7542,13 +7542,13 @@
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B137" t="s">
+        <v>494</v>
+      </c>
+      <c r="C137" t="s">
         <v>495</v>
-      </c>
-      <c r="C137" t="s">
-        <v>496</v>
       </c>
       <c r="D137">
         <v>46</v>
@@ -7565,13 +7565,13 @@
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
+        <v>493</v>
+      </c>
+      <c r="B138" t="s">
         <v>494</v>
       </c>
-      <c r="B138" t="s">
-        <v>495</v>
-      </c>
       <c r="C138" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D138">
         <v>56</v>
@@ -7586,7 +7586,7 @@
         <v>100</v>
       </c>
       <c r="H138" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="I138" t="s">
         <v>201</v>
@@ -7597,13 +7597,13 @@
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B139" t="s">
+        <v>500</v>
+      </c>
+      <c r="C139" t="s">
         <v>501</v>
-      </c>
-      <c r="C139" t="s">
-        <v>502</v>
       </c>
       <c r="D139">
         <v>48</v>
@@ -7620,13 +7620,13 @@
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B140" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C140" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D140">
         <v>140</v>
@@ -7643,13 +7643,13 @@
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
+        <v>499</v>
+      </c>
+      <c r="B141" t="s">
         <v>500</v>
       </c>
-      <c r="B141" t="s">
-        <v>501</v>
-      </c>
       <c r="C141" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>70</v>
@@ -7672,13 +7672,13 @@
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>508</v>
+      </c>
+      <c r="B142" t="s">
         <v>509</v>
       </c>
-      <c r="B142" t="s">
-        <v>510</v>
-      </c>
       <c r="C142" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D142">
         <v>44</v>
@@ -7695,13 +7695,13 @@
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B143" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C143" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D143">
         <v>54</v>
@@ -7745,13 +7745,13 @@
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>513</v>
+      </c>
+      <c r="B144" t="s">
         <v>514</v>
       </c>
-      <c r="B144" t="s">
-        <v>515</v>
-      </c>
       <c r="C144" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D144">
         <v>54</v>
@@ -7766,7 +7766,7 @@
         <v>70</v>
       </c>
       <c r="H144" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I144" t="s">
         <v>201</v>
@@ -7795,13 +7795,13 @@
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B145" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C145" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D145">
         <v>64</v>
@@ -7816,7 +7816,7 @@
         <v>60</v>
       </c>
       <c r="H145" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I145" t="s">
         <v>145</v>
@@ -7845,13 +7845,13 @@
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B146" t="s">
+        <v>520</v>
+      </c>
+      <c r="C146" t="s">
         <v>521</v>
-      </c>
-      <c r="C146" t="s">
-        <v>522</v>
       </c>
       <c r="D146">
         <v>46</v>
@@ -7868,19 +7868,19 @@
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
+        <v>519</v>
+      </c>
+      <c r="B147" t="s">
         <v>520</v>
       </c>
-      <c r="B147" t="s">
-        <v>521</v>
-      </c>
       <c r="C147" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D147">
         <v>56</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F147" t="s">
         <v>96</v>
@@ -7891,13 +7891,13 @@
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
+        <v>523</v>
+      </c>
+      <c r="B148" t="s">
         <v>524</v>
       </c>
-      <c r="B148" t="s">
-        <v>525</v>
-      </c>
       <c r="C148" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D148">
         <v>56</v>
@@ -7932,13 +7932,13 @@
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B149" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C149" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D149">
         <v>56</v>
@@ -7953,7 +7953,7 @@
         <v>150</v>
       </c>
       <c r="H149" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I149" t="s">
         <v>201</v>
@@ -7982,13 +7982,13 @@
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
+        <v>528</v>
+      </c>
+      <c r="B150" t="s">
         <v>529</v>
       </c>
-      <c r="B150" t="s">
-        <v>530</v>
-      </c>
       <c r="C150" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D150">
         <v>56</v>
@@ -8014,13 +8014,13 @@
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B151" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C151" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D151">
         <v>56</v>
@@ -8055,13 +8055,13 @@
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B152" t="s">
+        <v>535</v>
+      </c>
+      <c r="C152" t="s">
         <v>536</v>
-      </c>
-      <c r="C152" t="s">
-        <v>537</v>
       </c>
       <c r="D152">
         <v>48</v>
@@ -8078,13 +8078,13 @@
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
+        <v>534</v>
+      </c>
+      <c r="B153" t="s">
         <v>535</v>
       </c>
-      <c r="B153" t="s">
-        <v>536</v>
-      </c>
       <c r="C153" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D153">
         <v>58</v>
@@ -8110,13 +8110,13 @@
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B154" t="s">
+        <v>541</v>
+      </c>
+      <c r="C154" t="s">
         <v>542</v>
-      </c>
-      <c r="C154" t="s">
-        <v>543</v>
       </c>
       <c r="D154">
         <v>62</v>
@@ -8142,13 +8142,13 @@
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B155" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C155" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D155">
         <v>72</v>
@@ -8165,13 +8165,13 @@
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
+        <v>540</v>
+      </c>
+      <c r="B156" t="s">
         <v>541</v>
       </c>
-      <c r="B156" t="s">
-        <v>542</v>
-      </c>
       <c r="C156" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>84</v>
@@ -8194,13 +8194,13 @@
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B157" t="s">
+        <v>547</v>
+      </c>
+      <c r="C157" t="s">
         <v>548</v>
-      </c>
-      <c r="C157" t="s">
-        <v>549</v>
       </c>
       <c r="D157">
         <v>54</v>
@@ -8215,7 +8215,7 @@
         <v>150</v>
       </c>
       <c r="H157" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I157" t="s">
         <v>201</v>
@@ -8244,13 +8244,13 @@
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>546</v>
+      </c>
+      <c r="B158" t="s">
         <v>547</v>
       </c>
-      <c r="B158" t="s">
-        <v>548</v>
-      </c>
       <c r="C158" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D158">
         <v>44</v>
@@ -8276,13 +8276,13 @@
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B159" t="s">
+        <v>552</v>
+      </c>
+      <c r="C159" t="s">
         <v>553</v>
-      </c>
-      <c r="C159" t="s">
-        <v>554</v>
       </c>
       <c r="D159">
         <v>46</v>
@@ -8299,13 +8299,13 @@
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
+        <v>551</v>
+      </c>
+      <c r="B160" t="s">
         <v>552</v>
       </c>
-      <c r="B160" t="s">
-        <v>553</v>
-      </c>
       <c r="C160" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D160">
         <v>56</v>
@@ -8349,13 +8349,13 @@
     </row>
     <row r="161" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B161" t="s">
+        <v>557</v>
+      </c>
+      <c r="C161" t="s">
         <v>558</v>
-      </c>
-      <c r="C161" t="s">
-        <v>559</v>
       </c>
       <c r="D161">
         <v>56</v>
@@ -8390,13 +8390,13 @@
     </row>
     <row r="162" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
+        <v>556</v>
+      </c>
+      <c r="B162" t="s">
         <v>557</v>
       </c>
-      <c r="B162" t="s">
-        <v>558</v>
-      </c>
       <c r="C162" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D162">
         <v>66</v>
@@ -8413,13 +8413,13 @@
     </row>
     <row r="163" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B163" t="s">
+        <v>562</v>
+      </c>
+      <c r="C163" t="s">
         <v>563</v>
-      </c>
-      <c r="C163" t="s">
-        <v>564</v>
       </c>
       <c r="D163">
         <v>48</v>
@@ -8454,13 +8454,13 @@
     </row>
     <row r="164" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
+        <v>561</v>
+      </c>
+      <c r="B164" t="s">
         <v>562</v>
       </c>
-      <c r="B164" t="s">
-        <v>563</v>
-      </c>
       <c r="C164" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D164">
         <v>58</v>
@@ -8486,13 +8486,13 @@
     </row>
     <row r="165" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B165" t="s">
+        <v>567</v>
+      </c>
+      <c r="C165" t="s">
         <v>568</v>
-      </c>
-      <c r="C165" t="s">
-        <v>569</v>
       </c>
       <c r="D165">
         <v>48</v>
@@ -8527,13 +8527,13 @@
     </row>
     <row r="166" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
+        <v>566</v>
+      </c>
+      <c r="B166" t="s">
         <v>567</v>
       </c>
-      <c r="B166" t="s">
-        <v>568</v>
-      </c>
       <c r="C166" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D166">
         <v>48</v>
@@ -8559,13 +8559,13 @@
     </row>
     <row r="167" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B167" t="s">
+        <v>573</v>
+      </c>
+      <c r="C167" t="s">
         <v>574</v>
-      </c>
-      <c r="C167" t="s">
-        <v>575</v>
       </c>
       <c r="D167">
         <v>64</v>
@@ -8609,13 +8609,13 @@
     </row>
     <row r="168" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B168" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C168" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D168">
         <v>70</v>
@@ -8659,13 +8659,13 @@
     </row>
     <row r="169" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
+        <v>572</v>
+      </c>
+      <c r="B169" t="s">
         <v>573</v>
       </c>
-      <c r="B169" t="s">
-        <v>574</v>
-      </c>
       <c r="C169" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E169" s="1" t="s">
         <v>35</v>
@@ -8677,7 +8677,7 @@
         <v>5</v>
       </c>
       <c r="H169" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="I169" t="s">
         <v>96</v>
@@ -8688,13 +8688,13 @@
     </row>
     <row r="170" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
+        <v>583</v>
+      </c>
+      <c r="B170" t="s">
         <v>584</v>
       </c>
-      <c r="B170" t="s">
+      <c r="C170" t="s">
         <v>585</v>
-      </c>
-      <c r="C170" t="s">
-        <v>586</v>
       </c>
       <c r="D170">
         <v>66</v>
@@ -8709,7 +8709,7 @@
         <v>230</v>
       </c>
       <c r="H170" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I170" t="s">
         <v>201</v>
@@ -8720,13 +8720,13 @@
     </row>
     <row r="171" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B171" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C171" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D171">
         <v>80</v>
@@ -8752,13 +8752,13 @@
     </row>
     <row r="172" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B172" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C172" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>66</v>
@@ -8770,7 +8770,7 @@
         <v>50</v>
       </c>
       <c r="H172" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="I172" t="s">
         <v>96</v>
@@ -8779,7 +8779,7 @@
         <v>80</v>
       </c>
       <c r="K172" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L172" t="s">
         <v>96</v>
@@ -8788,7 +8788,7 @@
         <v>4</v>
       </c>
       <c r="N172" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="O172" t="s">
         <v>96</v>
@@ -8797,7 +8797,7 @@
         <v>60</v>
       </c>
       <c r="Q172" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="R172" t="s">
         <v>96</v>
@@ -8808,13 +8808,13 @@
     </row>
     <row r="173" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
+        <v>594</v>
+      </c>
+      <c r="B173" t="s">
         <v>595</v>
       </c>
-      <c r="B173" t="s">
+      <c r="C173" t="s">
         <v>596</v>
-      </c>
-      <c r="C173" t="s">
-        <v>597</v>
       </c>
       <c r="D173">
         <v>48</v>
@@ -8831,13 +8831,13 @@
     </row>
     <row r="174" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B174" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C174" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D174">
         <v>58</v>
@@ -8863,13 +8863,13 @@
     </row>
     <row r="175" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
+        <v>599</v>
+      </c>
+      <c r="B175" t="s">
         <v>600</v>
       </c>
-      <c r="B175" t="s">
-        <v>601</v>
-      </c>
       <c r="C175" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D175">
         <v>58</v>
@@ -8904,13 +8904,13 @@
     </row>
     <row r="176" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B176" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C176" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D176">
         <v>58</v>
@@ -8936,13 +8936,13 @@
     </row>
     <row r="177" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
+        <v>605</v>
+      </c>
+      <c r="B177" t="s">
         <v>606</v>
       </c>
-      <c r="B177" t="s">
+      <c r="C177" t="s">
         <v>607</v>
-      </c>
-      <c r="C177" t="s">
-        <v>608</v>
       </c>
       <c r="D177">
         <v>48</v>
@@ -8959,13 +8959,13 @@
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B178" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C178" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D178">
         <v>58</v>
@@ -8991,13 +8991,13 @@
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
+        <v>610</v>
+      </c>
+      <c r="B179" t="s">
         <v>611</v>
       </c>
-      <c r="B179" t="s">
+      <c r="C179" t="s">
         <v>612</v>
-      </c>
-      <c r="C179" t="s">
-        <v>613</v>
       </c>
       <c r="D179">
         <v>62</v>
@@ -9032,13 +9032,13 @@
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B180" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C180" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D180">
         <v>72</v>
@@ -9053,7 +9053,7 @@
         <v>65</v>
       </c>
       <c r="H180" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I180" t="s">
         <v>145</v>
@@ -9082,16 +9082,16 @@
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B181" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C181" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F181" t="s">
         <v>96</v>
@@ -9102,13 +9102,13 @@
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
+        <v>617</v>
+      </c>
+      <c r="B182" t="s">
         <v>618</v>
       </c>
-      <c r="B182" t="s">
+      <c r="C182" t="s">
         <v>619</v>
-      </c>
-      <c r="C182" t="s">
-        <v>620</v>
       </c>
       <c r="D182">
         <v>56</v>
@@ -9134,13 +9134,13 @@
     </row>
     <row r="183" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B183" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C183" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D183">
         <v>66</v>
@@ -9166,13 +9166,13 @@
     </row>
     <row r="184" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B184" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C184" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>16</v>
@@ -9186,13 +9186,13 @@
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
+        <v>623</v>
+      </c>
+      <c r="B185" t="s">
         <v>624</v>
       </c>
-      <c r="B185" t="s">
+      <c r="C185" t="s">
         <v>625</v>
-      </c>
-      <c r="C185" t="s">
-        <v>626</v>
       </c>
       <c r="D185">
         <v>56</v>
@@ -9209,13 +9209,13 @@
     </row>
     <row r="186" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B186" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C186" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D186">
         <v>58</v>
@@ -9241,13 +9241,13 @@
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B187" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C187" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E187" s="1" t="s">
         <v>16</v>
@@ -9261,13 +9261,13 @@
     </row>
     <row r="188" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
+        <v>629</v>
+      </c>
+      <c r="B188" t="s">
         <v>630</v>
       </c>
-      <c r="B188" t="s">
+      <c r="C188" t="s">
         <v>631</v>
-      </c>
-      <c r="C188" t="s">
-        <v>632</v>
       </c>
       <c r="D188">
         <v>64</v>
@@ -9302,13 +9302,13 @@
     </row>
     <row r="189" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B189" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C189" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D189">
         <v>74</v>
@@ -9343,13 +9343,13 @@
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B190" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C190" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>41</v>
@@ -9361,7 +9361,7 @@
         <v>50</v>
       </c>
       <c r="H190" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I190" t="s">
         <v>145</v>
@@ -9381,13 +9381,13 @@
     </row>
     <row r="191" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
+        <v>636</v>
+      </c>
+      <c r="B191" t="s">
         <v>637</v>
       </c>
-      <c r="B191" t="s">
+      <c r="C191" t="s">
         <v>638</v>
-      </c>
-      <c r="C191" t="s">
-        <v>639</v>
       </c>
       <c r="D191">
         <v>48</v>
@@ -9404,13 +9404,13 @@
     </row>
     <row r="192" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B192" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C192" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D192">
         <v>58</v>
@@ -9427,13 +9427,13 @@
     </row>
     <row r="193" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
+        <v>640</v>
+      </c>
+      <c r="B193" t="s">
         <v>641</v>
       </c>
-      <c r="B193" t="s">
+      <c r="C193" t="s">
         <v>642</v>
-      </c>
-      <c r="C193" t="s">
-        <v>643</v>
       </c>
       <c r="D193">
         <v>58</v>
@@ -9468,13 +9468,13 @@
     </row>
     <row r="194" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B194" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C194" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D194">
         <v>48</v>
@@ -9489,7 +9489,7 @@
         <v>150</v>
       </c>
       <c r="H194" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I194" t="s">
         <v>201</v>
@@ -9518,13 +9518,13 @@
     </row>
     <row r="195" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
+        <v>645</v>
+      </c>
+      <c r="B195" t="s">
+        <v>644</v>
+      </c>
+      <c r="C195" t="s">
         <v>646</v>
-      </c>
-      <c r="B195" t="s">
-        <v>645</v>
-      </c>
-      <c r="C195" t="s">
-        <v>647</v>
       </c>
       <c r="D195">
         <v>48</v>
@@ -9541,13 +9541,13 @@
     </row>
     <row r="196" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B196" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C196" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D196">
         <v>68</v>
@@ -9564,13 +9564,13 @@
     </row>
     <row r="197" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
+        <v>648</v>
+      </c>
+      <c r="B197" t="s">
         <v>649</v>
       </c>
-      <c r="B197" t="s">
+      <c r="C197" t="s">
         <v>650</v>
-      </c>
-      <c r="C197" t="s">
-        <v>651</v>
       </c>
       <c r="D197">
         <v>60</v>
@@ -9605,13 +9605,13 @@
     </row>
     <row r="198" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B198" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C198" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D198">
         <v>70</v>
@@ -9646,13 +9646,13 @@
     </row>
     <row r="199" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
+        <v>652</v>
+      </c>
+      <c r="B199" t="s">
         <v>653</v>
       </c>
-      <c r="B199" t="s">
+      <c r="C199" t="s">
         <v>654</v>
-      </c>
-      <c r="C199" t="s">
-        <v>655</v>
       </c>
       <c r="D199">
         <v>62</v>
@@ -9678,13 +9678,13 @@
     </row>
     <row r="200" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B200" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C200" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D200">
         <v>72</v>
@@ -9710,16 +9710,16 @@
     </row>
     <row r="201" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B201" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C201" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F201" t="s">
         <v>96</v>
@@ -9730,13 +9730,13 @@
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
+        <v>657</v>
+      </c>
+      <c r="B202" t="s">
         <v>658</v>
       </c>
-      <c r="B202" t="s">
+      <c r="C202" t="s">
         <v>659</v>
-      </c>
-      <c r="C202" t="s">
-        <v>660</v>
       </c>
       <c r="D202">
         <v>64</v>
@@ -9771,13 +9771,13 @@
     </row>
     <row r="203" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B203" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C203" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D203">
         <v>94</v>
@@ -9812,13 +9812,13 @@
     </row>
     <row r="204" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B204" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C204" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>17</v>
@@ -9832,13 +9832,13 @@
     </row>
     <row r="205" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
+        <v>662</v>
+      </c>
+      <c r="B205" t="s">
         <v>663</v>
       </c>
-      <c r="B205" t="s">
+      <c r="C205" t="s">
         <v>664</v>
-      </c>
-      <c r="C205" t="s">
-        <v>665</v>
       </c>
       <c r="D205">
         <v>90</v>
@@ -9873,13 +9873,13 @@
     </row>
     <row r="206" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B206" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C206" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D206">
         <v>76</v>
@@ -9894,7 +9894,7 @@
         <v>80</v>
       </c>
       <c r="H206" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I206" t="s">
         <v>145</v>
@@ -9923,13 +9923,13 @@
     </row>
     <row r="207" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B207" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C207" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>18</v>
@@ -9943,13 +9943,13 @@
     </row>
     <row r="208" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
+        <v>667</v>
+      </c>
+      <c r="B208" t="s">
         <v>668</v>
       </c>
-      <c r="B208" t="s">
+      <c r="C208" t="s">
         <v>669</v>
-      </c>
-      <c r="C208" t="s">
-        <v>670</v>
       </c>
       <c r="D208">
         <v>58</v>
@@ -9984,13 +9984,13 @@
     </row>
     <row r="209" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B209" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C209" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="D209">
         <v>120</v>
@@ -10007,13 +10007,13 @@
     </row>
     <row r="210" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
+        <v>671</v>
+      </c>
+      <c r="B210" t="s">
         <v>672</v>
       </c>
-      <c r="B210" t="s">
+      <c r="C210" t="s">
         <v>673</v>
-      </c>
-      <c r="C210" t="s">
-        <v>674</v>
       </c>
       <c r="D210">
         <v>58</v>
@@ -10048,13 +10048,13 @@
     </row>
     <row r="211" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B211" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C211" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D211">
         <v>88</v>
@@ -10080,13 +10080,13 @@
     </row>
     <row r="212" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
+        <v>675</v>
+      </c>
+      <c r="B212" t="s">
         <v>676</v>
       </c>
-      <c r="B212" t="s">
+      <c r="C212" t="s">
         <v>677</v>
-      </c>
-      <c r="C212" t="s">
-        <v>678</v>
       </c>
       <c r="D212">
         <v>54</v>
@@ -10103,13 +10103,13 @@
     </row>
     <row r="213" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B213" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C213" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D213">
         <v>74</v>
@@ -10144,16 +10144,16 @@
     </row>
     <row r="214" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B214" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C214" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="F214" t="s">
         <v>96</v>
@@ -10162,7 +10162,7 @@
         <v>60</v>
       </c>
       <c r="H214" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="I214" t="s">
         <v>96</v>
@@ -10173,13 +10173,13 @@
     </row>
     <row r="215" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
+        <v>680</v>
+      </c>
+      <c r="B215" t="s">
         <v>681</v>
       </c>
-      <c r="B215" t="s">
+      <c r="C215" t="s">
         <v>682</v>
-      </c>
-      <c r="C215" t="s">
-        <v>683</v>
       </c>
       <c r="D215">
         <v>54</v>
@@ -10194,7 +10194,7 @@
         <v>170</v>
       </c>
       <c r="H215" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I215" t="s">
         <v>201</v>
@@ -10223,13 +10223,13 @@
     </row>
     <row r="216" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B216" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C216" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D216">
         <v>74</v>
@@ -10250,7 +10250,7 @@
         <v>145</v>
       </c>
       <c r="J216" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="K216" s="1" t="s">
         <v>49</v>
@@ -10273,13 +10273,13 @@
     </row>
     <row r="217" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B217" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C217" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E217" s="1" t="s">
         <v>29</v>
@@ -10302,13 +10302,13 @@
     </row>
     <row r="218" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
+        <v>686</v>
+      </c>
+      <c r="B218" t="s">
         <v>687</v>
       </c>
-      <c r="B218" t="s">
+      <c r="C218" t="s">
         <v>688</v>
-      </c>
-      <c r="C218" t="s">
-        <v>689</v>
       </c>
       <c r="D218">
         <v>62</v>
@@ -10343,13 +10343,13 @@
     </row>
     <row r="219" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B219" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C219" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D219">
         <v>62</v>
@@ -10375,13 +10375,13 @@
     </row>
     <row r="220" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B220" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C220" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E220" s="1" t="s">
         <v>34</v>
@@ -10404,13 +10404,13 @@
     </row>
     <row r="221" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
+        <v>691</v>
+      </c>
+      <c r="B221" t="s">
         <v>692</v>
       </c>
-      <c r="B221" t="s">
+      <c r="C221" t="s">
         <v>693</v>
-      </c>
-      <c r="C221" t="s">
-        <v>694</v>
       </c>
       <c r="D221">
         <v>52</v>
@@ -10427,13 +10427,13 @@
     </row>
     <row r="222" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B222" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C222" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D222">
         <v>62</v>
@@ -10468,13 +10468,13 @@
     </row>
     <row r="223" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B223" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C223" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E223" s="1" t="s">
         <v>19</v>
@@ -10488,13 +10488,13 @@
     </row>
     <row r="224" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
+        <v>696</v>
+      </c>
+      <c r="B224" t="s">
         <v>697</v>
       </c>
-      <c r="B224" t="s">
+      <c r="C224" t="s">
         <v>698</v>
-      </c>
-      <c r="C224" t="s">
-        <v>699</v>
       </c>
       <c r="D224">
         <v>74</v>
@@ -10529,13 +10529,13 @@
     </row>
     <row r="225" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B225" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C225" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D225">
         <v>90</v>
@@ -10570,13 +10570,13 @@
     </row>
     <row r="226" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B226" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C226" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E226" s="1" t="s">
         <v>19</v>
@@ -10608,13 +10608,13 @@
     </row>
     <row r="227" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
+        <v>701</v>
+      </c>
+      <c r="B227" t="s">
         <v>702</v>
       </c>
-      <c r="B227" t="s">
+      <c r="C227" t="s">
         <v>703</v>
-      </c>
-      <c r="C227" t="s">
-        <v>704</v>
       </c>
       <c r="D227">
         <v>60</v>
@@ -10649,13 +10649,13 @@
     </row>
     <row r="228" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B228" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C228" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D228">
         <v>90</v>
@@ -10681,13 +10681,13 @@
     </row>
     <row r="229" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
+        <v>705</v>
+      </c>
+      <c r="B229" t="s">
         <v>706</v>
       </c>
-      <c r="B229" t="s">
+      <c r="C229" t="s">
         <v>707</v>
-      </c>
-      <c r="C229" t="s">
-        <v>708</v>
       </c>
       <c r="D229">
         <v>62</v>
@@ -10722,13 +10722,13 @@
     </row>
     <row r="230" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B230" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C230" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D230">
         <v>140</v>
@@ -10745,13 +10745,13 @@
     </row>
     <row r="231" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B231" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C231" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E231" s="1" t="s">
         <v>87</v>
@@ -10774,13 +10774,13 @@
     </row>
     <row r="232" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
+        <v>709</v>
+      </c>
+      <c r="B232" t="s">
         <v>710</v>
       </c>
-      <c r="B232" t="s">
+      <c r="C232" t="s">
         <v>711</v>
-      </c>
-      <c r="C232" t="s">
-        <v>712</v>
       </c>
       <c r="D232">
         <v>64</v>
@@ -10795,7 +10795,7 @@
         <v>160</v>
       </c>
       <c r="H232" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I232" t="s">
         <v>201</v>
@@ -10824,13 +10824,13 @@
     </row>
     <row r="233" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B233" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C233" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D233">
         <v>74</v>
@@ -10847,13 +10847,13 @@
     </row>
     <row r="234" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B234" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C234" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E234" s="1" t="s">
         <v>20</v>
@@ -10867,13 +10867,13 @@
     </row>
     <row r="235" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
+        <v>714</v>
+      </c>
+      <c r="B235" t="s">
         <v>715</v>
       </c>
-      <c r="B235" t="s">
+      <c r="C235" t="s">
         <v>716</v>
-      </c>
-      <c r="C235" t="s">
-        <v>717</v>
       </c>
       <c r="D235">
         <v>66</v>
@@ -10888,7 +10888,7 @@
         <v>170</v>
       </c>
       <c r="H235" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I235" t="s">
         <v>201</v>
@@ -10917,13 +10917,13 @@
     </row>
     <row r="236" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B236" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C236" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D236">
         <v>110</v>
@@ -10967,16 +10967,16 @@
     </row>
     <row r="237" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B237" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C237" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F237" t="s">
         <v>96</v>
@@ -10984,13 +10984,13 @@
     </row>
     <row r="238" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
+        <v>719</v>
+      </c>
+      <c r="B238" t="s">
         <v>720</v>
       </c>
-      <c r="B238" t="s">
+      <c r="C238" t="s">
         <v>721</v>
-      </c>
-      <c r="C238" t="s">
-        <v>722</v>
       </c>
       <c r="D238">
         <v>66</v>
@@ -11025,13 +11025,13 @@
     </row>
     <row r="239" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B239" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C239" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D239">
         <v>76</v>
@@ -11066,16 +11066,16 @@
     </row>
     <row r="240" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B240" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C240" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F240" t="s">
         <v>96</v>
@@ -11084,7 +11084,7 @@
         <v>60</v>
       </c>
       <c r="H240" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="I240" t="s">
         <v>96</v>
@@ -11095,13 +11095,13 @@
     </row>
     <row r="241" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
+        <v>728</v>
+      </c>
+      <c r="B241" t="s">
         <v>729</v>
       </c>
-      <c r="B241" t="s">
-        <v>730</v>
-      </c>
       <c r="C241" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D241">
         <v>80</v>
@@ -11163,13 +11163,13 @@
     </row>
     <row r="242" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="B242" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C242" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D242">
         <v>90</v>
@@ -11186,13 +11186,13 @@
     </row>
     <row r="243" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B243" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C243" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E243" s="1" t="s">
         <v>84</v>
@@ -11215,13 +11215,13 @@
     </row>
     <row r="244" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
+        <v>730</v>
+      </c>
+      <c r="B244" t="s">
         <v>731</v>
       </c>
-      <c r="B244" t="s">
+      <c r="C244" t="s">
         <v>732</v>
-      </c>
-      <c r="C244" t="s">
-        <v>733</v>
       </c>
       <c r="D244">
         <v>90</v>
@@ -11247,13 +11247,13 @@
     </row>
     <row r="245" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B245" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C245" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D245">
         <v>110</v>
@@ -11270,13 +11270,13 @@
     </row>
     <row r="246" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B246" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C246" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E246" s="1" t="s">
         <v>84</v>
@@ -11504,7 +11504,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B3" t="s">
         <v>135</v>
@@ -11520,7 +11520,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B5" t="s">
         <v>135</v>
@@ -11528,7 +11528,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B6" t="s">
         <v>135</v>
@@ -11560,7 +11560,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B10" t="s">
         <v>135</v>
@@ -11616,7 +11616,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B17" t="s">
         <v>136</v>
@@ -11624,7 +11624,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B18" t="s">
         <v>136</v>
@@ -11632,7 +11632,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B19" t="s">
         <v>136</v>
@@ -11640,7 +11640,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B20" t="s">
         <v>136</v>
@@ -11648,7 +11648,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B21" t="s">
         <v>136</v>
@@ -11656,7 +11656,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B22" t="s">
         <v>136</v>
@@ -11664,7 +11664,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B23" t="s">
         <v>136</v>
@@ -11672,7 +11672,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B24" t="s">
         <v>136</v>
@@ -11784,7 +11784,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B38" t="s">
         <v>134</v>
@@ -12000,7 +12000,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B65" t="s">
         <v>134</v>
@@ -12128,7 +12128,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B81" t="s">
         <v>2</v>
@@ -12168,7 +12168,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B86" t="s">
         <v>137</v>
@@ -12392,7 +12392,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B114" t="s">
         <v>137</v>
@@ -12552,7 +12552,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B134" t="s">
         <v>137</v>
@@ -12576,7 +12576,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B137" t="s">
         <v>175</v>
@@ -12584,7 +12584,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B138" t="s">
         <v>175</v>
@@ -12592,7 +12592,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B139" t="s">
         <v>175</v>

</xml_diff>

<commit_message>
Add functionality for 'one or more' target, :enemy_oom.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13014" windowHeight="10610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13014" windowHeight="10610" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2384" uniqueCount="777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2385" uniqueCount="778">
   <si>
     <t>attributes</t>
   </si>
@@ -2361,6 +2361,9 @@
   </si>
   <si>
     <t>Sprout's Friend MingMing</t>
+  </si>
+  <si>
+    <t>enemy_oom</t>
   </si>
 </sst>
 </file>
@@ -2687,8 +2690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -12629,10 +12632,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -12702,6 +12705,11 @@
         <v>145</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>777</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Importer now displays number of modified records. Fixed Velika and Coco. Displays game client's version.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -17,7 +17,7 @@
     <sheet name="LUT" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">attributes!$A$1:$B$136</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">attributes!$A$1:$B$137</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$AE$246</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2483" uniqueCount="809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2487" uniqueCount="810">
   <si>
     <t>attributes</t>
   </si>
@@ -1292,9 +1292,6 @@
     <t>Hamster Ninjutsu</t>
   </si>
   <si>
-    <t>Electrostatis</t>
-  </si>
-  <si>
     <t>catty_5_0</t>
   </si>
   <si>
@@ -2457,6 +2454,12 @@
   </si>
   <si>
     <t>Lightning Shower (Jas)</t>
+  </si>
+  <si>
+    <t>immunity_to_burn_turns</t>
+  </si>
+  <si>
+    <t>Electrostatic</t>
   </si>
 </sst>
 </file>
@@ -2783,8 +2786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE258"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3248,7 +3251,7 @@
         <v>147</v>
       </c>
       <c r="C10" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>37</v>
@@ -3269,7 +3272,7 @@
         <v>205</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="O10" t="s">
         <v>96</v>
@@ -3704,7 +3707,7 @@
         <v>166</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F22" t="s">
         <v>99</v>
@@ -3966,13 +3969,13 @@
         <v>217</v>
       </c>
       <c r="C30" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="D30">
         <v>140</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F30" t="s">
         <v>98</v>
@@ -4001,7 +4004,7 @@
         <v>5</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I31" t="s">
         <v>96</v>
@@ -4242,7 +4245,7 @@
         <v>142</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F39" t="s">
         <v>99</v>
@@ -4288,6 +4291,15 @@
       <c r="G40">
         <v>6</v>
       </c>
+      <c r="H40" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="I40" t="s">
+        <v>99</v>
+      </c>
+      <c r="J40">
+        <v>6</v>
+      </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -4839,7 +4851,7 @@
         <v>292</v>
       </c>
       <c r="C57" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D57">
         <v>82</v>
@@ -5171,7 +5183,7 @@
         <v>317</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F67" t="s">
         <v>99</v>
@@ -5180,7 +5192,7 @@
         <v>50</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I67" t="s">
         <v>99</v>
@@ -5247,7 +5259,7 @@
         <v>321</v>
       </c>
       <c r="C69" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D69">
         <v>70</v>
@@ -5496,7 +5508,7 @@
         <v>337</v>
       </c>
       <c r="C75" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D75">
         <v>70</v>
@@ -5718,7 +5730,7 @@
         <v>347</v>
       </c>
       <c r="C81" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D81">
         <v>74</v>
@@ -5838,7 +5850,7 @@
         <v>353</v>
       </c>
       <c r="C84" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D84">
         <v>120</v>
@@ -5870,7 +5882,7 @@
         <v>353</v>
       </c>
       <c r="C85" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>140</v>
@@ -5949,7 +5961,7 @@
         <v>361</v>
       </c>
       <c r="C87" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>61</v>
@@ -6029,7 +6041,7 @@
         <v>364</v>
       </c>
       <c r="B88" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C88" t="s">
         <v>367</v>
@@ -6070,7 +6082,7 @@
         <v>365</v>
       </c>
       <c r="B89" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C89" t="s">
         <v>368</v>
@@ -6102,7 +6114,7 @@
         <v>366</v>
       </c>
       <c r="B90" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C90" t="s">
         <v>369</v>
@@ -6219,7 +6231,7 @@
         <v>373</v>
       </c>
       <c r="C93" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>12</v>
@@ -6269,7 +6281,7 @@
         <v>381</v>
       </c>
       <c r="C94" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D94">
         <v>105</v>
@@ -6548,7 +6560,7 @@
         <v>399</v>
       </c>
       <c r="C103" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D103">
         <v>150</v>
@@ -6748,7 +6760,7 @@
         <v>415</v>
       </c>
       <c r="C110" t="s">
-        <v>420</v>
+        <v>809</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>56</v>
@@ -6771,13 +6783,13 @@
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B111" t="s">
+        <v>423</v>
+      </c>
+      <c r="C111" t="s">
         <v>424</v>
-      </c>
-      <c r="C111" t="s">
-        <v>425</v>
       </c>
       <c r="D111">
         <v>48</v>
@@ -6812,13 +6824,13 @@
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B112" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C112" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D112">
         <v>102</v>
@@ -6847,13 +6859,13 @@
     </row>
     <row r="113" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>422</v>
+      </c>
+      <c r="B113" t="s">
         <v>423</v>
       </c>
-      <c r="B113" t="s">
-        <v>424</v>
-      </c>
       <c r="C113" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>411</v>
@@ -6885,13 +6897,13 @@
     </row>
     <row r="114" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B114" t="s">
+        <v>430</v>
+      </c>
+      <c r="C114" t="s">
         <v>431</v>
-      </c>
-      <c r="C114" t="s">
-        <v>432</v>
       </c>
       <c r="D114">
         <v>80</v>
@@ -6926,13 +6938,13 @@
     </row>
     <row r="115" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B115" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C115" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D115">
         <v>120</v>
@@ -6949,16 +6961,16 @@
     </row>
     <row r="116" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>429</v>
+      </c>
+      <c r="B116" t="s">
         <v>430</v>
       </c>
-      <c r="B116" t="s">
-        <v>431</v>
-      </c>
       <c r="C116" t="s">
+        <v>433</v>
+      </c>
+      <c r="E116" s="1" t="s">
         <v>434</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>435</v>
       </c>
       <c r="F116" t="s">
         <v>96</v>
@@ -6996,13 +7008,13 @@
     </row>
     <row r="117" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>435</v>
+      </c>
+      <c r="B117" t="s">
         <v>436</v>
       </c>
-      <c r="B117" t="s">
-        <v>437</v>
-      </c>
       <c r="C117" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D117">
         <v>100</v>
@@ -7017,7 +7029,7 @@
         <v>60</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I117" t="s">
         <v>99</v>
@@ -7028,13 +7040,13 @@
     </row>
     <row r="118" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B118" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C118" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D118">
         <v>102</v>
@@ -7060,13 +7072,13 @@
     </row>
     <row r="119" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B119" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C119" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>53</v>
@@ -7125,13 +7137,13 @@
     </row>
     <row r="120" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
+        <v>442</v>
+      </c>
+      <c r="B120" t="s">
         <v>443</v>
       </c>
-      <c r="B120" t="s">
-        <v>444</v>
-      </c>
       <c r="C120" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D120">
         <v>72</v>
@@ -7175,13 +7187,13 @@
     </row>
     <row r="121" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B121" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C121" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D121">
         <v>82</v>
@@ -7225,16 +7237,16 @@
     </row>
     <row r="122" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B122" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C122" t="s">
+        <v>448</v>
+      </c>
+      <c r="E122" s="1" t="s">
         <v>449</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>450</v>
       </c>
       <c r="F122" t="s">
         <v>99</v>
@@ -7245,13 +7257,13 @@
     </row>
     <row r="123" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B123" t="s">
+        <v>453</v>
+      </c>
+      <c r="C123" t="s">
         <v>454</v>
-      </c>
-      <c r="C123" t="s">
-        <v>455</v>
       </c>
       <c r="D123">
         <v>90</v>
@@ -7277,13 +7289,13 @@
     </row>
     <row r="124" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B124" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C124" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D124">
         <v>85</v>
@@ -7327,13 +7339,13 @@
     </row>
     <row r="125" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
+        <v>452</v>
+      </c>
+      <c r="B125" t="s">
         <v>453</v>
       </c>
-      <c r="B125" t="s">
-        <v>454</v>
-      </c>
       <c r="C125" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>12</v>
@@ -7354,7 +7366,7 @@
         <v>205</v>
       </c>
       <c r="K125" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="L125" t="s">
         <v>96</v>
@@ -7374,13 +7386,13 @@
     </row>
     <row r="126" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B126" t="s">
+        <v>458</v>
+      </c>
+      <c r="C126" t="s">
         <v>459</v>
-      </c>
-      <c r="C126" t="s">
-        <v>460</v>
       </c>
       <c r="D126">
         <v>44</v>
@@ -7397,19 +7409,19 @@
     </row>
     <row r="127" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
+        <v>457</v>
+      </c>
+      <c r="B127" t="s">
         <v>458</v>
       </c>
-      <c r="B127" t="s">
-        <v>459</v>
-      </c>
       <c r="C127" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D127">
         <v>132</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F127" t="s">
         <v>96</v>
@@ -7420,13 +7432,13 @@
     </row>
     <row r="128" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B128" t="s">
+        <v>463</v>
+      </c>
+      <c r="C128" t="s">
         <v>464</v>
-      </c>
-      <c r="C128" t="s">
-        <v>465</v>
       </c>
       <c r="D128">
         <v>44</v>
@@ -7443,13 +7455,13 @@
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
+        <v>462</v>
+      </c>
+      <c r="B129" t="s">
         <v>463</v>
       </c>
-      <c r="B129" t="s">
-        <v>464</v>
-      </c>
       <c r="C129" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D129">
         <v>54</v>
@@ -7466,13 +7478,13 @@
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B130" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C130" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D130">
         <v>44</v>
@@ -7489,13 +7501,13 @@
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
+        <v>467</v>
+      </c>
+      <c r="B131" t="s">
         <v>468</v>
       </c>
-      <c r="B131" t="s">
+      <c r="C131" t="s">
         <v>469</v>
-      </c>
-      <c r="C131" t="s">
-        <v>470</v>
       </c>
       <c r="D131">
         <v>54</v>
@@ -7521,13 +7533,13 @@
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B132" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C132" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D132">
         <v>48</v>
@@ -7544,13 +7556,13 @@
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B133" t="s">
+        <v>473</v>
+      </c>
+      <c r="C133" t="s">
         <v>474</v>
-      </c>
-      <c r="C133" t="s">
-        <v>475</v>
       </c>
       <c r="D133">
         <v>58</v>
@@ -7567,16 +7579,16 @@
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
+        <v>472</v>
+      </c>
+      <c r="B134" t="s">
         <v>473</v>
       </c>
-      <c r="B134" t="s">
-        <v>474</v>
-      </c>
       <c r="C134" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F134" t="s">
         <v>96</v>
@@ -7587,13 +7599,13 @@
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B135" t="s">
+        <v>478</v>
+      </c>
+      <c r="C135" t="s">
         <v>479</v>
-      </c>
-      <c r="C135" t="s">
-        <v>480</v>
       </c>
       <c r="D135">
         <v>44</v>
@@ -7610,13 +7622,13 @@
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>477</v>
+      </c>
+      <c r="B136" t="s">
         <v>478</v>
       </c>
-      <c r="B136" t="s">
-        <v>479</v>
-      </c>
       <c r="C136" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D136">
         <v>54</v>
@@ -7642,13 +7654,13 @@
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B137" t="s">
+        <v>483</v>
+      </c>
+      <c r="C137" t="s">
         <v>484</v>
-      </c>
-      <c r="C137" t="s">
-        <v>485</v>
       </c>
       <c r="D137">
         <v>46</v>
@@ -7665,13 +7677,13 @@
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
+        <v>482</v>
+      </c>
+      <c r="B138" t="s">
         <v>483</v>
       </c>
-      <c r="B138" t="s">
-        <v>484</v>
-      </c>
       <c r="C138" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D138">
         <v>56</v>
@@ -7686,7 +7698,7 @@
         <v>100</v>
       </c>
       <c r="H138" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="I138" t="s">
         <v>200</v>
@@ -7697,13 +7709,13 @@
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B139" t="s">
+        <v>489</v>
+      </c>
+      <c r="C139" t="s">
         <v>490</v>
-      </c>
-      <c r="C139" t="s">
-        <v>491</v>
       </c>
       <c r="D139">
         <v>48</v>
@@ -7720,13 +7732,13 @@
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B140" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C140" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D140">
         <v>140</v>
@@ -7743,13 +7755,13 @@
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
+        <v>488</v>
+      </c>
+      <c r="B141" t="s">
         <v>489</v>
       </c>
-      <c r="B141" t="s">
-        <v>490</v>
-      </c>
       <c r="C141" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>70</v>
@@ -7772,13 +7784,13 @@
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>497</v>
+      </c>
+      <c r="B142" t="s">
         <v>498</v>
       </c>
-      <c r="B142" t="s">
-        <v>499</v>
-      </c>
       <c r="C142" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D142">
         <v>44</v>
@@ -7795,13 +7807,13 @@
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B143" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C143" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D143">
         <v>54</v>
@@ -7845,13 +7857,13 @@
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>502</v>
+      </c>
+      <c r="B144" t="s">
         <v>503</v>
       </c>
-      <c r="B144" t="s">
-        <v>504</v>
-      </c>
       <c r="C144" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D144">
         <v>54</v>
@@ -7895,13 +7907,13 @@
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B145" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C145" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D145">
         <v>64</v>
@@ -7945,13 +7957,13 @@
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B146" t="s">
+        <v>509</v>
+      </c>
+      <c r="C146" t="s">
         <v>510</v>
-      </c>
-      <c r="C146" t="s">
-        <v>511</v>
       </c>
       <c r="D146">
         <v>46</v>
@@ -7968,19 +7980,19 @@
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
+        <v>508</v>
+      </c>
+      <c r="B147" t="s">
         <v>509</v>
       </c>
-      <c r="B147" t="s">
-        <v>510</v>
-      </c>
       <c r="C147" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D147">
         <v>56</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F147" t="s">
         <v>96</v>
@@ -7991,13 +8003,13 @@
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
+        <v>512</v>
+      </c>
+      <c r="B148" t="s">
         <v>513</v>
       </c>
-      <c r="B148" t="s">
-        <v>514</v>
-      </c>
       <c r="C148" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D148">
         <v>56</v>
@@ -8032,13 +8044,13 @@
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B149" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C149" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D149">
         <v>56</v>
@@ -8082,13 +8094,13 @@
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
+        <v>517</v>
+      </c>
+      <c r="B150" t="s">
         <v>518</v>
       </c>
-      <c r="B150" t="s">
-        <v>519</v>
-      </c>
       <c r="C150" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D150">
         <v>56</v>
@@ -8114,13 +8126,13 @@
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B151" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C151" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D151">
         <v>56</v>
@@ -8155,13 +8167,13 @@
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B152" t="s">
+        <v>524</v>
+      </c>
+      <c r="C152" t="s">
         <v>525</v>
-      </c>
-      <c r="C152" t="s">
-        <v>526</v>
       </c>
       <c r="D152">
         <v>48</v>
@@ -8178,13 +8190,13 @@
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
+        <v>523</v>
+      </c>
+      <c r="B153" t="s">
         <v>524</v>
       </c>
-      <c r="B153" t="s">
-        <v>525</v>
-      </c>
       <c r="C153" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D153">
         <v>58</v>
@@ -8210,13 +8222,13 @@
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B154" t="s">
+        <v>530</v>
+      </c>
+      <c r="C154" t="s">
         <v>531</v>
-      </c>
-      <c r="C154" t="s">
-        <v>532</v>
       </c>
       <c r="D154">
         <v>62</v>
@@ -8242,13 +8254,13 @@
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B155" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C155" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D155">
         <v>72</v>
@@ -8265,13 +8277,13 @@
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
+        <v>529</v>
+      </c>
+      <c r="B156" t="s">
         <v>530</v>
       </c>
-      <c r="B156" t="s">
-        <v>531</v>
-      </c>
       <c r="C156" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>84</v>
@@ -8294,13 +8306,13 @@
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B157" t="s">
+        <v>536</v>
+      </c>
+      <c r="C157" t="s">
         <v>537</v>
-      </c>
-      <c r="C157" t="s">
-        <v>538</v>
       </c>
       <c r="D157">
         <v>54</v>
@@ -8344,13 +8356,13 @@
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>535</v>
+      </c>
+      <c r="B158" t="s">
         <v>536</v>
       </c>
-      <c r="B158" t="s">
-        <v>537</v>
-      </c>
       <c r="C158" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D158">
         <v>44</v>
@@ -8376,13 +8388,13 @@
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B159" t="s">
+        <v>541</v>
+      </c>
+      <c r="C159" t="s">
         <v>542</v>
-      </c>
-      <c r="C159" t="s">
-        <v>543</v>
       </c>
       <c r="D159">
         <v>46</v>
@@ -8399,13 +8411,13 @@
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
+        <v>540</v>
+      </c>
+      <c r="B160" t="s">
         <v>541</v>
       </c>
-      <c r="B160" t="s">
-        <v>542</v>
-      </c>
       <c r="C160" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D160">
         <v>56</v>
@@ -8449,13 +8461,13 @@
     </row>
     <row r="161" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B161" t="s">
+        <v>546</v>
+      </c>
+      <c r="C161" t="s">
         <v>547</v>
-      </c>
-      <c r="C161" t="s">
-        <v>548</v>
       </c>
       <c r="D161">
         <v>56</v>
@@ -8490,13 +8502,13 @@
     </row>
     <row r="162" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
+        <v>545</v>
+      </c>
+      <c r="B162" t="s">
         <v>546</v>
       </c>
-      <c r="B162" t="s">
-        <v>547</v>
-      </c>
       <c r="C162" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D162">
         <v>66</v>
@@ -8513,13 +8525,13 @@
     </row>
     <row r="163" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B163" t="s">
+        <v>551</v>
+      </c>
+      <c r="C163" t="s">
         <v>552</v>
-      </c>
-      <c r="C163" t="s">
-        <v>553</v>
       </c>
       <c r="D163">
         <v>48</v>
@@ -8554,13 +8566,13 @@
     </row>
     <row r="164" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
+        <v>550</v>
+      </c>
+      <c r="B164" t="s">
         <v>551</v>
       </c>
-      <c r="B164" t="s">
-        <v>552</v>
-      </c>
       <c r="C164" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D164">
         <v>58</v>
@@ -8586,13 +8598,13 @@
     </row>
     <row r="165" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B165" t="s">
+        <v>556</v>
+      </c>
+      <c r="C165" t="s">
         <v>557</v>
-      </c>
-      <c r="C165" t="s">
-        <v>558</v>
       </c>
       <c r="D165">
         <v>48</v>
@@ -8627,13 +8639,13 @@
     </row>
     <row r="166" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
+        <v>555</v>
+      </c>
+      <c r="B166" t="s">
         <v>556</v>
       </c>
-      <c r="B166" t="s">
-        <v>557</v>
-      </c>
       <c r="C166" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D166">
         <v>48</v>
@@ -8659,13 +8671,13 @@
     </row>
     <row r="167" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B167" t="s">
+        <v>562</v>
+      </c>
+      <c r="C167" t="s">
         <v>563</v>
-      </c>
-      <c r="C167" t="s">
-        <v>564</v>
       </c>
       <c r="D167">
         <v>64</v>
@@ -8709,13 +8721,13 @@
     </row>
     <row r="168" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B168" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C168" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D168">
         <v>70</v>
@@ -8759,13 +8771,13 @@
     </row>
     <row r="169" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
+        <v>561</v>
+      </c>
+      <c r="B169" t="s">
         <v>562</v>
       </c>
-      <c r="B169" t="s">
-        <v>563</v>
-      </c>
       <c r="C169" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E169" s="1" t="s">
         <v>35</v>
@@ -8777,7 +8789,7 @@
         <v>5</v>
       </c>
       <c r="H169" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I169" t="s">
         <v>96</v>
@@ -8788,13 +8800,13 @@
     </row>
     <row r="170" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
+        <v>572</v>
+      </c>
+      <c r="B170" t="s">
         <v>573</v>
       </c>
-      <c r="B170" t="s">
+      <c r="C170" t="s">
         <v>574</v>
-      </c>
-      <c r="C170" t="s">
-        <v>575</v>
       </c>
       <c r="D170">
         <v>66</v>
@@ -8809,7 +8821,7 @@
         <v>230</v>
       </c>
       <c r="H170" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I170" t="s">
         <v>200</v>
@@ -8820,13 +8832,13 @@
     </row>
     <row r="171" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B171" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C171" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D171">
         <v>80</v>
@@ -8852,13 +8864,13 @@
     </row>
     <row r="172" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B172" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C172" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>66</v>
@@ -8870,7 +8882,7 @@
         <v>50</v>
       </c>
       <c r="H172" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I172" t="s">
         <v>96</v>
@@ -8879,7 +8891,7 @@
         <v>80</v>
       </c>
       <c r="K172" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="L172" t="s">
         <v>96</v>
@@ -8888,7 +8900,7 @@
         <v>4</v>
       </c>
       <c r="N172" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="O172" t="s">
         <v>96</v>
@@ -8897,7 +8909,7 @@
         <v>60</v>
       </c>
       <c r="Q172" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="R172" t="s">
         <v>96</v>
@@ -8908,13 +8920,13 @@
     </row>
     <row r="173" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
+        <v>583</v>
+      </c>
+      <c r="B173" t="s">
         <v>584</v>
       </c>
-      <c r="B173" t="s">
+      <c r="C173" t="s">
         <v>585</v>
-      </c>
-      <c r="C173" t="s">
-        <v>586</v>
       </c>
       <c r="D173">
         <v>48</v>
@@ -8931,13 +8943,13 @@
     </row>
     <row r="174" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B174" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C174" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D174">
         <v>58</v>
@@ -8963,13 +8975,13 @@
     </row>
     <row r="175" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
+        <v>588</v>
+      </c>
+      <c r="B175" t="s">
         <v>589</v>
       </c>
-      <c r="B175" t="s">
-        <v>590</v>
-      </c>
       <c r="C175" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D175">
         <v>58</v>
@@ -9004,13 +9016,13 @@
     </row>
     <row r="176" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B176" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C176" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D176">
         <v>58</v>
@@ -9036,13 +9048,13 @@
     </row>
     <row r="177" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
+        <v>594</v>
+      </c>
+      <c r="B177" t="s">
         <v>595</v>
       </c>
-      <c r="B177" t="s">
+      <c r="C177" t="s">
         <v>596</v>
-      </c>
-      <c r="C177" t="s">
-        <v>597</v>
       </c>
       <c r="D177">
         <v>48</v>
@@ -9059,13 +9071,13 @@
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B178" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C178" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D178">
         <v>58</v>
@@ -9091,13 +9103,13 @@
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
+        <v>599</v>
+      </c>
+      <c r="B179" t="s">
         <v>600</v>
       </c>
-      <c r="B179" t="s">
+      <c r="C179" t="s">
         <v>601</v>
-      </c>
-      <c r="C179" t="s">
-        <v>602</v>
       </c>
       <c r="D179">
         <v>62</v>
@@ -9132,13 +9144,13 @@
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B180" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C180" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D180">
         <v>72</v>
@@ -9182,16 +9194,16 @@
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B181" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C181" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F181" t="s">
         <v>96</v>
@@ -9202,13 +9214,13 @@
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
+        <v>606</v>
+      </c>
+      <c r="B182" t="s">
         <v>607</v>
       </c>
-      <c r="B182" t="s">
+      <c r="C182" t="s">
         <v>608</v>
-      </c>
-      <c r="C182" t="s">
-        <v>609</v>
       </c>
       <c r="D182">
         <v>56</v>
@@ -9234,13 +9246,13 @@
     </row>
     <row r="183" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B183" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C183" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D183">
         <v>66</v>
@@ -9266,13 +9278,13 @@
     </row>
     <row r="184" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B184" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C184" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>16</v>
@@ -9286,13 +9298,13 @@
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
+        <v>612</v>
+      </c>
+      <c r="B185" t="s">
         <v>613</v>
       </c>
-      <c r="B185" t="s">
+      <c r="C185" t="s">
         <v>614</v>
-      </c>
-      <c r="C185" t="s">
-        <v>615</v>
       </c>
       <c r="D185">
         <v>56</v>
@@ -9309,13 +9321,13 @@
     </row>
     <row r="186" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B186" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C186" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D186">
         <v>58</v>
@@ -9341,13 +9353,13 @@
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B187" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C187" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E187" s="1" t="s">
         <v>16</v>
@@ -9361,13 +9373,13 @@
     </row>
     <row r="188" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
+        <v>618</v>
+      </c>
+      <c r="B188" t="s">
         <v>619</v>
       </c>
-      <c r="B188" t="s">
+      <c r="C188" t="s">
         <v>620</v>
-      </c>
-      <c r="C188" t="s">
-        <v>621</v>
       </c>
       <c r="D188">
         <v>64</v>
@@ -9402,13 +9414,13 @@
     </row>
     <row r="189" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B189" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C189" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D189">
         <v>74</v>
@@ -9443,13 +9455,13 @@
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B190" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C190" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>41</v>
@@ -9481,13 +9493,13 @@
     </row>
     <row r="191" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
+        <v>625</v>
+      </c>
+      <c r="B191" t="s">
         <v>626</v>
       </c>
-      <c r="B191" t="s">
+      <c r="C191" t="s">
         <v>627</v>
-      </c>
-      <c r="C191" t="s">
-        <v>628</v>
       </c>
       <c r="D191">
         <v>48</v>
@@ -9504,13 +9516,13 @@
     </row>
     <row r="192" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B192" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C192" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D192">
         <v>58</v>
@@ -9527,13 +9539,13 @@
     </row>
     <row r="193" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
+        <v>629</v>
+      </c>
+      <c r="B193" t="s">
         <v>630</v>
       </c>
-      <c r="B193" t="s">
+      <c r="C193" t="s">
         <v>631</v>
-      </c>
-      <c r="C193" t="s">
-        <v>632</v>
       </c>
       <c r="D193">
         <v>58</v>
@@ -9568,13 +9580,13 @@
     </row>
     <row r="194" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B194" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C194" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D194">
         <v>48</v>
@@ -9618,13 +9630,13 @@
     </row>
     <row r="195" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
+        <v>634</v>
+      </c>
+      <c r="B195" t="s">
+        <v>633</v>
+      </c>
+      <c r="C195" t="s">
         <v>635</v>
-      </c>
-      <c r="B195" t="s">
-        <v>634</v>
-      </c>
-      <c r="C195" t="s">
-        <v>636</v>
       </c>
       <c r="D195">
         <v>48</v>
@@ -9641,13 +9653,13 @@
     </row>
     <row r="196" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B196" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C196" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D196">
         <v>68</v>
@@ -9664,13 +9676,13 @@
     </row>
     <row r="197" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
+        <v>637</v>
+      </c>
+      <c r="B197" t="s">
         <v>638</v>
       </c>
-      <c r="B197" t="s">
+      <c r="C197" t="s">
         <v>639</v>
-      </c>
-      <c r="C197" t="s">
-        <v>640</v>
       </c>
       <c r="D197">
         <v>60</v>
@@ -9705,13 +9717,13 @@
     </row>
     <row r="198" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B198" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C198" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D198">
         <v>70</v>
@@ -9746,13 +9758,13 @@
     </row>
     <row r="199" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
+        <v>641</v>
+      </c>
+      <c r="B199" t="s">
         <v>642</v>
       </c>
-      <c r="B199" t="s">
+      <c r="C199" t="s">
         <v>643</v>
-      </c>
-      <c r="C199" t="s">
-        <v>644</v>
       </c>
       <c r="D199">
         <v>62</v>
@@ -9778,13 +9790,13 @@
     </row>
     <row r="200" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B200" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C200" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D200">
         <v>72</v>
@@ -9810,16 +9822,16 @@
     </row>
     <row r="201" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B201" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C201" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F201" t="s">
         <v>96</v>
@@ -9830,13 +9842,13 @@
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
+        <v>646</v>
+      </c>
+      <c r="B202" t="s">
         <v>647</v>
       </c>
-      <c r="B202" t="s">
+      <c r="C202" t="s">
         <v>648</v>
-      </c>
-      <c r="C202" t="s">
-        <v>649</v>
       </c>
       <c r="D202">
         <v>64</v>
@@ -9871,13 +9883,13 @@
     </row>
     <row r="203" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B203" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C203" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D203">
         <v>94</v>
@@ -9912,13 +9924,13 @@
     </row>
     <row r="204" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B204" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C204" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>17</v>
@@ -9932,13 +9944,13 @@
     </row>
     <row r="205" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
+        <v>651</v>
+      </c>
+      <c r="B205" t="s">
         <v>652</v>
       </c>
-      <c r="B205" t="s">
+      <c r="C205" t="s">
         <v>653</v>
-      </c>
-      <c r="C205" t="s">
-        <v>654</v>
       </c>
       <c r="D205">
         <v>90</v>
@@ -9973,13 +9985,13 @@
     </row>
     <row r="206" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B206" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C206" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D206">
         <v>76</v>
@@ -10023,13 +10035,13 @@
     </row>
     <row r="207" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B207" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C207" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>18</v>
@@ -10043,13 +10055,13 @@
     </row>
     <row r="208" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
+        <v>656</v>
+      </c>
+      <c r="B208" t="s">
         <v>657</v>
       </c>
-      <c r="B208" t="s">
+      <c r="C208" t="s">
         <v>658</v>
-      </c>
-      <c r="C208" t="s">
-        <v>659</v>
       </c>
       <c r="D208">
         <v>58</v>
@@ -10084,13 +10096,13 @@
     </row>
     <row r="209" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B209" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C209" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D209">
         <v>120</v>
@@ -10107,13 +10119,13 @@
     </row>
     <row r="210" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
+        <v>660</v>
+      </c>
+      <c r="B210" t="s">
         <v>661</v>
       </c>
-      <c r="B210" t="s">
+      <c r="C210" t="s">
         <v>662</v>
-      </c>
-      <c r="C210" t="s">
-        <v>663</v>
       </c>
       <c r="D210">
         <v>58</v>
@@ -10148,13 +10160,13 @@
     </row>
     <row r="211" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B211" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C211" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D211">
         <v>88</v>
@@ -10180,13 +10192,13 @@
     </row>
     <row r="212" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
+        <v>664</v>
+      </c>
+      <c r="B212" t="s">
         <v>665</v>
       </c>
-      <c r="B212" t="s">
+      <c r="C212" t="s">
         <v>666</v>
-      </c>
-      <c r="C212" t="s">
-        <v>667</v>
       </c>
       <c r="D212">
         <v>54</v>
@@ -10203,13 +10215,13 @@
     </row>
     <row r="213" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B213" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C213" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="D213">
         <v>74</v>
@@ -10244,16 +10256,16 @@
     </row>
     <row r="214" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B214" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C214" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F214" t="s">
         <v>96</v>
@@ -10262,7 +10274,7 @@
         <v>60</v>
       </c>
       <c r="H214" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="I214" t="s">
         <v>96</v>
@@ -10273,13 +10285,13 @@
     </row>
     <row r="215" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
+        <v>669</v>
+      </c>
+      <c r="B215" t="s">
         <v>670</v>
       </c>
-      <c r="B215" t="s">
+      <c r="C215" t="s">
         <v>671</v>
-      </c>
-      <c r="C215" t="s">
-        <v>672</v>
       </c>
       <c r="D215">
         <v>54</v>
@@ -10323,13 +10335,13 @@
     </row>
     <row r="216" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B216" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C216" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D216">
         <v>74</v>
@@ -10350,7 +10362,7 @@
         <v>145</v>
       </c>
       <c r="J216" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="K216" s="1" t="s">
         <v>49</v>
@@ -10373,13 +10385,13 @@
     </row>
     <row r="217" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B217" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C217" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E217" s="1" t="s">
         <v>29</v>
@@ -10402,13 +10414,13 @@
     </row>
     <row r="218" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
+        <v>675</v>
+      </c>
+      <c r="B218" t="s">
         <v>676</v>
       </c>
-      <c r="B218" t="s">
+      <c r="C218" t="s">
         <v>677</v>
-      </c>
-      <c r="C218" t="s">
-        <v>678</v>
       </c>
       <c r="D218">
         <v>62</v>
@@ -10443,13 +10455,13 @@
     </row>
     <row r="219" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B219" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C219" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D219">
         <v>62</v>
@@ -10475,13 +10487,13 @@
     </row>
     <row r="220" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B220" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C220" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E220" s="1" t="s">
         <v>34</v>
@@ -10504,13 +10516,13 @@
     </row>
     <row r="221" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
+        <v>680</v>
+      </c>
+      <c r="B221" t="s">
         <v>681</v>
       </c>
-      <c r="B221" t="s">
+      <c r="C221" t="s">
         <v>682</v>
-      </c>
-      <c r="C221" t="s">
-        <v>683</v>
       </c>
       <c r="D221">
         <v>52</v>
@@ -10527,13 +10539,13 @@
     </row>
     <row r="222" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B222" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C222" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D222">
         <v>62</v>
@@ -10568,13 +10580,13 @@
     </row>
     <row r="223" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B223" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C223" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E223" s="1" t="s">
         <v>19</v>
@@ -10588,13 +10600,13 @@
     </row>
     <row r="224" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
+        <v>685</v>
+      </c>
+      <c r="B224" t="s">
         <v>686</v>
       </c>
-      <c r="B224" t="s">
+      <c r="C224" t="s">
         <v>687</v>
-      </c>
-      <c r="C224" t="s">
-        <v>688</v>
       </c>
       <c r="D224">
         <v>74</v>
@@ -10629,13 +10641,13 @@
     </row>
     <row r="225" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B225" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C225" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D225">
         <v>90</v>
@@ -10670,13 +10682,13 @@
     </row>
     <row r="226" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B226" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C226" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E226" s="1" t="s">
         <v>19</v>
@@ -10708,13 +10720,13 @@
     </row>
     <row r="227" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
+        <v>690</v>
+      </c>
+      <c r="B227" t="s">
         <v>691</v>
       </c>
-      <c r="B227" t="s">
+      <c r="C227" t="s">
         <v>692</v>
-      </c>
-      <c r="C227" t="s">
-        <v>693</v>
       </c>
       <c r="D227">
         <v>60</v>
@@ -10749,13 +10761,13 @@
     </row>
     <row r="228" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B228" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C228" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D228">
         <v>90</v>
@@ -10781,13 +10793,13 @@
     </row>
     <row r="229" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
+        <v>694</v>
+      </c>
+      <c r="B229" t="s">
         <v>695</v>
       </c>
-      <c r="B229" t="s">
+      <c r="C229" t="s">
         <v>696</v>
-      </c>
-      <c r="C229" t="s">
-        <v>697</v>
       </c>
       <c r="D229">
         <v>62</v>
@@ -10822,13 +10834,13 @@
     </row>
     <row r="230" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B230" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C230" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="D230">
         <v>140</v>
@@ -10845,13 +10857,13 @@
     </row>
     <row r="231" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B231" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C231" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E231" s="1" t="s">
         <v>87</v>
@@ -10874,13 +10886,13 @@
     </row>
     <row r="232" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
+        <v>698</v>
+      </c>
+      <c r="B232" t="s">
         <v>699</v>
       </c>
-      <c r="B232" t="s">
+      <c r="C232" t="s">
         <v>700</v>
-      </c>
-      <c r="C232" t="s">
-        <v>701</v>
       </c>
       <c r="D232">
         <v>64</v>
@@ -10924,13 +10936,13 @@
     </row>
     <row r="233" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B233" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C233" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D233">
         <v>74</v>
@@ -10947,13 +10959,13 @@
     </row>
     <row r="234" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B234" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C234" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E234" s="1" t="s">
         <v>20</v>
@@ -10967,13 +10979,13 @@
     </row>
     <row r="235" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
+        <v>703</v>
+      </c>
+      <c r="B235" t="s">
         <v>704</v>
       </c>
-      <c r="B235" t="s">
+      <c r="C235" t="s">
         <v>705</v>
-      </c>
-      <c r="C235" t="s">
-        <v>706</v>
       </c>
       <c r="D235">
         <v>66</v>
@@ -11017,13 +11029,13 @@
     </row>
     <row r="236" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B236" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C236" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D236">
         <v>110</v>
@@ -11067,16 +11079,16 @@
     </row>
     <row r="237" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B237" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C237" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F237" t="s">
         <v>96</v>
@@ -11084,13 +11096,13 @@
     </row>
     <row r="238" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
+        <v>708</v>
+      </c>
+      <c r="B238" t="s">
         <v>709</v>
       </c>
-      <c r="B238" t="s">
+      <c r="C238" t="s">
         <v>710</v>
-      </c>
-      <c r="C238" t="s">
-        <v>711</v>
       </c>
       <c r="D238">
         <v>66</v>
@@ -11125,13 +11137,13 @@
     </row>
     <row r="239" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B239" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C239" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D239">
         <v>76</v>
@@ -11166,16 +11178,16 @@
     </row>
     <row r="240" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B240" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C240" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="F240" t="s">
         <v>96</v>
@@ -11184,7 +11196,7 @@
         <v>60</v>
       </c>
       <c r="H240" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="I240" t="s">
         <v>96</v>
@@ -11195,13 +11207,13 @@
     </row>
     <row r="241" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
+        <v>717</v>
+      </c>
+      <c r="B241" t="s">
         <v>718</v>
       </c>
-      <c r="B241" t="s">
-        <v>719</v>
-      </c>
       <c r="C241" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D241">
         <v>80</v>
@@ -11263,13 +11275,13 @@
     </row>
     <row r="242" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B242" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C242" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D242">
         <v>90</v>
@@ -11286,13 +11298,13 @@
     </row>
     <row r="243" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B243" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C243" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E243" s="1" t="s">
         <v>84</v>
@@ -11315,13 +11327,13 @@
     </row>
     <row r="244" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
+        <v>719</v>
+      </c>
+      <c r="B244" t="s">
         <v>720</v>
       </c>
-      <c r="B244" t="s">
+      <c r="C244" t="s">
         <v>721</v>
-      </c>
-      <c r="C244" t="s">
-        <v>722</v>
       </c>
       <c r="D244">
         <v>90</v>
@@ -11347,13 +11359,13 @@
     </row>
     <row r="245" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B245" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D245">
         <v>110</v>
@@ -11370,13 +11382,13 @@
     </row>
     <row r="246" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B246" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C246" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E246" s="1" t="s">
         <v>84</v>
@@ -11399,13 +11411,13 @@
     </row>
     <row r="247" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
+        <v>766</v>
+      </c>
+      <c r="B247" t="s">
         <v>767</v>
       </c>
-      <c r="B247" t="s">
-        <v>768</v>
-      </c>
       <c r="C247" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D247">
         <v>72</v>
@@ -11440,13 +11452,13 @@
     </row>
     <row r="248" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B248" t="s">
+        <v>767</v>
+      </c>
+      <c r="C248" t="s">
         <v>768</v>
-      </c>
-      <c r="C248" t="s">
-        <v>769</v>
       </c>
       <c r="D248">
         <v>72</v>
@@ -11461,7 +11473,7 @@
         <v>70</v>
       </c>
       <c r="H248" s="1" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="I248" t="s">
         <v>145</v>
@@ -11470,7 +11482,7 @@
         <v>20</v>
       </c>
       <c r="K248" s="1" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="L248" t="s">
         <v>145</v>
@@ -11479,7 +11491,7 @@
         <v>120</v>
       </c>
       <c r="N248" s="1" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="O248" t="s">
         <v>145</v>
@@ -11490,13 +11502,13 @@
     </row>
     <row r="249" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B249" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C249" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E249" s="1" t="s">
         <v>9</v>
@@ -11510,13 +11522,13 @@
     </row>
     <row r="250" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
+        <v>773</v>
+      </c>
+      <c r="B250" t="s">
         <v>774</v>
       </c>
-      <c r="B250" t="s">
+      <c r="C250" t="s">
         <v>775</v>
-      </c>
-      <c r="C250" t="s">
-        <v>776</v>
       </c>
       <c r="D250">
         <v>70</v>
@@ -11551,13 +11563,13 @@
     </row>
     <row r="251" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B251" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C251" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D251">
         <v>64</v>
@@ -11583,16 +11595,16 @@
     </row>
     <row r="252" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B252" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C252" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F252" t="s">
         <v>96</v>
@@ -11603,13 +11615,13 @@
     </row>
     <row r="253" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
+        <v>778</v>
+      </c>
+      <c r="B253" t="s">
         <v>779</v>
       </c>
-      <c r="B253" t="s">
+      <c r="C253" t="s">
         <v>780</v>
-      </c>
-      <c r="C253" t="s">
-        <v>781</v>
       </c>
       <c r="D253">
         <v>70</v>
@@ -11624,7 +11636,7 @@
         <v>180</v>
       </c>
       <c r="H253" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="I253" t="s">
         <v>200</v>
@@ -11644,13 +11656,13 @@
     </row>
     <row r="254" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="B254" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C254" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D254">
         <v>70</v>
@@ -11667,13 +11679,13 @@
     </row>
     <row r="255" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B255" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C255" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E255" s="1" t="s">
         <v>21</v>
@@ -11687,13 +11699,13 @@
     </row>
     <row r="256" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
+        <v>784</v>
+      </c>
+      <c r="B256" t="s">
         <v>785</v>
       </c>
-      <c r="B256" t="s">
+      <c r="C256" t="s">
         <v>786</v>
-      </c>
-      <c r="C256" t="s">
-        <v>787</v>
       </c>
       <c r="D256">
         <v>150</v>
@@ -11710,13 +11722,13 @@
     </row>
     <row r="257" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B257" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C257" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="D257">
         <v>72</v>
@@ -11760,13 +11772,13 @@
     </row>
     <row r="258" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B258" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C258" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E258" s="1" t="s">
         <v>16</v>
@@ -11783,7 +11795,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="35">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="39">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>LUT!$C:$C</xm:f>
@@ -11866,7 +11878,13 @@
           <x14:formula1>
             <xm:f>attributes!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>N249:N256 N258:N1048576</xm:sqref>
+          <xm:sqref>N249:N256</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>N258:N1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -11884,7 +11902,13 @@
           <x14:formula1>
             <xm:f>attributes!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>K249:K256 K258:K1048576</xm:sqref>
+          <xm:sqref>K249:K256</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>K258:K1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -11914,7 +11938,19 @@
           <x14:formula1>
             <xm:f>attributes!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>H252:H1048576 K257 N257</xm:sqref>
+          <xm:sqref>H252:H1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>K257</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>N257</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -12002,11 +12038,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B145"/>
+  <dimension ref="A1:B146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -12033,7 +12069,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B3" t="s">
         <v>135</v>
@@ -12049,7 +12085,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B5" t="s">
         <v>135</v>
@@ -12089,7 +12125,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B10" t="s">
         <v>135</v>
@@ -12105,7 +12141,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B12" t="s">
         <v>135</v>
@@ -12153,7 +12189,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B18" t="s">
         <v>136</v>
@@ -12161,7 +12197,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B19" t="s">
         <v>136</v>
@@ -12169,7 +12205,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B20" t="s">
         <v>136</v>
@@ -12177,7 +12213,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B21" t="s">
         <v>136</v>
@@ -12185,7 +12221,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B22" t="s">
         <v>136</v>
@@ -12201,7 +12237,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B24" t="s">
         <v>136</v>
@@ -12209,7 +12245,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B25" t="s">
         <v>136</v>
@@ -12249,7 +12285,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>808</v>
       </c>
       <c r="B30" t="s">
         <v>133</v>
@@ -12257,7 +12293,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
         <v>133</v>
@@ -12265,7 +12301,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
         <v>133</v>
@@ -12273,7 +12309,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
         <v>133</v>
@@ -12281,7 +12317,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B34" t="s">
         <v>133</v>
@@ -12289,7 +12325,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
         <v>133</v>
@@ -12297,7 +12333,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
         <v>133</v>
@@ -12305,31 +12341,31 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B37" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B38" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>411</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>23</v>
+        <v>411</v>
       </c>
       <c r="B40" t="s">
         <v>134</v>
@@ -12337,7 +12373,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B41" t="s">
         <v>134</v>
@@ -12345,7 +12381,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42" t="s">
         <v>134</v>
@@ -12353,7 +12389,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B43" t="s">
         <v>134</v>
@@ -12361,7 +12397,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B44" t="s">
         <v>134</v>
@@ -12369,7 +12405,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B45" t="s">
         <v>134</v>
@@ -12377,7 +12413,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>285</v>
+        <v>26</v>
       </c>
       <c r="B46" t="s">
         <v>134</v>
@@ -12385,7 +12421,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B47" t="s">
         <v>134</v>
@@ -12393,7 +12429,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>27</v>
+        <v>284</v>
       </c>
       <c r="B48" t="s">
         <v>134</v>
@@ -12401,7 +12437,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B49" t="s">
         <v>134</v>
@@ -12409,7 +12445,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>287</v>
+        <v>28</v>
       </c>
       <c r="B50" t="s">
         <v>134</v>
@@ -12417,7 +12453,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B51" t="s">
         <v>134</v>
@@ -12425,7 +12461,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>29</v>
+        <v>286</v>
       </c>
       <c r="B52" t="s">
         <v>134</v>
@@ -12433,7 +12469,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B53" t="s">
         <v>134</v>
@@ -12441,7 +12477,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B54" t="s">
         <v>134</v>
@@ -12449,7 +12485,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B55" t="s">
         <v>134</v>
@@ -12457,7 +12493,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B56" t="s">
         <v>134</v>
@@ -12465,7 +12501,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="B57" t="s">
         <v>134</v>
@@ -12473,7 +12509,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>134</v>
@@ -12481,7 +12517,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B59" t="s">
         <v>134</v>
@@ -12489,7 +12525,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60" t="s">
         <v>134</v>
@@ -12497,7 +12533,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B61" t="s">
         <v>134</v>
@@ -12505,7 +12541,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B62" t="s">
         <v>134</v>
@@ -12513,7 +12549,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B63" t="s">
         <v>134</v>
@@ -12521,7 +12557,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B64" t="s">
         <v>134</v>
@@ -12529,7 +12565,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B65" t="s">
         <v>134</v>
@@ -12537,7 +12573,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>412</v>
+        <v>77</v>
       </c>
       <c r="B66" t="s">
         <v>134</v>
@@ -12545,7 +12581,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>78</v>
+        <v>412</v>
       </c>
       <c r="B67" t="s">
         <v>134</v>
@@ -12553,7 +12589,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B68" t="s">
         <v>134</v>
@@ -12561,7 +12597,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B69" t="s">
         <v>134</v>
@@ -12569,7 +12605,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B70" t="s">
         <v>134</v>
@@ -12577,7 +12613,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>302</v>
+        <v>81</v>
       </c>
       <c r="B71" t="s">
         <v>134</v>
@@ -12585,7 +12621,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B72" t="s">
         <v>134</v>
@@ -12593,7 +12629,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>82</v>
+        <v>301</v>
       </c>
       <c r="B73" t="s">
         <v>134</v>
@@ -12601,7 +12637,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B74" t="s">
         <v>134</v>
@@ -12609,15 +12645,15 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B75" t="s">
-        <v>174</v>
+        <v>134</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>173</v>
+        <v>3</v>
       </c>
       <c r="B76" t="s">
         <v>174</v>
@@ -12625,7 +12661,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>206</v>
+        <v>173</v>
       </c>
       <c r="B77" t="s">
         <v>174</v>
@@ -12633,7 +12669,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B78" t="s">
         <v>174</v>
@@ -12641,15 +12677,15 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>356</v>
+        <v>207</v>
       </c>
       <c r="B79" t="s">
-        <v>2</v>
+        <v>174</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B80" t="s">
         <v>2</v>
@@ -12657,7 +12693,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>138</v>
+        <v>355</v>
       </c>
       <c r="B81" t="s">
         <v>2</v>
@@ -12665,7 +12701,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>567</v>
+        <v>138</v>
       </c>
       <c r="B82" t="s">
         <v>2</v>
@@ -12673,7 +12709,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>5</v>
+        <v>566</v>
       </c>
       <c r="B83" t="s">
         <v>2</v>
@@ -12681,7 +12717,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B84" t="s">
         <v>2</v>
@@ -12689,23 +12725,23 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>150</v>
+        <v>4</v>
       </c>
       <c r="B85" t="s">
-        <v>174</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>770</v>
+        <v>150</v>
       </c>
       <c r="B86" t="s">
-        <v>137</v>
+        <v>174</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="B87" t="s">
         <v>137</v>
@@ -12713,7 +12749,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="B88" t="s">
         <v>137</v>
@@ -12721,7 +12757,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>41</v>
+        <v>771</v>
       </c>
       <c r="B89" t="s">
         <v>137</v>
@@ -12729,7 +12765,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>370</v>
+        <v>41</v>
       </c>
       <c r="B90" t="s">
         <v>137</v>
@@ -12737,7 +12773,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>246</v>
+        <v>370</v>
       </c>
       <c r="B91" t="s">
         <v>137</v>
@@ -12745,7 +12781,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>38</v>
+        <v>246</v>
       </c>
       <c r="B92" t="s">
         <v>137</v>
@@ -12753,7 +12789,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>247</v>
+        <v>38</v>
       </c>
       <c r="B93" t="s">
         <v>137</v>
@@ -12761,7 +12797,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>39</v>
+        <v>247</v>
       </c>
       <c r="B94" t="s">
         <v>137</v>
@@ -12769,7 +12805,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>331</v>
+        <v>39</v>
       </c>
       <c r="B95" t="s">
         <v>137</v>
@@ -12777,7 +12813,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B96" t="s">
         <v>137</v>
@@ -12785,7 +12821,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>37</v>
+        <v>333</v>
       </c>
       <c r="B97" t="s">
         <v>137</v>
@@ -12793,7 +12829,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>332</v>
+        <v>37</v>
       </c>
       <c r="B98" t="s">
         <v>137</v>
@@ -12801,7 +12837,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>42</v>
+        <v>332</v>
       </c>
       <c r="B99" t="s">
         <v>137</v>
@@ -12809,7 +12845,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B100" t="s">
         <v>137</v>
@@ -12817,7 +12853,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B101" t="s">
         <v>137</v>
@@ -12825,7 +12861,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B102" t="s">
         <v>137</v>
@@ -12833,7 +12869,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B103" t="s">
         <v>137</v>
@@ -12841,7 +12877,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="B104" t="s">
         <v>137</v>
@@ -12849,7 +12885,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B105" t="s">
         <v>137</v>
@@ -12857,7 +12893,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B106" t="s">
         <v>137</v>
@@ -12865,7 +12901,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B107" t="s">
         <v>137</v>
@@ -12873,7 +12909,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>225</v>
+        <v>61</v>
       </c>
       <c r="B108" t="s">
         <v>137</v>
@@ -12881,7 +12917,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>48</v>
+        <v>225</v>
       </c>
       <c r="B109" t="s">
         <v>137</v>
@@ -12889,7 +12925,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B110" t="s">
         <v>137</v>
@@ -12897,7 +12933,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B111" t="s">
         <v>137</v>
@@ -12905,7 +12941,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B112" t="s">
         <v>137</v>
@@ -12913,7 +12949,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B113" t="s">
         <v>137</v>
@@ -12921,7 +12957,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B114" t="s">
         <v>137</v>
@@ -12929,7 +12965,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B115" t="s">
         <v>137</v>
@@ -12937,23 +12973,23 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>140</v>
+        <v>52</v>
       </c>
       <c r="B116" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>84</v>
+        <v>140</v>
       </c>
       <c r="B117" t="s">
-        <v>137</v>
+        <v>174</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>450</v>
+        <v>84</v>
       </c>
       <c r="B118" t="s">
         <v>137</v>
@@ -12961,7 +12997,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>85</v>
+        <v>449</v>
       </c>
       <c r="B119" t="s">
         <v>137</v>
@@ -12969,7 +13005,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B120" t="s">
         <v>137</v>
@@ -12977,7 +13013,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>142</v>
+        <v>86</v>
       </c>
       <c r="B121" t="s">
         <v>137</v>
@@ -12985,7 +13021,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>357</v>
+        <v>142</v>
       </c>
       <c r="B122" t="s">
         <v>137</v>
@@ -12993,7 +13029,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>141</v>
+        <v>357</v>
       </c>
       <c r="B123" t="s">
         <v>137</v>
@@ -13001,7 +13037,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>87</v>
+        <v>141</v>
       </c>
       <c r="B124" t="s">
         <v>137</v>
@@ -13009,7 +13045,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B125" t="s">
         <v>137</v>
@@ -13017,7 +13053,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B126" t="s">
         <v>137</v>
@@ -13025,7 +13061,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B127" t="s">
         <v>137</v>
@@ -13033,7 +13069,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="B128" t="s">
         <v>137</v>
@@ -13041,7 +13077,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B129" t="s">
         <v>137</v>
@@ -13049,7 +13085,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B130" t="s">
         <v>137</v>
@@ -13057,7 +13093,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B131" t="s">
         <v>137</v>
@@ -13065,7 +13101,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B132" t="s">
         <v>137</v>
@@ -13073,7 +13109,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B133" t="s">
         <v>137</v>
@@ -13081,7 +13117,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="B134" t="s">
         <v>137</v>
@@ -13089,7 +13125,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B135" t="s">
         <v>137</v>
@@ -13097,7 +13133,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B136" t="s">
         <v>137</v>
@@ -13105,7 +13141,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B137" t="s">
         <v>137</v>
@@ -13113,7 +13149,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>435</v>
+        <v>70</v>
       </c>
       <c r="B138" t="s">
         <v>137</v>
@@ -13121,7 +13157,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>71</v>
+        <v>434</v>
       </c>
       <c r="B139" t="s">
         <v>137</v>
@@ -13129,7 +13165,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B140" t="s">
         <v>137</v>
@@ -13137,15 +13173,15 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>579</v>
+        <v>72</v>
       </c>
       <c r="B141" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B142" t="s">
         <v>174</v>
@@ -13161,7 +13197,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>15</v>
+        <v>579</v>
       </c>
       <c r="B144" t="s">
         <v>174</v>
@@ -13169,14 +13205,22 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B145" t="s">
         <v>174</v>
       </c>
     </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>12</v>
+      </c>
+      <c r="B146" t="s">
+        <v>174</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B136">
+  <autoFilter ref="A1:B137">
     <sortState ref="A2:B139">
       <sortCondition ref="A1:A130"/>
     </sortState>

</xml_diff>

<commit_message>
MingMing name reverted to single word.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13014" windowHeight="10610" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13014" windowHeight="10610"/>
   </bookViews>
   <sheets>
     <sheet name="skills" sheetId="1" r:id="rId1"/>
@@ -2760,9 +2760,6 @@
     <t>mingming_6_2</t>
   </si>
   <si>
-    <t>Sprout's Friend Ming Ming</t>
-  </si>
-  <si>
     <t>Static Name</t>
   </si>
   <si>
@@ -2806,6 +2803,9 @@
   </si>
   <si>
     <t>mingming_6</t>
+  </si>
+  <si>
+    <t>Sprout's Friend MingMing</t>
   </si>
 </sst>
 </file>
@@ -3132,8 +3132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE258"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88:B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -6406,7 +6406,7 @@
         <v>906</v>
       </c>
       <c r="B88" t="s">
-        <v>909</v>
+        <v>924</v>
       </c>
       <c r="C88" t="s">
         <v>364</v>
@@ -6447,7 +6447,7 @@
         <v>907</v>
       </c>
       <c r="B89" t="s">
-        <v>909</v>
+        <v>924</v>
       </c>
       <c r="C89" t="s">
         <v>365</v>
@@ -6479,7 +6479,7 @@
         <v>908</v>
       </c>
       <c r="B90" t="s">
-        <v>909</v>
+        <v>924</v>
       </c>
       <c r="C90" t="s">
         <v>366</v>
@@ -12405,7 +12405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+    <sheetView topLeftCell="A47" workbookViewId="0">
       <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
@@ -12417,40 +12417,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>909</v>
+      </c>
+      <c r="B1" t="s">
+        <v>911</v>
+      </c>
+      <c r="C1" t="s">
         <v>910</v>
       </c>
-      <c r="B1" t="s">
-        <v>912</v>
-      </c>
-      <c r="C1" t="s">
-        <v>911</v>
-      </c>
       <c r="D1" t="s">
+        <v>914</v>
+      </c>
+      <c r="E1" t="s">
         <v>915</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>916</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>917</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>918</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>919</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>920</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>921</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>922</v>
-      </c>
-      <c r="L1" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -12458,7 +12458,7 @@
         <v>812</v>
       </c>
       <c r="B2" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C2">
         <v>19</v>
@@ -12469,7 +12469,7 @@
         <v>813</v>
       </c>
       <c r="B3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C3">
         <v>21</v>
@@ -12480,7 +12480,7 @@
         <v>814</v>
       </c>
       <c r="B4" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C4">
         <v>21</v>
@@ -12491,7 +12491,7 @@
         <v>815</v>
       </c>
       <c r="B5" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C5">
         <v>31</v>
@@ -12502,7 +12502,7 @@
         <v>816</v>
       </c>
       <c r="B6" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C6">
         <v>21</v>
@@ -12513,7 +12513,7 @@
         <v>817</v>
       </c>
       <c r="B7" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C7">
         <v>21</v>
@@ -12524,7 +12524,7 @@
         <v>818</v>
       </c>
       <c r="B8" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C8">
         <v>21</v>
@@ -12535,7 +12535,7 @@
         <v>819</v>
       </c>
       <c r="B9" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C9">
         <v>22</v>
@@ -12546,7 +12546,7 @@
         <v>820</v>
       </c>
       <c r="B10" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C10">
         <v>14</v>
@@ -12557,7 +12557,7 @@
         <v>821</v>
       </c>
       <c r="B11" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C11">
         <v>12</v>
@@ -12568,7 +12568,7 @@
         <v>822</v>
       </c>
       <c r="B12" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C12">
         <v>26</v>
@@ -12579,7 +12579,7 @@
         <v>823</v>
       </c>
       <c r="B13" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C13">
         <v>16</v>
@@ -12590,7 +12590,7 @@
         <v>824</v>
       </c>
       <c r="B14" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C14">
         <v>12</v>
@@ -12601,7 +12601,7 @@
         <v>825</v>
       </c>
       <c r="B15" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C15">
         <v>26</v>
@@ -12612,7 +12612,7 @@
         <v>826</v>
       </c>
       <c r="B16" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C16">
         <v>14</v>
@@ -12623,7 +12623,7 @@
         <v>827</v>
       </c>
       <c r="B17" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C17">
         <v>26</v>
@@ -12634,7 +12634,7 @@
         <v>828</v>
       </c>
       <c r="B18" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C18">
         <v>26</v>
@@ -12645,7 +12645,7 @@
         <v>829</v>
       </c>
       <c r="B19" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C19">
         <v>26</v>
@@ -12656,7 +12656,7 @@
         <v>830</v>
       </c>
       <c r="B20" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C20">
         <v>12</v>
@@ -12667,7 +12667,7 @@
         <v>831</v>
       </c>
       <c r="B21" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C21">
         <v>16</v>
@@ -12678,7 +12678,7 @@
         <v>832</v>
       </c>
       <c r="B22" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C22">
         <v>12</v>
@@ -12689,7 +12689,7 @@
         <v>833</v>
       </c>
       <c r="B23" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C23">
         <v>26</v>
@@ -12700,7 +12700,7 @@
         <v>834</v>
       </c>
       <c r="B24" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C24">
         <v>26</v>
@@ -12711,7 +12711,7 @@
         <v>835</v>
       </c>
       <c r="B25" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C25">
         <v>14</v>
@@ -12722,7 +12722,7 @@
         <v>836</v>
       </c>
       <c r="B26" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C26">
         <v>16</v>
@@ -12733,7 +12733,7 @@
         <v>837</v>
       </c>
       <c r="B27" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C27">
         <v>26</v>
@@ -12744,7 +12744,7 @@
         <v>838</v>
       </c>
       <c r="B28" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C28">
         <v>26</v>
@@ -12755,7 +12755,7 @@
         <v>839</v>
       </c>
       <c r="B29" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C29">
         <v>12</v>
@@ -12766,7 +12766,7 @@
         <v>840</v>
       </c>
       <c r="B30" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C30">
         <v>20</v>
@@ -12774,10 +12774,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B31" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C31">
         <v>27</v>
@@ -12788,7 +12788,7 @@
         <v>841</v>
       </c>
       <c r="B32" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C32">
         <v>26</v>
@@ -12799,7 +12799,7 @@
         <v>842</v>
       </c>
       <c r="B33" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C33">
         <v>30</v>
@@ -12810,7 +12810,7 @@
         <v>843</v>
       </c>
       <c r="B34" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C34">
         <v>26</v>
@@ -12821,7 +12821,7 @@
         <v>844</v>
       </c>
       <c r="B35" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C35">
         <v>26</v>
@@ -12832,7 +12832,7 @@
         <v>845</v>
       </c>
       <c r="B36" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C36">
         <v>16</v>
@@ -12843,7 +12843,7 @@
         <v>846</v>
       </c>
       <c r="B37" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C37">
         <v>16</v>
@@ -12854,7 +12854,7 @@
         <v>847</v>
       </c>
       <c r="B38" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C38">
         <v>16</v>
@@ -12865,7 +12865,7 @@
         <v>848</v>
       </c>
       <c r="B39" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C39">
         <v>20</v>
@@ -12876,7 +12876,7 @@
         <v>849</v>
       </c>
       <c r="B40" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C40">
         <v>14</v>
@@ -12887,7 +12887,7 @@
         <v>850</v>
       </c>
       <c r="B41" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C41">
         <v>12</v>
@@ -12898,7 +12898,7 @@
         <v>851</v>
       </c>
       <c r="B42" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C42">
         <v>26</v>
@@ -12909,7 +12909,7 @@
         <v>852</v>
       </c>
       <c r="B43" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C43">
         <v>26</v>
@@ -12920,7 +12920,7 @@
         <v>853</v>
       </c>
       <c r="B44" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C44">
         <v>8</v>
@@ -12931,7 +12931,7 @@
         <v>854</v>
       </c>
       <c r="B45" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C45">
         <v>6</v>
@@ -12942,7 +12942,7 @@
         <v>855</v>
       </c>
       <c r="B46" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C46">
         <v>8</v>
@@ -12953,7 +12953,7 @@
         <v>856</v>
       </c>
       <c r="B47" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C47">
         <v>10</v>
@@ -12964,7 +12964,7 @@
         <v>857</v>
       </c>
       <c r="B48" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C48">
         <v>13</v>
@@ -12975,7 +12975,7 @@
         <v>858</v>
       </c>
       <c r="B49" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C49">
         <v>13</v>
@@ -12986,7 +12986,7 @@
         <v>859</v>
       </c>
       <c r="B50" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C50">
         <v>16</v>
@@ -12997,7 +12997,7 @@
         <v>860</v>
       </c>
       <c r="B51" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C51">
         <v>13</v>
@@ -13008,7 +13008,7 @@
         <v>861</v>
       </c>
       <c r="B52" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C52">
         <v>13</v>
@@ -13019,7 +13019,7 @@
         <v>862</v>
       </c>
       <c r="B53" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C53">
         <v>13</v>
@@ -13030,7 +13030,7 @@
         <v>863</v>
       </c>
       <c r="B54" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C54">
         <v>13</v>
@@ -13041,7 +13041,7 @@
         <v>864</v>
       </c>
       <c r="B55" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C55">
         <v>13</v>
@@ -13052,7 +13052,7 @@
         <v>865</v>
       </c>
       <c r="B56" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C56">
         <v>13</v>
@@ -13063,7 +13063,7 @@
         <v>866</v>
       </c>
       <c r="B57" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C57">
         <v>12</v>
@@ -13074,7 +13074,7 @@
         <v>867</v>
       </c>
       <c r="B58" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C58">
         <v>13</v>
@@ -13085,7 +13085,7 @@
         <v>868</v>
       </c>
       <c r="B59" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C59">
         <v>13</v>
@@ -13096,7 +13096,7 @@
         <v>869</v>
       </c>
       <c r="B60" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C60">
         <v>13</v>
@@ -13107,7 +13107,7 @@
         <v>870</v>
       </c>
       <c r="B61" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C61">
         <v>8</v>
@@ -13118,7 +13118,7 @@
         <v>871</v>
       </c>
       <c r="B62" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C62">
         <v>8</v>
@@ -13129,7 +13129,7 @@
         <v>872</v>
       </c>
       <c r="B63" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C63">
         <v>16</v>
@@ -13140,7 +13140,7 @@
         <v>873</v>
       </c>
       <c r="B64" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C64">
         <v>20</v>
@@ -13151,7 +13151,7 @@
         <v>874</v>
       </c>
       <c r="B65" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C65">
         <v>8</v>
@@ -13162,7 +13162,7 @@
         <v>875</v>
       </c>
       <c r="B66" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C66">
         <v>13</v>
@@ -13173,7 +13173,7 @@
         <v>876</v>
       </c>
       <c r="B67" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C67">
         <v>13</v>
@@ -13184,7 +13184,7 @@
         <v>877</v>
       </c>
       <c r="B68" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C68">
         <v>16</v>
@@ -13195,7 +13195,7 @@
         <v>878</v>
       </c>
       <c r="B69" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C69">
         <v>20</v>
@@ -13206,7 +13206,7 @@
         <v>879</v>
       </c>
       <c r="B70" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C70">
         <v>20</v>
@@ -13217,7 +13217,7 @@
         <v>880</v>
       </c>
       <c r="B71" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C71">
         <v>16</v>
@@ -13228,7 +13228,7 @@
         <v>881</v>
       </c>
       <c r="B72" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C72">
         <v>13</v>
@@ -13239,7 +13239,7 @@
         <v>882</v>
       </c>
       <c r="B73" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C73">
         <v>13</v>
@@ -13250,7 +13250,7 @@
         <v>883</v>
       </c>
       <c r="B74" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C74">
         <v>13</v>
@@ -13261,7 +13261,7 @@
         <v>884</v>
       </c>
       <c r="B75" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C75">
         <v>13</v>
@@ -13272,7 +13272,7 @@
         <v>885</v>
       </c>
       <c r="B76" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C76">
         <v>8</v>
@@ -13283,7 +13283,7 @@
         <v>886</v>
       </c>
       <c r="B77" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C77">
         <v>20</v>
@@ -13294,7 +13294,7 @@
         <v>887</v>
       </c>
       <c r="B78" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C78">
         <v>16</v>
@@ -13305,7 +13305,7 @@
         <v>888</v>
       </c>
       <c r="B79" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C79">
         <v>13</v>
@@ -13316,7 +13316,7 @@
         <v>889</v>
       </c>
       <c r="B80" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C80">
         <v>13</v>
@@ -13327,7 +13327,7 @@
         <v>890</v>
       </c>
       <c r="B81" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C81">
         <v>10</v>
@@ -13338,7 +13338,7 @@
         <v>891</v>
       </c>
       <c r="B82" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C82">
         <v>20</v>
@@ -13349,7 +13349,7 @@
         <v>892</v>
       </c>
       <c r="B83" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C83">
         <v>10</v>
@@ -13360,7 +13360,7 @@
         <v>893</v>
       </c>
       <c r="B84" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C84">
         <v>16</v>
@@ -13371,7 +13371,7 @@
         <v>894</v>
       </c>
       <c r="B85" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C85">
         <v>16</v>
@@ -13382,7 +13382,7 @@
         <v>895</v>
       </c>
       <c r="B86" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C86">
         <v>13</v>
@@ -13393,7 +13393,7 @@
         <v>896</v>
       </c>
       <c r="B87" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C87">
         <v>10</v>
@@ -13404,7 +13404,7 @@
         <v>897</v>
       </c>
       <c r="B88" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C88">
         <v>16</v>
@@ -13415,7 +13415,7 @@
         <v>898</v>
       </c>
       <c r="B89" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C89">
         <v>20</v>
@@ -13426,7 +13426,7 @@
         <v>899</v>
       </c>
       <c r="B90" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C90">
         <v>16</v>
@@ -13437,7 +13437,7 @@
         <v>900</v>
       </c>
       <c r="B91" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C91">
         <v>12</v>
@@ -13448,7 +13448,7 @@
         <v>901</v>
       </c>
       <c r="B92" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C92">
         <v>16</v>
@@ -13459,7 +13459,7 @@
         <v>902</v>
       </c>
       <c r="B93" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C93">
         <v>14</v>
@@ -13470,7 +13470,7 @@
         <v>903</v>
       </c>
       <c r="B94" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C94">
         <v>12</v>
@@ -13481,7 +13481,7 @@
         <v>904</v>
       </c>
       <c r="B95" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C95">
         <v>27</v>
@@ -13492,7 +13492,7 @@
         <v>905</v>
       </c>
       <c r="B96" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C96">
         <v>28</v>

</xml_diff>

<commit_message>
Prep work for the remainder of stats.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13014" windowHeight="10610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13014" windowHeight="10610" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="skills" sheetId="1" r:id="rId1"/>
@@ -3132,7 +3132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B88" sqref="B88:B90"/>
     </sheetView>
   </sheetViews>
@@ -12405,8 +12405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L96"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -13500,6 +13500,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Wired Stat logic to View and JS.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -14,11 +14,12 @@
   <sheets>
     <sheet name="skills" sheetId="1" r:id="rId1"/>
     <sheet name="stats" sheetId="4" r:id="rId2"/>
-    <sheet name="attributes" sheetId="2" r:id="rId3"/>
-    <sheet name="LUT" sheetId="3" r:id="rId4"/>
+    <sheet name="stats_base" sheetId="5" r:id="rId3"/>
+    <sheet name="attributes" sheetId="2" r:id="rId4"/>
+    <sheet name="LUT" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">attributes!$A$1:$B$137</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">attributes!$A$1:$B$137</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">skills!$A$1:$AE$246</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2695" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2805" uniqueCount="937">
   <si>
     <t>attributes</t>
   </si>
@@ -2806,6 +2807,42 @@
   </si>
   <si>
     <t>Sprout's Friend MingMing</t>
+  </si>
+  <si>
+    <t>element</t>
+  </si>
+  <si>
+    <t>7_knight</t>
+  </si>
+  <si>
+    <t>4_lord</t>
+  </si>
+  <si>
+    <t>regular</t>
+  </si>
+  <si>
+    <t>asgar</t>
+  </si>
+  <si>
+    <t>aisha</t>
+  </si>
+  <si>
+    <t>earth</t>
+  </si>
+  <si>
+    <t>dark</t>
+  </si>
+  <si>
+    <t>fire</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>light</t>
+  </si>
+  <si>
+    <t>surrogate</t>
   </si>
 </sst>
 </file>
@@ -2821,7 +2858,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2831,6 +2868,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2847,9 +2890,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12403,10 +12447,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L96"/>
+  <dimension ref="A1:N96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:L2"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -12415,7 +12459,7 @@
     <col min="2" max="2" width="4.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>909</v>
       </c>
@@ -12452,8 +12496,14 @@
       <c r="L1" t="s">
         <v>922</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>139</v>
+      </c>
+      <c r="N1" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>812</v>
       </c>
@@ -12463,8 +12513,50 @@
       <c r="C2">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M2,"_",$N2),stats_base!$C:$C,0))</f>
+        <v>1743</v>
+      </c>
+      <c r="E2">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M2,"_",$N2),stats_base!$C:$C,0))</f>
+        <v>460</v>
+      </c>
+      <c r="F2">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M2,"_",$N2),stats_base!$C:$C,0))</f>
+        <v>475</v>
+      </c>
+      <c r="G2">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M2,"_",$N2),stats_base!$C:$C,0))</f>
+        <v>4275</v>
+      </c>
+      <c r="H2">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M2,"_",$N2),stats_base!$C:$C,0))</f>
+        <v>1180</v>
+      </c>
+      <c r="I2">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M2,"_",$N2),stats_base!$C:$C,0))</f>
+        <v>1189</v>
+      </c>
+      <c r="J2">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M2,"_",$N2),stats_base!$C:$C,0))</f>
+        <v>5070</v>
+      </c>
+      <c r="K2">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M2,"_",$N2),stats_base!$C:$C,0))</f>
+        <v>1315</v>
+      </c>
+      <c r="L2">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M2,"_",$N2),stats_base!$C:$C,0))</f>
+        <v>1334</v>
+      </c>
+      <c r="M2" t="s">
+        <v>926</v>
+      </c>
+      <c r="N2" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>813</v>
       </c>
@@ -12474,8 +12566,50 @@
       <c r="C3">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M3,"_",$N3),stats_base!$C:$C,0))</f>
+        <v>1086</v>
+      </c>
+      <c r="E3">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M3,"_",$N3),stats_base!$C:$C,0))</f>
+        <v>696</v>
+      </c>
+      <c r="F3">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M3,"_",$N3),stats_base!$C:$C,0))</f>
+        <v>328</v>
+      </c>
+      <c r="G3">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M3,"_",$N3),stats_base!$C:$C,0))</f>
+        <v>2730</v>
+      </c>
+      <c r="H3">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M3,"_",$N3),stats_base!$C:$C,0))</f>
+        <v>1680</v>
+      </c>
+      <c r="I3">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M3,"_",$N3),stats_base!$C:$C,0))</f>
+        <v>874</v>
+      </c>
+      <c r="J3">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M3,"_",$N3),stats_base!$C:$C,0))</f>
+        <v>3205</v>
+      </c>
+      <c r="K3">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M3,"_",$N3),stats_base!$C:$C,0))</f>
+        <v>1910</v>
+      </c>
+      <c r="L3">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M3,"_",$N3),stats_base!$C:$C,0))</f>
+        <v>979</v>
+      </c>
+      <c r="M3" t="s">
+        <v>926</v>
+      </c>
+      <c r="N3" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>814</v>
       </c>
@@ -12485,8 +12619,50 @@
       <c r="C4">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M4,"_",$N4),stats_base!$C:$C,0))</f>
+        <v>1086</v>
+      </c>
+      <c r="E4">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M4,"_",$N4),stats_base!$C:$C,0))</f>
+        <v>696</v>
+      </c>
+      <c r="F4">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M4,"_",$N4),stats_base!$C:$C,0))</f>
+        <v>328</v>
+      </c>
+      <c r="G4">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M4,"_",$N4),stats_base!$C:$C,0))</f>
+        <v>2730</v>
+      </c>
+      <c r="H4">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M4,"_",$N4),stats_base!$C:$C,0))</f>
+        <v>1680</v>
+      </c>
+      <c r="I4">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M4,"_",$N4),stats_base!$C:$C,0))</f>
+        <v>874</v>
+      </c>
+      <c r="J4">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M4,"_",$N4),stats_base!$C:$C,0))</f>
+        <v>3205</v>
+      </c>
+      <c r="K4">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M4,"_",$N4),stats_base!$C:$C,0))</f>
+        <v>1910</v>
+      </c>
+      <c r="L4">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M4,"_",$N4),stats_base!$C:$C,0))</f>
+        <v>979</v>
+      </c>
+      <c r="M4" t="s">
+        <v>926</v>
+      </c>
+      <c r="N4" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>815</v>
       </c>
@@ -12496,8 +12672,50 @@
       <c r="C5">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M5,"_",$N5),stats_base!$C:$C,0))</f>
+        <v>1486</v>
+      </c>
+      <c r="E5">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M5,"_",$N5),stats_base!$C:$C,0))</f>
+        <v>637</v>
+      </c>
+      <c r="F5">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M5,"_",$N5),stats_base!$C:$C,0))</f>
+        <v>415</v>
+      </c>
+      <c r="G5">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M5,"_",$N5),stats_base!$C:$C,0))</f>
+        <v>3688</v>
+      </c>
+      <c r="H5">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M5,"_",$N5),stats_base!$C:$C,0))</f>
+        <v>1555</v>
+      </c>
+      <c r="I5">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M5,"_",$N5),stats_base!$C:$C,0))</f>
+        <v>1039</v>
+      </c>
+      <c r="J5">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M5,"_",$N5),stats_base!$C:$C,0))</f>
+        <v>4343</v>
+      </c>
+      <c r="K5">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M5,"_",$N5),stats_base!$C:$C,0))</f>
+        <v>1750</v>
+      </c>
+      <c r="L5">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M5,"_",$N5),stats_base!$C:$C,0))</f>
+        <v>1174</v>
+      </c>
+      <c r="M5" t="s">
+        <v>926</v>
+      </c>
+      <c r="N5" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>816</v>
       </c>
@@ -12507,8 +12725,50 @@
       <c r="C6">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M6,"_",$N6),stats_base!$C:$C,0))</f>
+        <v>1486</v>
+      </c>
+      <c r="E6">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M6,"_",$N6),stats_base!$C:$C,0))</f>
+        <v>637</v>
+      </c>
+      <c r="F6">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M6,"_",$N6),stats_base!$C:$C,0))</f>
+        <v>415</v>
+      </c>
+      <c r="G6">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M6,"_",$N6),stats_base!$C:$C,0))</f>
+        <v>3688</v>
+      </c>
+      <c r="H6">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M6,"_",$N6),stats_base!$C:$C,0))</f>
+        <v>1555</v>
+      </c>
+      <c r="I6">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M6,"_",$N6),stats_base!$C:$C,0))</f>
+        <v>1039</v>
+      </c>
+      <c r="J6">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M6,"_",$N6),stats_base!$C:$C,0))</f>
+        <v>4343</v>
+      </c>
+      <c r="K6">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M6,"_",$N6),stats_base!$C:$C,0))</f>
+        <v>1750</v>
+      </c>
+      <c r="L6">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M6,"_",$N6),stats_base!$C:$C,0))</f>
+        <v>1174</v>
+      </c>
+      <c r="M6" t="s">
+        <v>926</v>
+      </c>
+      <c r="N6" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>817</v>
       </c>
@@ -12518,8 +12778,50 @@
       <c r="C7">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M7,"_",$N7),stats_base!$C:$C,0))</f>
+        <v>1486</v>
+      </c>
+      <c r="E7">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M7,"_",$N7),stats_base!$C:$C,0))</f>
+        <v>637</v>
+      </c>
+      <c r="F7">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M7,"_",$N7),stats_base!$C:$C,0))</f>
+        <v>415</v>
+      </c>
+      <c r="G7">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M7,"_",$N7),stats_base!$C:$C,0))</f>
+        <v>3688</v>
+      </c>
+      <c r="H7">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M7,"_",$N7),stats_base!$C:$C,0))</f>
+        <v>1555</v>
+      </c>
+      <c r="I7">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M7,"_",$N7),stats_base!$C:$C,0))</f>
+        <v>1039</v>
+      </c>
+      <c r="J7">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M7,"_",$N7),stats_base!$C:$C,0))</f>
+        <v>4343</v>
+      </c>
+      <c r="K7">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M7,"_",$N7),stats_base!$C:$C,0))</f>
+        <v>1750</v>
+      </c>
+      <c r="L7">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M7,"_",$N7),stats_base!$C:$C,0))</f>
+        <v>1174</v>
+      </c>
+      <c r="M7" t="s">
+        <v>926</v>
+      </c>
+      <c r="N7" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>818</v>
       </c>
@@ -12529,8 +12831,50 @@
       <c r="C8">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M8,"_",$N8),stats_base!$C:$C,0))</f>
+        <v>1486</v>
+      </c>
+      <c r="E8">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M8,"_",$N8),stats_base!$C:$C,0))</f>
+        <v>637</v>
+      </c>
+      <c r="F8">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M8,"_",$N8),stats_base!$C:$C,0))</f>
+        <v>415</v>
+      </c>
+      <c r="G8">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M8,"_",$N8),stats_base!$C:$C,0))</f>
+        <v>3688</v>
+      </c>
+      <c r="H8">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M8,"_",$N8),stats_base!$C:$C,0))</f>
+        <v>1555</v>
+      </c>
+      <c r="I8">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M8,"_",$N8),stats_base!$C:$C,0))</f>
+        <v>1039</v>
+      </c>
+      <c r="J8">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M8,"_",$N8),stats_base!$C:$C,0))</f>
+        <v>4343</v>
+      </c>
+      <c r="K8">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M8,"_",$N8),stats_base!$C:$C,0))</f>
+        <v>1750</v>
+      </c>
+      <c r="L8">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M8,"_",$N8),stats_base!$C:$C,0))</f>
+        <v>1174</v>
+      </c>
+      <c r="M8" t="s">
+        <v>926</v>
+      </c>
+      <c r="N8" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>819</v>
       </c>
@@ -12540,8 +12884,41 @@
       <c r="C9">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D9" s="2">
+        <v>1451</v>
+      </c>
+      <c r="E9" s="2">
+        <v>622</v>
+      </c>
+      <c r="F9" s="2">
+        <v>380</v>
+      </c>
+      <c r="G9" s="2">
+        <v>3617</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1516</v>
+      </c>
+      <c r="I9" s="2">
+        <v>950</v>
+      </c>
+      <c r="J9" s="2">
+        <v>4272</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1711</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1085</v>
+      </c>
+      <c r="M9" t="s">
+        <v>927</v>
+      </c>
+      <c r="N9" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>820</v>
       </c>
@@ -12551,8 +12928,50 @@
       <c r="C10">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M10,"_",$N10),stats_base!$C:$C,0))</f>
+        <v>1456</v>
+      </c>
+      <c r="E10">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M10,"_",$N10),stats_base!$C:$C,0))</f>
+        <v>333</v>
+      </c>
+      <c r="F10">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M10,"_",$N10),stats_base!$C:$C,0))</f>
+        <v>347</v>
+      </c>
+      <c r="G10">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M10,"_",$N10),stats_base!$C:$C,0))</f>
+        <v>3808</v>
+      </c>
+      <c r="H10">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M10,"_",$N10),stats_base!$C:$C,0))</f>
+        <v>873</v>
+      </c>
+      <c r="I10">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M10,"_",$N10),stats_base!$C:$C,0))</f>
+        <v>881</v>
+      </c>
+      <c r="J10">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M10,"_",$N10),stats_base!$C:$C,0))</f>
+        <v>4603</v>
+      </c>
+      <c r="K10">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M10,"_",$N10),stats_base!$C:$C,0))</f>
+        <v>1008</v>
+      </c>
+      <c r="L10">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M10,"_",$N10),stats_base!$C:$C,0))</f>
+        <v>1026</v>
+      </c>
+      <c r="M10" t="s">
+        <v>928</v>
+      </c>
+      <c r="N10" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>821</v>
       </c>
@@ -12562,8 +12981,41 @@
       <c r="C11">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D11" s="2">
+        <v>1076</v>
+      </c>
+      <c r="E11" s="2">
+        <v>377</v>
+      </c>
+      <c r="F11" s="2">
+        <v>236</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2762</v>
+      </c>
+      <c r="H11" s="2">
+        <v>983</v>
+      </c>
+      <c r="I11" s="2">
+        <v>632</v>
+      </c>
+      <c r="J11" s="2">
+        <v>3302</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1128</v>
+      </c>
+      <c r="L11" s="2">
+        <v>742</v>
+      </c>
+      <c r="M11" t="s">
+        <v>928</v>
+      </c>
+      <c r="N11" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>822</v>
       </c>
@@ -12573,8 +13025,50 @@
       <c r="C12">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M12,"_",$N12),stats_base!$C:$C,0))</f>
+        <v>882</v>
+      </c>
+      <c r="E12">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M12,"_",$N12),stats_base!$C:$C,0))</f>
+        <v>511</v>
+      </c>
+      <c r="F12">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M12,"_",$N12),stats_base!$C:$C,0))</f>
+        <v>199</v>
+      </c>
+      <c r="G12">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M12,"_",$N12),stats_base!$C:$C,0))</f>
+        <v>2310</v>
+      </c>
+      <c r="H12">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M12,"_",$N12),stats_base!$C:$C,0))</f>
+        <v>1279</v>
+      </c>
+      <c r="I12">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M12,"_",$N12),stats_base!$C:$C,0))</f>
+        <v>529</v>
+      </c>
+      <c r="J12">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M12,"_",$N12),stats_base!$C:$C,0))</f>
+        <v>2785</v>
+      </c>
+      <c r="K12">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M12,"_",$N12),stats_base!$C:$C,0))</f>
+        <v>1509</v>
+      </c>
+      <c r="L12">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M12,"_",$N12),stats_base!$C:$C,0))</f>
+        <v>634</v>
+      </c>
+      <c r="M12" t="s">
+        <v>928</v>
+      </c>
+      <c r="N12" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>823</v>
       </c>
@@ -12584,8 +13078,50 @@
       <c r="C13">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M13,"_",$N13),stats_base!$C:$C,0))</f>
+        <v>1231</v>
+      </c>
+      <c r="E13">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M13,"_",$N13),stats_base!$C:$C,0))</f>
+        <v>467</v>
+      </c>
+      <c r="F13">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M13,"_",$N13),stats_base!$C:$C,0))</f>
+        <v>270</v>
+      </c>
+      <c r="G13">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M13,"_",$N13),stats_base!$C:$C,0))</f>
+        <v>3217</v>
+      </c>
+      <c r="H13">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M13,"_",$N13),stats_base!$C:$C,0))</f>
+        <v>1169</v>
+      </c>
+      <c r="I13">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M13,"_",$N13),stats_base!$C:$C,0))</f>
+        <v>678</v>
+      </c>
+      <c r="J13">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M13,"_",$N13),stats_base!$C:$C,0))</f>
+        <v>3872</v>
+      </c>
+      <c r="K13">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M13,"_",$N13),stats_base!$C:$C,0))</f>
+        <v>1364</v>
+      </c>
+      <c r="L13">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M13,"_",$N13),stats_base!$C:$C,0))</f>
+        <v>813</v>
+      </c>
+      <c r="M13" t="s">
+        <v>928</v>
+      </c>
+      <c r="N13" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>824</v>
       </c>
@@ -12595,8 +13131,41 @@
       <c r="C14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D14" s="2">
+        <v>1049</v>
+      </c>
+      <c r="E14" s="2">
+        <v>360</v>
+      </c>
+      <c r="F14" s="2">
+        <v>219</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2699</v>
+      </c>
+      <c r="H14" s="2">
+        <v>930</v>
+      </c>
+      <c r="I14" s="2">
+        <v>579</v>
+      </c>
+      <c r="J14" s="2">
+        <v>3239</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1075</v>
+      </c>
+      <c r="L14" s="2">
+        <v>689</v>
+      </c>
+      <c r="M14" t="s">
+        <v>928</v>
+      </c>
+      <c r="N14" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>825</v>
       </c>
@@ -12606,8 +13175,50 @@
       <c r="C15">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M15,"_",$N15),stats_base!$C:$C,0))</f>
+        <v>882</v>
+      </c>
+      <c r="E15">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M15,"_",$N15),stats_base!$C:$C,0))</f>
+        <v>511</v>
+      </c>
+      <c r="F15">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M15,"_",$N15),stats_base!$C:$C,0))</f>
+        <v>199</v>
+      </c>
+      <c r="G15">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M15,"_",$N15),stats_base!$C:$C,0))</f>
+        <v>2310</v>
+      </c>
+      <c r="H15">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M15,"_",$N15),stats_base!$C:$C,0))</f>
+        <v>1279</v>
+      </c>
+      <c r="I15">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M15,"_",$N15),stats_base!$C:$C,0))</f>
+        <v>529</v>
+      </c>
+      <c r="J15">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M15,"_",$N15),stats_base!$C:$C,0))</f>
+        <v>2785</v>
+      </c>
+      <c r="K15">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M15,"_",$N15),stats_base!$C:$C,0))</f>
+        <v>1509</v>
+      </c>
+      <c r="L15">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M15,"_",$N15),stats_base!$C:$C,0))</f>
+        <v>634</v>
+      </c>
+      <c r="M15" t="s">
+        <v>928</v>
+      </c>
+      <c r="N15" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>826</v>
       </c>
@@ -12617,8 +13228,41 @@
       <c r="C16">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="2">
+        <v>1439</v>
+      </c>
+      <c r="E16" s="2">
+        <v>315</v>
+      </c>
+      <c r="F16" s="2">
+        <v>323</v>
+      </c>
+      <c r="G16" s="2">
+        <v>3755</v>
+      </c>
+      <c r="H16" s="2">
+        <v>819</v>
+      </c>
+      <c r="I16" s="2">
+        <v>821</v>
+      </c>
+      <c r="J16" s="2">
+        <v>4550</v>
+      </c>
+      <c r="K16" s="2">
+        <v>954</v>
+      </c>
+      <c r="L16" s="2">
+        <v>966</v>
+      </c>
+      <c r="M16" t="s">
+        <v>928</v>
+      </c>
+      <c r="N16" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>827</v>
       </c>
@@ -12628,8 +13272,50 @@
       <c r="C17">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M17,"_",$N17),stats_base!$C:$C,0))</f>
+        <v>882</v>
+      </c>
+      <c r="E17">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M17,"_",$N17),stats_base!$C:$C,0))</f>
+        <v>511</v>
+      </c>
+      <c r="F17">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M17,"_",$N17),stats_base!$C:$C,0))</f>
+        <v>199</v>
+      </c>
+      <c r="G17">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M17,"_",$N17),stats_base!$C:$C,0))</f>
+        <v>2310</v>
+      </c>
+      <c r="H17">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M17,"_",$N17),stats_base!$C:$C,0))</f>
+        <v>1279</v>
+      </c>
+      <c r="I17">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M17,"_",$N17),stats_base!$C:$C,0))</f>
+        <v>529</v>
+      </c>
+      <c r="J17">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M17,"_",$N17),stats_base!$C:$C,0))</f>
+        <v>2785</v>
+      </c>
+      <c r="K17">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M17,"_",$N17),stats_base!$C:$C,0))</f>
+        <v>1509</v>
+      </c>
+      <c r="L17">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M17,"_",$N17),stats_base!$C:$C,0))</f>
+        <v>634</v>
+      </c>
+      <c r="M17" t="s">
+        <v>928</v>
+      </c>
+      <c r="N17" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>828</v>
       </c>
@@ -12639,8 +13325,50 @@
       <c r="C18">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M18,"_",$N18),stats_base!$C:$C,0))</f>
+        <v>882</v>
+      </c>
+      <c r="E18">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M18,"_",$N18),stats_base!$C:$C,0))</f>
+        <v>511</v>
+      </c>
+      <c r="F18">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M18,"_",$N18),stats_base!$C:$C,0))</f>
+        <v>199</v>
+      </c>
+      <c r="G18">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M18,"_",$N18),stats_base!$C:$C,0))</f>
+        <v>2310</v>
+      </c>
+      <c r="H18">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M18,"_",$N18),stats_base!$C:$C,0))</f>
+        <v>1279</v>
+      </c>
+      <c r="I18">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M18,"_",$N18),stats_base!$C:$C,0))</f>
+        <v>529</v>
+      </c>
+      <c r="J18">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M18,"_",$N18),stats_base!$C:$C,0))</f>
+        <v>2785</v>
+      </c>
+      <c r="K18">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M18,"_",$N18),stats_base!$C:$C,0))</f>
+        <v>1509</v>
+      </c>
+      <c r="L18">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M18,"_",$N18),stats_base!$C:$C,0))</f>
+        <v>634</v>
+      </c>
+      <c r="M18" t="s">
+        <v>928</v>
+      </c>
+      <c r="N18" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>829</v>
       </c>
@@ -12650,8 +13378,50 @@
       <c r="C19">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M19,"_",$N19),stats_base!$C:$C,0))</f>
+        <v>882</v>
+      </c>
+      <c r="E19">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M19,"_",$N19),stats_base!$C:$C,0))</f>
+        <v>511</v>
+      </c>
+      <c r="F19">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M19,"_",$N19),stats_base!$C:$C,0))</f>
+        <v>199</v>
+      </c>
+      <c r="G19">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M19,"_",$N19),stats_base!$C:$C,0))</f>
+        <v>2310</v>
+      </c>
+      <c r="H19">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M19,"_",$N19),stats_base!$C:$C,0))</f>
+        <v>1279</v>
+      </c>
+      <c r="I19">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M19,"_",$N19),stats_base!$C:$C,0))</f>
+        <v>529</v>
+      </c>
+      <c r="J19">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M19,"_",$N19),stats_base!$C:$C,0))</f>
+        <v>2785</v>
+      </c>
+      <c r="K19">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M19,"_",$N19),stats_base!$C:$C,0))</f>
+        <v>1509</v>
+      </c>
+      <c r="L19">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M19,"_",$N19),stats_base!$C:$C,0))</f>
+        <v>634</v>
+      </c>
+      <c r="M19" t="s">
+        <v>928</v>
+      </c>
+      <c r="N19" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>830</v>
       </c>
@@ -12661,8 +13431,50 @@
       <c r="C20">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M20,"_",$N20),stats_base!$C:$C,0))</f>
+        <v>1049</v>
+      </c>
+      <c r="E20">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M20,"_",$N20),stats_base!$C:$C,0))</f>
+        <v>360</v>
+      </c>
+      <c r="F20">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M20,"_",$N20),stats_base!$C:$C,0))</f>
+        <v>219</v>
+      </c>
+      <c r="G20">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M20,"_",$N20),stats_base!$C:$C,0))</f>
+        <v>2699</v>
+      </c>
+      <c r="H20">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M20,"_",$N20),stats_base!$C:$C,0))</f>
+        <v>930</v>
+      </c>
+      <c r="I20">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M20,"_",$N20),stats_base!$C:$C,0))</f>
+        <v>579</v>
+      </c>
+      <c r="J20">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M20,"_",$N20),stats_base!$C:$C,0))</f>
+        <v>3239</v>
+      </c>
+      <c r="K20">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M20,"_",$N20),stats_base!$C:$C,0))</f>
+        <v>1075</v>
+      </c>
+      <c r="L20">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M20,"_",$N20),stats_base!$C:$C,0))</f>
+        <v>689</v>
+      </c>
+      <c r="M20" t="s">
+        <v>928</v>
+      </c>
+      <c r="N20" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>831</v>
       </c>
@@ -12672,8 +13484,50 @@
       <c r="C21">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M21,"_",$N21),stats_base!$C:$C,0))</f>
+        <v>1231</v>
+      </c>
+      <c r="E21">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M21,"_",$N21),stats_base!$C:$C,0))</f>
+        <v>467</v>
+      </c>
+      <c r="F21">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M21,"_",$N21),stats_base!$C:$C,0))</f>
+        <v>270</v>
+      </c>
+      <c r="G21">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M21,"_",$N21),stats_base!$C:$C,0))</f>
+        <v>3217</v>
+      </c>
+      <c r="H21">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M21,"_",$N21),stats_base!$C:$C,0))</f>
+        <v>1169</v>
+      </c>
+      <c r="I21">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M21,"_",$N21),stats_base!$C:$C,0))</f>
+        <v>678</v>
+      </c>
+      <c r="J21">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M21,"_",$N21),stats_base!$C:$C,0))</f>
+        <v>3872</v>
+      </c>
+      <c r="K21">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M21,"_",$N21),stats_base!$C:$C,0))</f>
+        <v>1364</v>
+      </c>
+      <c r="L21">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M21,"_",$N21),stats_base!$C:$C,0))</f>
+        <v>813</v>
+      </c>
+      <c r="M21" t="s">
+        <v>928</v>
+      </c>
+      <c r="N21" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>832</v>
       </c>
@@ -12683,8 +13537,50 @@
       <c r="C22">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M22,"_",$N22),stats_base!$C:$C,0))</f>
+        <v>1049</v>
+      </c>
+      <c r="E22">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M22,"_",$N22),stats_base!$C:$C,0))</f>
+        <v>360</v>
+      </c>
+      <c r="F22">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M22,"_",$N22),stats_base!$C:$C,0))</f>
+        <v>219</v>
+      </c>
+      <c r="G22">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M22,"_",$N22),stats_base!$C:$C,0))</f>
+        <v>2699</v>
+      </c>
+      <c r="H22">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M22,"_",$N22),stats_base!$C:$C,0))</f>
+        <v>930</v>
+      </c>
+      <c r="I22">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M22,"_",$N22),stats_base!$C:$C,0))</f>
+        <v>579</v>
+      </c>
+      <c r="J22">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M22,"_",$N22),stats_base!$C:$C,0))</f>
+        <v>3239</v>
+      </c>
+      <c r="K22">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M22,"_",$N22),stats_base!$C:$C,0))</f>
+        <v>1075</v>
+      </c>
+      <c r="L22">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M22,"_",$N22),stats_base!$C:$C,0))</f>
+        <v>689</v>
+      </c>
+      <c r="M22" t="s">
+        <v>928</v>
+      </c>
+      <c r="N22" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>833</v>
       </c>
@@ -12694,8 +13590,50 @@
       <c r="C23">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M23,"_",$N23),stats_base!$C:$C,0))</f>
+        <v>882</v>
+      </c>
+      <c r="E23">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M23,"_",$N23),stats_base!$C:$C,0))</f>
+        <v>511</v>
+      </c>
+      <c r="F23">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M23,"_",$N23),stats_base!$C:$C,0))</f>
+        <v>199</v>
+      </c>
+      <c r="G23">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M23,"_",$N23),stats_base!$C:$C,0))</f>
+        <v>2310</v>
+      </c>
+      <c r="H23">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M23,"_",$N23),stats_base!$C:$C,0))</f>
+        <v>1279</v>
+      </c>
+      <c r="I23">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M23,"_",$N23),stats_base!$C:$C,0))</f>
+        <v>529</v>
+      </c>
+      <c r="J23">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M23,"_",$N23),stats_base!$C:$C,0))</f>
+        <v>2785</v>
+      </c>
+      <c r="K23">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M23,"_",$N23),stats_base!$C:$C,0))</f>
+        <v>1509</v>
+      </c>
+      <c r="L23">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M23,"_",$N23),stats_base!$C:$C,0))</f>
+        <v>634</v>
+      </c>
+      <c r="M23" t="s">
+        <v>928</v>
+      </c>
+      <c r="N23" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>834</v>
       </c>
@@ -12705,8 +13643,50 @@
       <c r="C24">
         <v>26</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M24,"_",$N24),stats_base!$C:$C,0))</f>
+        <v>882</v>
+      </c>
+      <c r="E24">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M24,"_",$N24),stats_base!$C:$C,0))</f>
+        <v>511</v>
+      </c>
+      <c r="F24">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M24,"_",$N24),stats_base!$C:$C,0))</f>
+        <v>199</v>
+      </c>
+      <c r="G24">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M24,"_",$N24),stats_base!$C:$C,0))</f>
+        <v>2310</v>
+      </c>
+      <c r="H24">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M24,"_",$N24),stats_base!$C:$C,0))</f>
+        <v>1279</v>
+      </c>
+      <c r="I24">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M24,"_",$N24),stats_base!$C:$C,0))</f>
+        <v>529</v>
+      </c>
+      <c r="J24">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M24,"_",$N24),stats_base!$C:$C,0))</f>
+        <v>2785</v>
+      </c>
+      <c r="K24">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M24,"_",$N24),stats_base!$C:$C,0))</f>
+        <v>1509</v>
+      </c>
+      <c r="L24">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M24,"_",$N24),stats_base!$C:$C,0))</f>
+        <v>634</v>
+      </c>
+      <c r="M24" t="s">
+        <v>928</v>
+      </c>
+      <c r="N24" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>835</v>
       </c>
@@ -12716,8 +13696,50 @@
       <c r="C25">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M25,"_",$N25),stats_base!$C:$C,0))</f>
+        <v>1456</v>
+      </c>
+      <c r="E25">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M25,"_",$N25),stats_base!$C:$C,0))</f>
+        <v>333</v>
+      </c>
+      <c r="F25">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M25,"_",$N25),stats_base!$C:$C,0))</f>
+        <v>347</v>
+      </c>
+      <c r="G25">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M25,"_",$N25),stats_base!$C:$C,0))</f>
+        <v>3808</v>
+      </c>
+      <c r="H25">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M25,"_",$N25),stats_base!$C:$C,0))</f>
+        <v>873</v>
+      </c>
+      <c r="I25">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M25,"_",$N25),stats_base!$C:$C,0))</f>
+        <v>881</v>
+      </c>
+      <c r="J25">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M25,"_",$N25),stats_base!$C:$C,0))</f>
+        <v>4603</v>
+      </c>
+      <c r="K25">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M25,"_",$N25),stats_base!$C:$C,0))</f>
+        <v>1008</v>
+      </c>
+      <c r="L25">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M25,"_",$N25),stats_base!$C:$C,0))</f>
+        <v>1026</v>
+      </c>
+      <c r="M25" t="s">
+        <v>928</v>
+      </c>
+      <c r="N25" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>836</v>
       </c>
@@ -12727,8 +13749,41 @@
       <c r="C26">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="2">
+        <v>1249</v>
+      </c>
+      <c r="E26" s="2">
+        <v>490</v>
+      </c>
+      <c r="F26" s="2">
+        <v>293</v>
+      </c>
+      <c r="G26" s="2">
+        <v>3271</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1228</v>
+      </c>
+      <c r="I26" s="2">
+        <v>737</v>
+      </c>
+      <c r="J26" s="2">
+        <v>3926</v>
+      </c>
+      <c r="K26" s="2">
+        <v>1423</v>
+      </c>
+      <c r="L26" s="2">
+        <v>872</v>
+      </c>
+      <c r="M26" t="s">
+        <v>928</v>
+      </c>
+      <c r="N26" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>837</v>
       </c>
@@ -12738,8 +13793,41 @@
       <c r="C27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="2">
+        <v>899</v>
+      </c>
+      <c r="E27" s="2">
+        <v>534</v>
+      </c>
+      <c r="F27" s="2">
+        <v>216</v>
+      </c>
+      <c r="G27" s="2">
+        <v>2363</v>
+      </c>
+      <c r="H27" s="2">
+        <v>1338</v>
+      </c>
+      <c r="I27" s="2">
+        <v>582</v>
+      </c>
+      <c r="J27" s="2">
+        <v>2838</v>
+      </c>
+      <c r="K27" s="2">
+        <v>1568</v>
+      </c>
+      <c r="L27" s="2">
+        <v>687</v>
+      </c>
+      <c r="M27" t="s">
+        <v>928</v>
+      </c>
+      <c r="N27" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>838</v>
       </c>
@@ -12749,8 +13837,41 @@
       <c r="C28">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="2">
+        <v>917</v>
+      </c>
+      <c r="E28" s="2">
+        <v>534</v>
+      </c>
+      <c r="F28" s="2">
+        <v>216</v>
+      </c>
+      <c r="G28" s="2">
+        <v>2417</v>
+      </c>
+      <c r="H28" s="2">
+        <v>1338</v>
+      </c>
+      <c r="I28" s="2">
+        <v>582</v>
+      </c>
+      <c r="J28" s="2">
+        <v>2892</v>
+      </c>
+      <c r="K28" s="2">
+        <v>1568</v>
+      </c>
+      <c r="L28" s="2">
+        <v>687</v>
+      </c>
+      <c r="M28" t="s">
+        <v>928</v>
+      </c>
+      <c r="N28" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>839</v>
       </c>
@@ -12760,8 +13881,41 @@
       <c r="C29">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="2">
+        <v>2119</v>
+      </c>
+      <c r="E29" s="2">
+        <v>405</v>
+      </c>
+      <c r="F29" s="2">
+        <v>259</v>
+      </c>
+      <c r="G29" s="2">
+        <v>3841</v>
+      </c>
+      <c r="H29" s="2">
+        <v>1047</v>
+      </c>
+      <c r="I29" s="2">
+        <v>691</v>
+      </c>
+      <c r="J29" s="2">
+        <v>4381</v>
+      </c>
+      <c r="K29" s="2">
+        <v>1192</v>
+      </c>
+      <c r="L29" s="2">
+        <v>801</v>
+      </c>
+      <c r="M29" t="s">
+        <v>928</v>
+      </c>
+      <c r="N29" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>840</v>
       </c>
@@ -12771,8 +13925,41 @@
       <c r="C30">
         <v>20</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="2">
+        <v>1258</v>
+      </c>
+      <c r="E30" s="2">
+        <v>540</v>
+      </c>
+      <c r="F30" s="2">
+        <v>296</v>
+      </c>
+      <c r="G30" s="2">
+        <v>3298</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1380</v>
+      </c>
+      <c r="I30" s="2">
+        <v>746</v>
+      </c>
+      <c r="J30" s="2">
+        <v>3953</v>
+      </c>
+      <c r="K30" s="2">
+        <v>1575</v>
+      </c>
+      <c r="L30" s="2">
+        <v>881</v>
+      </c>
+      <c r="M30" t="s">
+        <v>928</v>
+      </c>
+      <c r="N30" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>923</v>
       </c>
@@ -12782,8 +13969,41 @@
       <c r="C31">
         <v>27</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="2">
+        <v>937</v>
+      </c>
+      <c r="E31" s="2">
+        <v>567</v>
+      </c>
+      <c r="F31" s="2">
+        <v>253</v>
+      </c>
+      <c r="G31" s="2">
+        <v>2437</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1407</v>
+      </c>
+      <c r="I31" s="2">
+        <v>685</v>
+      </c>
+      <c r="J31" s="2">
+        <v>2912</v>
+      </c>
+      <c r="K31" s="2">
+        <v>1637</v>
+      </c>
+      <c r="L31" s="2">
+        <v>790</v>
+      </c>
+      <c r="M31" t="s">
+        <v>928</v>
+      </c>
+      <c r="N31" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>841</v>
       </c>
@@ -12793,8 +14013,50 @@
       <c r="C32">
         <v>26</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M32,"_",$N32),stats_base!$C:$C,0))</f>
+        <v>882</v>
+      </c>
+      <c r="E32">
+        <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M32,"_",$N32),stats_base!$C:$C,0))</f>
+        <v>511</v>
+      </c>
+      <c r="F32">
+        <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M32,"_",$N32),stats_base!$C:$C,0))</f>
+        <v>199</v>
+      </c>
+      <c r="G32">
+        <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M32,"_",$N32),stats_base!$C:$C,0))</f>
+        <v>2310</v>
+      </c>
+      <c r="H32">
+        <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M32,"_",$N32),stats_base!$C:$C,0))</f>
+        <v>1279</v>
+      </c>
+      <c r="I32">
+        <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M32,"_",$N32),stats_base!$C:$C,0))</f>
+        <v>529</v>
+      </c>
+      <c r="J32">
+        <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M32,"_",$N32),stats_base!$C:$C,0))</f>
+        <v>2785</v>
+      </c>
+      <c r="K32">
+        <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M32,"_",$N32),stats_base!$C:$C,0))</f>
+        <v>1509</v>
+      </c>
+      <c r="L32">
+        <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M32,"_",$N32),stats_base!$C:$C,0))</f>
+        <v>634</v>
+      </c>
+      <c r="M32" t="s">
+        <v>928</v>
+      </c>
+      <c r="N32" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>842</v>
       </c>
@@ -12804,8 +14066,41 @@
       <c r="C33">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="2">
+        <v>899</v>
+      </c>
+      <c r="E33" s="2">
+        <v>552</v>
+      </c>
+      <c r="F33" s="2">
+        <v>216</v>
+      </c>
+      <c r="G33" s="2">
+        <v>2363</v>
+      </c>
+      <c r="H33" s="2">
+        <v>1392</v>
+      </c>
+      <c r="I33" s="2">
+        <v>582</v>
+      </c>
+      <c r="J33" s="2">
+        <v>2838</v>
+      </c>
+      <c r="K33" s="2">
+        <v>1622</v>
+      </c>
+      <c r="L33" s="2">
+        <v>687</v>
+      </c>
+      <c r="M33" t="s">
+        <v>928</v>
+      </c>
+      <c r="N33" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>843</v>
       </c>
@@ -12815,8 +14110,41 @@
       <c r="C34">
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="2">
+        <v>917</v>
+      </c>
+      <c r="E34" s="2">
+        <v>552</v>
+      </c>
+      <c r="F34" s="2">
+        <v>216</v>
+      </c>
+      <c r="G34" s="2">
+        <v>2417</v>
+      </c>
+      <c r="H34" s="2">
+        <v>1392</v>
+      </c>
+      <c r="I34" s="2">
+        <v>582</v>
+      </c>
+      <c r="J34" s="2">
+        <v>2892</v>
+      </c>
+      <c r="K34" s="2">
+        <v>1622</v>
+      </c>
+      <c r="L34" s="2">
+        <v>687</v>
+      </c>
+      <c r="M34" t="s">
+        <v>928</v>
+      </c>
+      <c r="N34" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>844</v>
       </c>
@@ -12826,8 +14154,41 @@
       <c r="C35">
         <v>26</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="2">
+        <v>917</v>
+      </c>
+      <c r="E35" s="2">
+        <v>552</v>
+      </c>
+      <c r="F35" s="2">
+        <v>216</v>
+      </c>
+      <c r="G35" s="2">
+        <v>2417</v>
+      </c>
+      <c r="H35" s="2">
+        <v>1392</v>
+      </c>
+      <c r="I35" s="2">
+        <v>582</v>
+      </c>
+      <c r="J35" s="2">
+        <v>2892</v>
+      </c>
+      <c r="K35" s="2">
+        <v>1622</v>
+      </c>
+      <c r="L35" s="2">
+        <v>687</v>
+      </c>
+      <c r="M35" t="s">
+        <v>928</v>
+      </c>
+      <c r="N35" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>845</v>
       </c>
@@ -12837,8 +14198,41 @@
       <c r="C36">
         <v>16</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="2">
+        <v>1258</v>
+      </c>
+      <c r="E36" s="2">
+        <v>511</v>
+      </c>
+      <c r="F36" s="2">
+        <v>296</v>
+      </c>
+      <c r="G36" s="2">
+        <v>3298</v>
+      </c>
+      <c r="H36" s="2">
+        <v>1291</v>
+      </c>
+      <c r="I36" s="2">
+        <v>746</v>
+      </c>
+      <c r="J36" s="2">
+        <v>3953</v>
+      </c>
+      <c r="K36" s="2">
+        <v>1486</v>
+      </c>
+      <c r="L36" s="2">
+        <v>881</v>
+      </c>
+      <c r="M36" t="s">
+        <v>928</v>
+      </c>
+      <c r="N36" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>846</v>
       </c>
@@ -12848,8 +14242,41 @@
       <c r="C37">
         <v>16</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="2">
+        <v>1258</v>
+      </c>
+      <c r="E37" s="2">
+        <v>511</v>
+      </c>
+      <c r="F37" s="2">
+        <v>296</v>
+      </c>
+      <c r="G37" s="2">
+        <v>3298</v>
+      </c>
+      <c r="H37" s="2">
+        <v>1291</v>
+      </c>
+      <c r="I37" s="2">
+        <v>746</v>
+      </c>
+      <c r="J37" s="2">
+        <v>3953</v>
+      </c>
+      <c r="K37" s="2">
+        <v>1486</v>
+      </c>
+      <c r="L37" s="2">
+        <v>881</v>
+      </c>
+      <c r="M37" t="s">
+        <v>928</v>
+      </c>
+      <c r="N37" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>847</v>
       </c>
@@ -12860,7 +14287,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>848</v>
       </c>
@@ -12871,7 +14298,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>849</v>
       </c>
@@ -12882,7 +14309,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>850</v>
       </c>
@@ -12893,7 +14320,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>851</v>
       </c>
@@ -12904,7 +14331,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>852</v>
       </c>
@@ -12915,7 +14342,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>853</v>
       </c>
@@ -12926,7 +14353,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>854</v>
       </c>
@@ -12937,7 +14364,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>855</v>
       </c>
@@ -12948,7 +14375,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>856</v>
       </c>
@@ -12959,7 +14386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>857</v>
       </c>
@@ -12970,7 +14397,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>858</v>
       </c>
@@ -12981,7 +14408,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>859</v>
       </c>
@@ -12992,7 +14419,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>860</v>
       </c>
@@ -13003,7 +14430,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>861</v>
       </c>
@@ -13014,7 +14441,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>862</v>
       </c>
@@ -13025,7 +14452,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>863</v>
       </c>
@@ -13036,7 +14463,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>864</v>
       </c>
@@ -13047,7 +14474,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>865</v>
       </c>
@@ -13058,7 +14485,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>866</v>
       </c>
@@ -13069,7 +14496,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>867</v>
       </c>
@@ -13080,7 +14507,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>868</v>
       </c>
@@ -13091,7 +14518,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>869</v>
       </c>
@@ -13102,7 +14529,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>870</v>
       </c>
@@ -13113,7 +14540,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>871</v>
       </c>
@@ -13124,7 +14551,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>872</v>
       </c>
@@ -13135,7 +14562,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>873</v>
       </c>
@@ -13144,6 +14571,39 @@
       </c>
       <c r="C64">
         <v>20</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1451</v>
+      </c>
+      <c r="E64" s="2">
+        <v>622</v>
+      </c>
+      <c r="F64" s="2">
+        <v>391</v>
+      </c>
+      <c r="G64" s="2">
+        <v>3617</v>
+      </c>
+      <c r="H64" s="2">
+        <v>1516</v>
+      </c>
+      <c r="I64" s="2">
+        <v>979</v>
+      </c>
+      <c r="J64" s="2">
+        <v>4272</v>
+      </c>
+      <c r="K64" s="2">
+        <v>1711</v>
+      </c>
+      <c r="L64" s="2">
+        <v>1114</v>
+      </c>
+      <c r="M64" t="s">
+        <v>927</v>
+      </c>
+      <c r="N64" t="s">
+        <v>932</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -13505,6 +14965,416 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" t="s">
+        <v>925</v>
+      </c>
+      <c r="C1" t="s">
+        <v>936</v>
+      </c>
+      <c r="D1" t="s">
+        <v>914</v>
+      </c>
+      <c r="E1" t="s">
+        <v>915</v>
+      </c>
+      <c r="F1" t="s">
+        <v>916</v>
+      </c>
+      <c r="G1" t="s">
+        <v>917</v>
+      </c>
+      <c r="H1" t="s">
+        <v>918</v>
+      </c>
+      <c r="I1" t="s">
+        <v>919</v>
+      </c>
+      <c r="J1" t="s">
+        <v>920</v>
+      </c>
+      <c r="K1" t="s">
+        <v>921</v>
+      </c>
+      <c r="L1" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>926</v>
+      </c>
+      <c r="B2" t="s">
+        <v>931</v>
+      </c>
+      <c r="C2" t="str">
+        <f>CONCATENATE(A2,"_",B2)</f>
+        <v>7_knight_earth</v>
+      </c>
+      <c r="D2">
+        <v>1743</v>
+      </c>
+      <c r="E2">
+        <v>460</v>
+      </c>
+      <c r="F2">
+        <v>475</v>
+      </c>
+      <c r="G2">
+        <v>4275</v>
+      </c>
+      <c r="H2">
+        <v>1180</v>
+      </c>
+      <c r="I2">
+        <v>1189</v>
+      </c>
+      <c r="J2">
+        <v>5070</v>
+      </c>
+      <c r="K2">
+        <v>1315</v>
+      </c>
+      <c r="L2">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>926</v>
+      </c>
+      <c r="B3" t="s">
+        <v>932</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C13" si="0">CONCATENATE(A3,"_",B3)</f>
+        <v>7_knight_dark</v>
+      </c>
+      <c r="D3">
+        <v>1486</v>
+      </c>
+      <c r="E3">
+        <v>637</v>
+      </c>
+      <c r="F3">
+        <v>415</v>
+      </c>
+      <c r="G3">
+        <v>3688</v>
+      </c>
+      <c r="H3">
+        <v>1555</v>
+      </c>
+      <c r="I3">
+        <v>1039</v>
+      </c>
+      <c r="J3">
+        <v>4343</v>
+      </c>
+      <c r="K3">
+        <v>1750</v>
+      </c>
+      <c r="L3">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>926</v>
+      </c>
+      <c r="B4" t="s">
+        <v>933</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>7_knight_fire</v>
+      </c>
+      <c r="D4">
+        <v>1086</v>
+      </c>
+      <c r="E4">
+        <v>696</v>
+      </c>
+      <c r="F4">
+        <v>328</v>
+      </c>
+      <c r="G4">
+        <v>2730</v>
+      </c>
+      <c r="H4">
+        <v>1680</v>
+      </c>
+      <c r="I4">
+        <v>874</v>
+      </c>
+      <c r="J4">
+        <v>3205</v>
+      </c>
+      <c r="K4">
+        <v>1910</v>
+      </c>
+      <c r="L4">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>926</v>
+      </c>
+      <c r="B5" t="s">
+        <v>934</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>7_knight_water</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>926</v>
+      </c>
+      <c r="B6" t="s">
+        <v>935</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>7_knight_light</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>928</v>
+      </c>
+      <c r="B7" t="s">
+        <v>931</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>regular_earth</v>
+      </c>
+      <c r="D7">
+        <v>1456</v>
+      </c>
+      <c r="E7">
+        <v>333</v>
+      </c>
+      <c r="F7">
+        <v>347</v>
+      </c>
+      <c r="G7">
+        <v>3808</v>
+      </c>
+      <c r="H7">
+        <v>873</v>
+      </c>
+      <c r="I7">
+        <v>881</v>
+      </c>
+      <c r="J7">
+        <v>4603</v>
+      </c>
+      <c r="K7">
+        <v>1008</v>
+      </c>
+      <c r="L7">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>928</v>
+      </c>
+      <c r="B8" t="s">
+        <v>932</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>regular_dark</v>
+      </c>
+      <c r="D8">
+        <v>1231</v>
+      </c>
+      <c r="E8">
+        <v>467</v>
+      </c>
+      <c r="F8">
+        <v>270</v>
+      </c>
+      <c r="G8">
+        <v>3217</v>
+      </c>
+      <c r="H8">
+        <v>1169</v>
+      </c>
+      <c r="I8">
+        <v>678</v>
+      </c>
+      <c r="J8">
+        <v>3872</v>
+      </c>
+      <c r="K8">
+        <v>1364</v>
+      </c>
+      <c r="L8">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>928</v>
+      </c>
+      <c r="B9" t="s">
+        <v>933</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>regular_fire</v>
+      </c>
+      <c r="D9">
+        <v>882</v>
+      </c>
+      <c r="E9">
+        <v>511</v>
+      </c>
+      <c r="F9">
+        <v>199</v>
+      </c>
+      <c r="G9">
+        <v>2310</v>
+      </c>
+      <c r="H9">
+        <v>1279</v>
+      </c>
+      <c r="I9">
+        <v>529</v>
+      </c>
+      <c r="J9">
+        <v>2785</v>
+      </c>
+      <c r="K9">
+        <v>1509</v>
+      </c>
+      <c r="L9">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>928</v>
+      </c>
+      <c r="B10" t="s">
+        <v>934</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>regular_water</v>
+      </c>
+      <c r="D10">
+        <v>882</v>
+      </c>
+      <c r="E10">
+        <v>511</v>
+      </c>
+      <c r="F10">
+        <v>199</v>
+      </c>
+      <c r="G10">
+        <v>2310</v>
+      </c>
+      <c r="H10">
+        <v>1279</v>
+      </c>
+      <c r="I10">
+        <v>529</v>
+      </c>
+      <c r="J10">
+        <v>2785</v>
+      </c>
+      <c r="K10">
+        <v>1509</v>
+      </c>
+      <c r="L10">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>928</v>
+      </c>
+      <c r="B11" t="s">
+        <v>935</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>regular_light</v>
+      </c>
+      <c r="D11">
+        <v>1049</v>
+      </c>
+      <c r="E11">
+        <v>360</v>
+      </c>
+      <c r="F11">
+        <v>219</v>
+      </c>
+      <c r="G11">
+        <v>2699</v>
+      </c>
+      <c r="H11">
+        <v>930</v>
+      </c>
+      <c r="I11">
+        <v>579</v>
+      </c>
+      <c r="J11">
+        <v>3239</v>
+      </c>
+      <c r="K11">
+        <v>1075</v>
+      </c>
+      <c r="L11">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>929</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>asgar_</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>930</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>aisha_</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B146"/>
   <sheetViews>
@@ -14700,7 +16570,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added element images. Clarified stack table allies/opponents division.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -3176,8 +3176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D89" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J99" sqref="J99"/>
+    <sheetView tabSelected="1" topLeftCell="B23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Recommended equips and tier list added to seed file.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13014" windowHeight="10610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11479" windowHeight="10610" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="skills" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">attributes!$A$1:$B$137</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">skills!$A$1:$AE$246</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">stats!$A$1:$Z$96</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2927" uniqueCount="937">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3427" uniqueCount="986">
   <si>
     <t>attributes</t>
   </si>
@@ -2843,6 +2844,153 @@
   </si>
   <si>
     <t>skull_3_1</t>
+  </si>
+  <si>
+    <t>rec_weapon</t>
+  </si>
+  <si>
+    <t>rec_armor</t>
+  </si>
+  <si>
+    <t>t_adv</t>
+  </si>
+  <si>
+    <t>t_ecr</t>
+  </si>
+  <si>
+    <t>t_ncr</t>
+  </si>
+  <si>
+    <t>t_pvp</t>
+  </si>
+  <si>
+    <t>t_tower</t>
+  </si>
+  <si>
+    <t>t_raid</t>
+  </si>
+  <si>
+    <t>S-</t>
+  </si>
+  <si>
+    <t>S (Mon)</t>
+  </si>
+  <si>
+    <t>S+ (Mon)</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>S+</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>t_boss</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>S+ (Sun)</t>
+  </si>
+  <si>
+    <t>A-</t>
+  </si>
+  <si>
+    <t>B-</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>S+ (Tue)</t>
+  </si>
+  <si>
+    <t>S+ (Thu)</t>
+  </si>
+  <si>
+    <t>S (Sun)</t>
+  </si>
+  <si>
+    <t>S- (Sat)</t>
+  </si>
+  <si>
+    <t>Double speed</t>
+  </si>
+  <si>
+    <t>Double HP</t>
+  </si>
+  <si>
+    <t>rej_jewel_0</t>
+  </si>
+  <si>
+    <t>rej_jewel_1</t>
+  </si>
+  <si>
+    <t>rej_jewel_2</t>
+  </si>
+  <si>
+    <t>Critical Rate</t>
+  </si>
+  <si>
+    <t>Damage Output</t>
+  </si>
+  <si>
+    <t>Critical Damage</t>
+  </si>
+  <si>
+    <t>Block Rate</t>
+  </si>
+  <si>
+    <t>Lethal Rate</t>
+  </si>
+  <si>
+    <t>Counter Rate</t>
+  </si>
+  <si>
+    <t>Double speed / Double critical</t>
+  </si>
+  <si>
+    <t>Double lethal</t>
+  </si>
+  <si>
+    <t>Double HP / HP+block</t>
+  </si>
+  <si>
+    <t>Double counter</t>
+  </si>
+  <si>
+    <t>Double counter / Double HP</t>
+  </si>
+  <si>
+    <t>Double critical</t>
+  </si>
+  <si>
+    <t>Double speed / Speed+lethal</t>
+  </si>
+  <si>
+    <t>Double counter / HP+counter</t>
+  </si>
+  <si>
+    <t>HP+block</t>
+  </si>
+  <si>
+    <t>HP+block / HP+counter</t>
+  </si>
+  <si>
+    <t>Double lethal / Speed+lethal</t>
   </si>
 </sst>
 </file>
@@ -3176,8 +3324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M42" sqref="M42"/>
+    <sheetView topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -12438,19 +12586,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N96"/>
+  <dimension ref="A1:Z96"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92:N92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="14" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="0" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="26" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>906</v>
       </c>
@@ -12493,8 +12650,44 @@
       <c r="N1" t="s">
         <v>922</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>937</v>
+      </c>
+      <c r="P1" t="s">
+        <v>938</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>966</v>
+      </c>
+      <c r="R1" t="s">
+        <v>967</v>
+      </c>
+      <c r="S1" t="s">
+        <v>968</v>
+      </c>
+      <c r="T1" t="s">
+        <v>939</v>
+      </c>
+      <c r="U1" t="s">
+        <v>940</v>
+      </c>
+      <c r="V1" t="s">
+        <v>941</v>
+      </c>
+      <c r="W1" t="s">
+        <v>942</v>
+      </c>
+      <c r="X1" t="s">
+        <v>943</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>944</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>810</v>
       </c>
@@ -12546,8 +12739,44 @@
       <c r="N2" t="s">
         <v>928</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>964</v>
+      </c>
+      <c r="P2" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>974</v>
+      </c>
+      <c r="R2" t="s">
+        <v>969</v>
+      </c>
+      <c r="S2" t="s">
+        <v>970</v>
+      </c>
+      <c r="T2" t="s">
+        <v>945</v>
+      </c>
+      <c r="U2" t="s">
+        <v>946</v>
+      </c>
+      <c r="V2" t="s">
+        <v>947</v>
+      </c>
+      <c r="W2" t="s">
+        <v>948</v>
+      </c>
+      <c r="X2" t="s">
+        <v>948</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>949</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>811</v>
       </c>
@@ -12599,8 +12828,44 @@
       <c r="N3" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>964</v>
+      </c>
+      <c r="P3" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>971</v>
+      </c>
+      <c r="R3" t="s">
+        <v>972</v>
+      </c>
+      <c r="S3" t="s">
+        <v>973</v>
+      </c>
+      <c r="T3" t="s">
+        <v>950</v>
+      </c>
+      <c r="U3" t="s">
+        <v>950</v>
+      </c>
+      <c r="V3" t="s">
+        <v>949</v>
+      </c>
+      <c r="W3" t="s">
+        <v>950</v>
+      </c>
+      <c r="X3" t="s">
+        <v>951</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>951</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>812</v>
       </c>
@@ -12652,8 +12917,44 @@
       <c r="N4" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>964</v>
+      </c>
+      <c r="P4" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>971</v>
+      </c>
+      <c r="R4" t="s">
+        <v>972</v>
+      </c>
+      <c r="S4" t="s">
+        <v>973</v>
+      </c>
+      <c r="T4" t="s">
+        <v>951</v>
+      </c>
+      <c r="U4" t="s">
+        <v>948</v>
+      </c>
+      <c r="V4" t="s">
+        <v>948</v>
+      </c>
+      <c r="W4" t="s">
+        <v>949</v>
+      </c>
+      <c r="X4" t="s">
+        <v>948</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>954</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>813</v>
       </c>
@@ -12705,8 +13006,44 @@
       <c r="N5" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" t="s">
+        <v>964</v>
+      </c>
+      <c r="P5" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>971</v>
+      </c>
+      <c r="R5" t="s">
+        <v>974</v>
+      </c>
+      <c r="S5" t="s">
+        <v>973</v>
+      </c>
+      <c r="T5" t="s">
+        <v>950</v>
+      </c>
+      <c r="U5" t="s">
+        <v>948</v>
+      </c>
+      <c r="V5" t="s">
+        <v>948</v>
+      </c>
+      <c r="W5" t="s">
+        <v>950</v>
+      </c>
+      <c r="X5" t="s">
+        <v>950</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>948</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>814</v>
       </c>
@@ -12758,8 +13095,44 @@
       <c r="N6" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" t="s">
+        <v>964</v>
+      </c>
+      <c r="P6" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>971</v>
+      </c>
+      <c r="R6" t="s">
+        <v>969</v>
+      </c>
+      <c r="S6" t="s">
+        <v>973</v>
+      </c>
+      <c r="T6" t="s">
+        <v>948</v>
+      </c>
+      <c r="U6" t="s">
+        <v>953</v>
+      </c>
+      <c r="V6" t="s">
+        <v>953</v>
+      </c>
+      <c r="W6" t="s">
+        <v>948</v>
+      </c>
+      <c r="X6" t="s">
+        <v>951</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>953</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>815</v>
       </c>
@@ -12811,8 +13184,44 @@
       <c r="N7" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>964</v>
+      </c>
+      <c r="P7" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>971</v>
+      </c>
+      <c r="R7" t="s">
+        <v>972</v>
+      </c>
+      <c r="S7" t="s">
+        <v>973</v>
+      </c>
+      <c r="T7" t="s">
+        <v>950</v>
+      </c>
+      <c r="U7" t="s">
+        <v>950</v>
+      </c>
+      <c r="V7" t="s">
+        <v>950</v>
+      </c>
+      <c r="W7" t="s">
+        <v>950</v>
+      </c>
+      <c r="X7" t="s">
+        <v>951</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>949</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>816</v>
       </c>
@@ -12864,8 +13273,44 @@
       <c r="N8" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8" t="s">
+        <v>964</v>
+      </c>
+      <c r="P8" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>971</v>
+      </c>
+      <c r="R8" t="s">
+        <v>974</v>
+      </c>
+      <c r="S8" t="s">
+        <v>973</v>
+      </c>
+      <c r="T8" t="s">
+        <v>950</v>
+      </c>
+      <c r="U8" t="s">
+        <v>953</v>
+      </c>
+      <c r="V8" t="s">
+        <v>953</v>
+      </c>
+      <c r="W8" t="s">
+        <v>948</v>
+      </c>
+      <c r="X8" t="s">
+        <v>950</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>954</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>817</v>
       </c>
@@ -12908,8 +13353,44 @@
       <c r="N9" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" t="s">
+        <v>964</v>
+      </c>
+      <c r="P9" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>971</v>
+      </c>
+      <c r="R9" t="s">
+        <v>972</v>
+      </c>
+      <c r="S9" t="s">
+        <v>973</v>
+      </c>
+      <c r="T9" t="s">
+        <v>948</v>
+      </c>
+      <c r="U9" t="s">
+        <v>950</v>
+      </c>
+      <c r="V9" t="s">
+        <v>948</v>
+      </c>
+      <c r="W9" t="s">
+        <v>948</v>
+      </c>
+      <c r="X9" t="s">
+        <v>951</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>953</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>818</v>
       </c>
@@ -12961,8 +13442,38 @@
       <c r="N10" t="s">
         <v>928</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" t="s">
+        <v>964</v>
+      </c>
+      <c r="P10" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>969</v>
+      </c>
+      <c r="R10" t="s">
+        <v>974</v>
+      </c>
+      <c r="S10" t="s">
+        <v>973</v>
+      </c>
+      <c r="T10" t="s">
+        <v>955</v>
+      </c>
+      <c r="U10" t="s">
+        <v>955</v>
+      </c>
+      <c r="W10" t="s">
+        <v>949</v>
+      </c>
+      <c r="X10" t="s">
+        <v>955</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>819</v>
       </c>
@@ -13005,8 +13516,38 @@
       <c r="N11" t="s">
         <v>932</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11" t="s">
+        <v>964</v>
+      </c>
+      <c r="P11" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>972</v>
+      </c>
+      <c r="R11" t="s">
+        <v>974</v>
+      </c>
+      <c r="S11" t="s">
+        <v>973</v>
+      </c>
+      <c r="T11" t="s">
+        <v>955</v>
+      </c>
+      <c r="U11" t="s">
+        <v>956</v>
+      </c>
+      <c r="W11" t="s">
+        <v>957</v>
+      </c>
+      <c r="X11" t="s">
+        <v>957</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>820</v>
       </c>
@@ -13058,8 +13599,38 @@
       <c r="N12" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12" t="s">
+        <v>964</v>
+      </c>
+      <c r="P12" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>972</v>
+      </c>
+      <c r="R12" t="s">
+        <v>974</v>
+      </c>
+      <c r="S12" t="s">
+        <v>973</v>
+      </c>
+      <c r="T12" t="s">
+        <v>951</v>
+      </c>
+      <c r="U12" t="s">
+        <v>955</v>
+      </c>
+      <c r="W12" t="s">
+        <v>945</v>
+      </c>
+      <c r="X12" t="s">
+        <v>949</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>821</v>
       </c>
@@ -13111,8 +13682,38 @@
       <c r="N13" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13" t="s">
+        <v>964</v>
+      </c>
+      <c r="P13" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>969</v>
+      </c>
+      <c r="R13" t="s">
+        <v>970</v>
+      </c>
+      <c r="S13" t="s">
+        <v>973</v>
+      </c>
+      <c r="T13" t="s">
+        <v>954</v>
+      </c>
+      <c r="U13" t="s">
+        <v>958</v>
+      </c>
+      <c r="W13" t="s">
+        <v>955</v>
+      </c>
+      <c r="X13" t="s">
+        <v>953</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>822</v>
       </c>
@@ -13155,8 +13756,38 @@
       <c r="N14" t="s">
         <v>932</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" t="s">
+        <v>976</v>
+      </c>
+      <c r="P14" t="s">
+        <v>977</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>972</v>
+      </c>
+      <c r="R14" t="s">
+        <v>974</v>
+      </c>
+      <c r="S14" t="s">
+        <v>973</v>
+      </c>
+      <c r="T14" t="s">
+        <v>959</v>
+      </c>
+      <c r="U14" t="s">
+        <v>961</v>
+      </c>
+      <c r="W14" t="s">
+        <v>953</v>
+      </c>
+      <c r="X14" t="s">
+        <v>958</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>823</v>
       </c>
@@ -13208,8 +13839,38 @@
       <c r="N15" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" t="s">
+        <v>964</v>
+      </c>
+      <c r="P15" t="s">
+        <v>978</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>969</v>
+      </c>
+      <c r="R15" t="s">
+        <v>970</v>
+      </c>
+      <c r="S15" t="s">
+        <v>973</v>
+      </c>
+      <c r="T15" t="s">
+        <v>949</v>
+      </c>
+      <c r="U15" t="s">
+        <v>948</v>
+      </c>
+      <c r="W15" t="s">
+        <v>955</v>
+      </c>
+      <c r="X15" t="s">
+        <v>949</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>824</v>
       </c>
@@ -13252,8 +13913,38 @@
       <c r="N16" t="s">
         <v>928</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" t="s">
+        <v>964</v>
+      </c>
+      <c r="P16" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>971</v>
+      </c>
+      <c r="R16" t="s">
+        <v>969</v>
+      </c>
+      <c r="S16" t="s">
+        <v>974</v>
+      </c>
+      <c r="T16" t="s">
+        <v>955</v>
+      </c>
+      <c r="U16" t="s">
+        <v>956</v>
+      </c>
+      <c r="W16" t="s">
+        <v>957</v>
+      </c>
+      <c r="X16" t="s">
+        <v>957</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>825</v>
       </c>
@@ -13305,8 +13996,38 @@
       <c r="N17" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>964</v>
+      </c>
+      <c r="P17" t="s">
+        <v>978</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>971</v>
+      </c>
+      <c r="R17" t="s">
+        <v>969</v>
+      </c>
+      <c r="S17" t="s">
+        <v>974</v>
+      </c>
+      <c r="T17" t="s">
+        <v>959</v>
+      </c>
+      <c r="U17" t="s">
+        <v>955</v>
+      </c>
+      <c r="W17" t="s">
+        <v>945</v>
+      </c>
+      <c r="X17" t="s">
+        <v>954</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>826</v>
       </c>
@@ -13358,8 +14079,38 @@
       <c r="N18" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" t="s">
+        <v>964</v>
+      </c>
+      <c r="P18" t="s">
+        <v>978</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>971</v>
+      </c>
+      <c r="R18" t="s">
+        <v>969</v>
+      </c>
+      <c r="S18" t="s">
+        <v>974</v>
+      </c>
+      <c r="T18" t="s">
+        <v>954</v>
+      </c>
+      <c r="U18" t="s">
+        <v>953</v>
+      </c>
+      <c r="W18" t="s">
+        <v>959</v>
+      </c>
+      <c r="X18" t="s">
+        <v>954</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>827</v>
       </c>
@@ -13411,8 +14162,38 @@
       <c r="N19" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" t="s">
+        <v>964</v>
+      </c>
+      <c r="P19" t="s">
+        <v>978</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>971</v>
+      </c>
+      <c r="R19" t="s">
+        <v>969</v>
+      </c>
+      <c r="S19" t="s">
+        <v>974</v>
+      </c>
+      <c r="T19" t="s">
+        <v>950</v>
+      </c>
+      <c r="U19" t="s">
+        <v>955</v>
+      </c>
+      <c r="W19" t="s">
+        <v>949</v>
+      </c>
+      <c r="X19" t="s">
+        <v>955</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>828</v>
       </c>
@@ -13464,8 +14245,38 @@
       <c r="N20" t="s">
         <v>932</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20" t="s">
+        <v>976</v>
+      </c>
+      <c r="P20" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>972</v>
+      </c>
+      <c r="R20" t="s">
+        <v>974</v>
+      </c>
+      <c r="S20" t="s">
+        <v>973</v>
+      </c>
+      <c r="T20" t="s">
+        <v>958</v>
+      </c>
+      <c r="U20" t="s">
+        <v>948</v>
+      </c>
+      <c r="W20" t="s">
+        <v>953</v>
+      </c>
+      <c r="X20" t="s">
+        <v>957</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>829</v>
       </c>
@@ -13517,8 +14328,38 @@
       <c r="N21" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21" t="s">
+        <v>964</v>
+      </c>
+      <c r="P21" t="s">
+        <v>977</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>972</v>
+      </c>
+      <c r="R21" t="s">
+        <v>974</v>
+      </c>
+      <c r="S21" t="s">
+        <v>973</v>
+      </c>
+      <c r="T21" t="s">
+        <v>959</v>
+      </c>
+      <c r="U21" t="s">
+        <v>960</v>
+      </c>
+      <c r="W21" t="s">
+        <v>953</v>
+      </c>
+      <c r="X21" t="s">
+        <v>954</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>830</v>
       </c>
@@ -13570,8 +14411,38 @@
       <c r="N22" t="s">
         <v>932</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22" t="s">
+        <v>964</v>
+      </c>
+      <c r="P22" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>972</v>
+      </c>
+      <c r="R22" t="s">
+        <v>974</v>
+      </c>
+      <c r="S22" t="s">
+        <v>973</v>
+      </c>
+      <c r="T22" t="s">
+        <v>958</v>
+      </c>
+      <c r="U22" t="s">
+        <v>957</v>
+      </c>
+      <c r="W22" t="s">
+        <v>945</v>
+      </c>
+      <c r="X22" t="s">
+        <v>945</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>831</v>
       </c>
@@ -13623,8 +14494,38 @@
       <c r="N23" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23" t="s">
+        <v>964</v>
+      </c>
+      <c r="P23" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>972</v>
+      </c>
+      <c r="R23" t="s">
+        <v>969</v>
+      </c>
+      <c r="S23" t="s">
+        <v>971</v>
+      </c>
+      <c r="T23" t="s">
+        <v>948</v>
+      </c>
+      <c r="U23" t="s">
+        <v>953</v>
+      </c>
+      <c r="W23" t="s">
+        <v>954</v>
+      </c>
+      <c r="X23" t="s">
+        <v>953</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>832</v>
       </c>
@@ -13676,8 +14577,38 @@
       <c r="N24" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24" t="s">
+        <v>964</v>
+      </c>
+      <c r="P24" t="s">
+        <v>978</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>974</v>
+      </c>
+      <c r="R24" t="s">
+        <v>969</v>
+      </c>
+      <c r="S24" t="s">
+        <v>971</v>
+      </c>
+      <c r="T24" t="s">
+        <v>949</v>
+      </c>
+      <c r="U24" t="s">
+        <v>951</v>
+      </c>
+      <c r="W24" t="s">
+        <v>954</v>
+      </c>
+      <c r="X24" t="s">
+        <v>949</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>833</v>
       </c>
@@ -13729,8 +14660,38 @@
       <c r="N25" t="s">
         <v>928</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25" t="s">
+        <v>964</v>
+      </c>
+      <c r="P25" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>972</v>
+      </c>
+      <c r="R25" t="s">
+        <v>974</v>
+      </c>
+      <c r="S25" t="s">
+        <v>973</v>
+      </c>
+      <c r="T25" t="s">
+        <v>958</v>
+      </c>
+      <c r="U25" t="s">
+        <v>954</v>
+      </c>
+      <c r="W25" t="s">
+        <v>953</v>
+      </c>
+      <c r="X25" t="s">
+        <v>953</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>834</v>
       </c>
@@ -13773,8 +14734,38 @@
       <c r="N26" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26" t="s">
+        <v>964</v>
+      </c>
+      <c r="P26" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>972</v>
+      </c>
+      <c r="R26" t="s">
+        <v>974</v>
+      </c>
+      <c r="S26" t="s">
+        <v>969</v>
+      </c>
+      <c r="T26" t="s">
+        <v>954</v>
+      </c>
+      <c r="U26" t="s">
+        <v>949</v>
+      </c>
+      <c r="W26" t="s">
+        <v>953</v>
+      </c>
+      <c r="X26" t="s">
+        <v>953</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>835</v>
       </c>
@@ -13817,8 +14808,38 @@
       <c r="N27" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27" t="s">
+        <v>976</v>
+      </c>
+      <c r="P27" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>972</v>
+      </c>
+      <c r="R27" t="s">
+        <v>974</v>
+      </c>
+      <c r="S27" t="s">
+        <v>973</v>
+      </c>
+      <c r="T27" t="s">
+        <v>954</v>
+      </c>
+      <c r="U27" t="s">
+        <v>947</v>
+      </c>
+      <c r="W27" t="s">
+        <v>953</v>
+      </c>
+      <c r="X27" t="s">
+        <v>958</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>836</v>
       </c>
@@ -13861,8 +14882,38 @@
       <c r="N28" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28" t="s">
+        <v>964</v>
+      </c>
+      <c r="P28" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>972</v>
+      </c>
+      <c r="R28" t="s">
+        <v>974</v>
+      </c>
+      <c r="S28" t="s">
+        <v>973</v>
+      </c>
+      <c r="T28" t="s">
+        <v>950</v>
+      </c>
+      <c r="U28" t="s">
+        <v>951</v>
+      </c>
+      <c r="W28" t="s">
+        <v>951</v>
+      </c>
+      <c r="X28" t="s">
+        <v>951</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>837</v>
       </c>
@@ -13905,8 +14956,38 @@
       <c r="N29" t="s">
         <v>932</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29" t="s">
+        <v>964</v>
+      </c>
+      <c r="P29" t="s">
+        <v>977</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>972</v>
+      </c>
+      <c r="R29" t="s">
+        <v>974</v>
+      </c>
+      <c r="S29" t="s">
+        <v>973</v>
+      </c>
+      <c r="T29" t="s">
+        <v>951</v>
+      </c>
+      <c r="U29" t="s">
+        <v>957</v>
+      </c>
+      <c r="W29" t="s">
+        <v>951</v>
+      </c>
+      <c r="X29" t="s">
+        <v>951</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>838</v>
       </c>
@@ -13949,8 +15030,38 @@
       <c r="N30" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30" t="s">
+        <v>964</v>
+      </c>
+      <c r="P30" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>969</v>
+      </c>
+      <c r="R30" t="s">
+        <v>970</v>
+      </c>
+      <c r="S30" t="s">
+        <v>971</v>
+      </c>
+      <c r="T30" t="s">
+        <v>945</v>
+      </c>
+      <c r="U30" t="s">
+        <v>959</v>
+      </c>
+      <c r="W30" t="s">
+        <v>959</v>
+      </c>
+      <c r="X30" t="s">
+        <v>955</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>920</v>
       </c>
@@ -13993,8 +15104,38 @@
       <c r="N31" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31" t="s">
+        <v>964</v>
+      </c>
+      <c r="P31" t="s">
+        <v>978</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>974</v>
+      </c>
+      <c r="R31" t="s">
+        <v>969</v>
+      </c>
+      <c r="S31" t="s">
+        <v>971</v>
+      </c>
+      <c r="T31" t="s">
+        <v>951</v>
+      </c>
+      <c r="U31" t="s">
+        <v>953</v>
+      </c>
+      <c r="W31" t="s">
+        <v>951</v>
+      </c>
+      <c r="X31" t="s">
+        <v>953</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>839</v>
       </c>
@@ -14046,8 +15187,23 @@
       <c r="N32" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T32" t="s">
+        <v>954</v>
+      </c>
+      <c r="U32" t="s">
+        <v>949</v>
+      </c>
+      <c r="W32" t="s">
+        <v>958</v>
+      </c>
+      <c r="X32" t="s">
+        <v>957</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>840</v>
       </c>
@@ -14090,8 +15246,38 @@
       <c r="N33" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33" t="s">
+        <v>964</v>
+      </c>
+      <c r="P33" t="s">
+        <v>979</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>974</v>
+      </c>
+      <c r="R33" t="s">
+        <v>970</v>
+      </c>
+      <c r="S33" t="s">
+        <v>971</v>
+      </c>
+      <c r="T33" t="s">
+        <v>950</v>
+      </c>
+      <c r="U33" t="s">
+        <v>955</v>
+      </c>
+      <c r="W33" t="s">
+        <v>948</v>
+      </c>
+      <c r="X33" t="s">
+        <v>945</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>841</v>
       </c>
@@ -14134,8 +15320,38 @@
       <c r="N34" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34" t="s">
+        <v>980</v>
+      </c>
+      <c r="P34" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>969</v>
+      </c>
+      <c r="R34" t="s">
+        <v>970</v>
+      </c>
+      <c r="S34" t="s">
+        <v>971</v>
+      </c>
+      <c r="T34" t="s">
+        <v>958</v>
+      </c>
+      <c r="U34" t="s">
+        <v>953</v>
+      </c>
+      <c r="W34" t="s">
+        <v>951</v>
+      </c>
+      <c r="X34" t="s">
+        <v>945</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>842</v>
       </c>
@@ -14178,8 +15394,38 @@
       <c r="N35" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O35" t="s">
+        <v>976</v>
+      </c>
+      <c r="P35" t="s">
+        <v>978</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>971</v>
+      </c>
+      <c r="R35" t="s">
+        <v>970</v>
+      </c>
+      <c r="S35" t="s">
+        <v>973</v>
+      </c>
+      <c r="T35" t="s">
+        <v>949</v>
+      </c>
+      <c r="U35" t="s">
+        <v>948</v>
+      </c>
+      <c r="W35" t="s">
+        <v>955</v>
+      </c>
+      <c r="X35" t="s">
+        <v>950</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>843</v>
       </c>
@@ -14222,8 +15468,38 @@
       <c r="N36" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36" t="s">
+        <v>981</v>
+      </c>
+      <c r="P36" t="s">
+        <v>982</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>971</v>
+      </c>
+      <c r="R36" t="s">
+        <v>970</v>
+      </c>
+      <c r="S36" t="s">
+        <v>973</v>
+      </c>
+      <c r="T36" t="s">
+        <v>958</v>
+      </c>
+      <c r="U36" t="s">
+        <v>950</v>
+      </c>
+      <c r="W36" t="s">
+        <v>958</v>
+      </c>
+      <c r="X36" t="s">
+        <v>945</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>844</v>
       </c>
@@ -14266,8 +15542,38 @@
       <c r="N37" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37" t="s">
+        <v>964</v>
+      </c>
+      <c r="P37" t="s">
+        <v>978</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>969</v>
+      </c>
+      <c r="R37" t="s">
+        <v>970</v>
+      </c>
+      <c r="S37" t="s">
+        <v>974</v>
+      </c>
+      <c r="T37" t="s">
+        <v>948</v>
+      </c>
+      <c r="U37" t="s">
+        <v>955</v>
+      </c>
+      <c r="W37" t="s">
+        <v>948</v>
+      </c>
+      <c r="X37" t="s">
+        <v>945</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>845</v>
       </c>
@@ -14311,7 +15617,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>846</v>
       </c>
@@ -14355,7 +15661,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>847</v>
       </c>
@@ -14398,8 +15704,38 @@
       <c r="N40" t="s">
         <v>928</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40" t="s">
+        <v>964</v>
+      </c>
+      <c r="P40" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>969</v>
+      </c>
+      <c r="R40" t="s">
+        <v>970</v>
+      </c>
+      <c r="S40" t="s">
+        <v>974</v>
+      </c>
+      <c r="T40" t="s">
+        <v>959</v>
+      </c>
+      <c r="U40" t="s">
+        <v>955</v>
+      </c>
+      <c r="W40" t="s">
+        <v>955</v>
+      </c>
+      <c r="X40" t="s">
+        <v>955</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>848</v>
       </c>
@@ -14442,8 +15778,38 @@
       <c r="N41" t="s">
         <v>932</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41" t="s">
+        <v>985</v>
+      </c>
+      <c r="P41" t="s">
+        <v>977</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>974</v>
+      </c>
+      <c r="R41" t="s">
+        <v>972</v>
+      </c>
+      <c r="S41" t="s">
+        <v>973</v>
+      </c>
+      <c r="T41" t="s">
+        <v>948</v>
+      </c>
+      <c r="U41" t="s">
+        <v>948</v>
+      </c>
+      <c r="W41" t="s">
+        <v>955</v>
+      </c>
+      <c r="X41" t="s">
+        <v>948</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>849</v>
       </c>
@@ -14486,8 +15852,38 @@
       <c r="N42" t="s">
         <v>931</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42" t="s">
+        <v>980</v>
+      </c>
+      <c r="P42" t="s">
+        <v>983</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>969</v>
+      </c>
+      <c r="R42" t="s">
+        <v>972</v>
+      </c>
+      <c r="S42" t="s">
+        <v>970</v>
+      </c>
+      <c r="T42" t="s">
+        <v>954</v>
+      </c>
+      <c r="U42" t="s">
+        <v>958</v>
+      </c>
+      <c r="W42" t="s">
+        <v>958</v>
+      </c>
+      <c r="X42" t="s">
+        <v>954</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>850</v>
       </c>
@@ -14530,8 +15926,38 @@
       <c r="N43" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43" t="s">
+        <v>980</v>
+      </c>
+      <c r="P43" t="s">
+        <v>983</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>969</v>
+      </c>
+      <c r="R43" t="s">
+        <v>972</v>
+      </c>
+      <c r="S43" t="s">
+        <v>970</v>
+      </c>
+      <c r="T43" t="s">
+        <v>948</v>
+      </c>
+      <c r="U43" t="s">
+        <v>953</v>
+      </c>
+      <c r="W43" t="s">
+        <v>959</v>
+      </c>
+      <c r="X43" t="s">
+        <v>953</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>851</v>
       </c>
@@ -14575,7 +16001,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>852</v>
       </c>
@@ -14619,7 +16045,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>853</v>
       </c>
@@ -14663,7 +16089,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>854</v>
       </c>
@@ -14707,7 +16133,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>855</v>
       </c>
@@ -14751,7 +16177,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>856</v>
       </c>
@@ -14795,7 +16221,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>857</v>
       </c>
@@ -14839,7 +16265,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>858</v>
       </c>
@@ -14883,7 +16309,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>859</v>
       </c>
@@ -14927,7 +16353,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>860</v>
       </c>
@@ -14971,7 +16397,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>861</v>
       </c>
@@ -15015,7 +16441,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>862</v>
       </c>
@@ -15059,7 +16485,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>863</v>
       </c>
@@ -15103,7 +16529,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>864</v>
       </c>
@@ -15147,7 +16573,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>865</v>
       </c>
@@ -15191,7 +16617,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>866</v>
       </c>
@@ -15235,7 +16661,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>867</v>
       </c>
@@ -15279,7 +16705,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>868</v>
       </c>
@@ -15323,7 +16749,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>869</v>
       </c>
@@ -15367,7 +16793,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>870</v>
       </c>
@@ -15410,8 +16836,23 @@
       <c r="N63" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T63" t="s">
+        <v>954</v>
+      </c>
+      <c r="U63" t="s">
+        <v>962</v>
+      </c>
+      <c r="W63" t="s">
+        <v>953</v>
+      </c>
+      <c r="X63" t="s">
+        <v>954</v>
+      </c>
+      <c r="Y63" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>871</v>
       </c>
@@ -15454,8 +16895,44 @@
       <c r="N64" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O64" t="s">
+        <v>975</v>
+      </c>
+      <c r="P64" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>971</v>
+      </c>
+      <c r="R64" t="s">
+        <v>969</v>
+      </c>
+      <c r="S64" t="s">
+        <v>970</v>
+      </c>
+      <c r="T64" t="s">
+        <v>950</v>
+      </c>
+      <c r="U64" t="s">
+        <v>955</v>
+      </c>
+      <c r="V64" t="s">
+        <v>953</v>
+      </c>
+      <c r="W64" t="s">
+        <v>948</v>
+      </c>
+      <c r="X64" t="s">
+        <v>955</v>
+      </c>
+      <c r="Y64" t="s">
+        <v>953</v>
+      </c>
+      <c r="Z64" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>872</v>
       </c>
@@ -15499,7 +16976,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>934</v>
       </c>
@@ -15543,7 +17020,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>873</v>
       </c>
@@ -15587,7 +17064,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>874</v>
       </c>
@@ -15631,7 +17108,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>875</v>
       </c>
@@ -15675,7 +17152,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>876</v>
       </c>
@@ -15719,7 +17196,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>877</v>
       </c>
@@ -15762,8 +17239,23 @@
       <c r="N71" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T71" t="s">
+        <v>959</v>
+      </c>
+      <c r="U71" t="s">
+        <v>953</v>
+      </c>
+      <c r="W71" t="s">
+        <v>954</v>
+      </c>
+      <c r="X71" t="s">
+        <v>953</v>
+      </c>
+      <c r="Y71" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>878</v>
       </c>
@@ -15807,7 +17299,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>879</v>
       </c>
@@ -15851,7 +17343,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>880</v>
       </c>
@@ -15895,7 +17387,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>881</v>
       </c>
@@ -15939,7 +17431,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>882</v>
       </c>
@@ -15983,7 +17475,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>883</v>
       </c>
@@ -16027,7 +17519,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>884</v>
       </c>
@@ -16070,8 +17562,23 @@
       <c r="N78" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T78" t="s">
+        <v>954</v>
+      </c>
+      <c r="U78" t="s">
+        <v>953</v>
+      </c>
+      <c r="W78" t="s">
+        <v>957</v>
+      </c>
+      <c r="X78" t="s">
+        <v>953</v>
+      </c>
+      <c r="Y78" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>885</v>
       </c>
@@ -16115,7 +17622,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>886</v>
       </c>
@@ -16159,7 +17666,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>887</v>
       </c>
@@ -16203,7 +17710,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>888</v>
       </c>
@@ -16247,7 +17754,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>889</v>
       </c>
@@ -16291,7 +17798,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>890</v>
       </c>
@@ -16335,7 +17842,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>891</v>
       </c>
@@ -16378,8 +17885,38 @@
       <c r="N85" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O85" t="s">
+        <v>980</v>
+      </c>
+      <c r="P85" t="s">
+        <v>983</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>974</v>
+      </c>
+      <c r="R85" t="s">
+        <v>972</v>
+      </c>
+      <c r="S85" t="s">
+        <v>973</v>
+      </c>
+      <c r="T85" t="s">
+        <v>958</v>
+      </c>
+      <c r="U85" t="s">
+        <v>963</v>
+      </c>
+      <c r="W85" t="s">
+        <v>957</v>
+      </c>
+      <c r="X85" t="s">
+        <v>953</v>
+      </c>
+      <c r="Y85" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>892</v>
       </c>
@@ -16423,7 +17960,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>893</v>
       </c>
@@ -16467,7 +18004,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>894</v>
       </c>
@@ -16511,7 +18048,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>895</v>
       </c>
@@ -16555,7 +18092,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>896</v>
       </c>
@@ -16599,7 +18136,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>897</v>
       </c>
@@ -16642,8 +18179,38 @@
       <c r="N91" t="s">
         <v>932</v>
       </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O91" t="s">
+        <v>976</v>
+      </c>
+      <c r="P91" t="s">
+        <v>984</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>974</v>
+      </c>
+      <c r="R91" t="s">
+        <v>972</v>
+      </c>
+      <c r="S91" t="s">
+        <v>973</v>
+      </c>
+      <c r="T91" t="s">
+        <v>955</v>
+      </c>
+      <c r="U91" t="s">
+        <v>951</v>
+      </c>
+      <c r="W91" t="s">
+        <v>953</v>
+      </c>
+      <c r="X91" t="s">
+        <v>948</v>
+      </c>
+      <c r="Y91" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>898</v>
       </c>
@@ -16686,8 +18253,38 @@
       <c r="N92" t="s">
         <v>929</v>
       </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O92" t="s">
+        <v>964</v>
+      </c>
+      <c r="P92" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>974</v>
+      </c>
+      <c r="R92" t="s">
+        <v>972</v>
+      </c>
+      <c r="S92" t="s">
+        <v>973</v>
+      </c>
+      <c r="T92" t="s">
+        <v>955</v>
+      </c>
+      <c r="U92" t="s">
+        <v>953</v>
+      </c>
+      <c r="W92" t="s">
+        <v>957</v>
+      </c>
+      <c r="X92" t="s">
+        <v>957</v>
+      </c>
+      <c r="Y92" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>899</v>
       </c>
@@ -16731,7 +18328,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>900</v>
       </c>
@@ -16775,7 +18372,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>901</v>
       </c>
@@ -16818,8 +18415,38 @@
       <c r="N95" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O95" t="s">
+        <v>964</v>
+      </c>
+      <c r="P95" t="s">
+        <v>977</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>969</v>
+      </c>
+      <c r="R95" t="s">
+        <v>972</v>
+      </c>
+      <c r="S95" t="s">
+        <v>970</v>
+      </c>
+      <c r="T95" t="s">
+        <v>945</v>
+      </c>
+      <c r="U95" t="s">
+        <v>955</v>
+      </c>
+      <c r="W95" t="s">
+        <v>949</v>
+      </c>
+      <c r="X95" t="s">
+        <v>957</v>
+      </c>
+      <c r="Y95" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>902</v>
       </c>
@@ -16862,8 +18489,39 @@
       <c r="N96" t="s">
         <v>931</v>
       </c>
+      <c r="O96" t="s">
+        <v>964</v>
+      </c>
+      <c r="P96" t="s">
+        <v>978</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>969</v>
+      </c>
+      <c r="R96" t="s">
+        <v>970</v>
+      </c>
+      <c r="S96" t="s">
+        <v>974</v>
+      </c>
+      <c r="T96" t="s">
+        <v>948</v>
+      </c>
+      <c r="U96" t="s">
+        <v>959</v>
+      </c>
+      <c r="W96" t="s">
+        <v>951</v>
+      </c>
+      <c r="X96" t="s">
+        <v>949</v>
+      </c>
+      <c r="Y96" t="s">
+        <v>950</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Z96"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>

<commit_message>
Synced with game client GA 1.0.46
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -19,7 +19,7 @@
     <sheet name="LUT" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">attributes!$A$1:$B$137</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">attributes!$A$1:$B$148</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">skills!$A$1:$AE$246</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">stats!$A$1:$Z$96</definedName>
   </definedNames>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3427" uniqueCount="986">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3630" uniqueCount="1030">
   <si>
     <t>attributes</t>
   </si>
@@ -2991,6 +2991,138 @@
   </si>
   <si>
     <t>rec_jewel_2</t>
+  </si>
+  <si>
+    <t>tsingtao_6_0</t>
+  </si>
+  <si>
+    <t>Drunken Master TsingTao</t>
+  </si>
+  <si>
+    <t>Liquor Burn</t>
+  </si>
+  <si>
+    <t>One More Shot</t>
+  </si>
+  <si>
+    <t>Limber Moves</t>
+  </si>
+  <si>
+    <t>inflict_stun_on_counter_attack_probability</t>
+  </si>
+  <si>
+    <t>inflict_stun_on_counter_attack_turns</t>
+  </si>
+  <si>
+    <t>inflict_stun_on_speed_attack_probability</t>
+  </si>
+  <si>
+    <t>inflict_stun_on_speed_attack_turns</t>
+  </si>
+  <si>
+    <t>lingling_6_0</t>
+  </si>
+  <si>
+    <t>Pure Energy LingLing</t>
+  </si>
+  <si>
+    <t>Swirling Energy Orb</t>
+  </si>
+  <si>
+    <t>Furious Dragon Kick</t>
+  </si>
+  <si>
+    <t>stat_magical_attack_decrease_fraction</t>
+  </si>
+  <si>
+    <t>stat_magical_attack_decrease_turns</t>
+  </si>
+  <si>
+    <t>stat_magical_attack_decrease_probability</t>
+  </si>
+  <si>
+    <t>Energy Conversion</t>
+  </si>
+  <si>
+    <t>immunity_to_all_debuff_on_enemy_death_turns</t>
+  </si>
+  <si>
+    <t>maosong_6_0</t>
+  </si>
+  <si>
+    <t>Leader MaoSong</t>
+  </si>
+  <si>
+    <t>Dual Blade Slasher</t>
+  </si>
+  <si>
+    <t>Stone Destroyer</t>
+  </si>
+  <si>
+    <t>Tiger Skin Armor</t>
+  </si>
+  <si>
+    <t>bailong_6_0</t>
+  </si>
+  <si>
+    <t>Flash Fist BaiLong</t>
+  </si>
+  <si>
+    <t>Ten Flash Strike</t>
+  </si>
+  <si>
+    <t>Nunchuck Storm</t>
+  </si>
+  <si>
+    <t>Legend Reborn</t>
+  </si>
+  <si>
+    <t>berserk_before_dying_invincible_turns</t>
+  </si>
+  <si>
+    <t>berserk_before_dying_critical_rate_increase_fraction</t>
+  </si>
+  <si>
+    <t>berserk_before_dying_counter_rate_increase_fraction</t>
+  </si>
+  <si>
+    <t>tsingtao_6_1</t>
+  </si>
+  <si>
+    <t>tsingtao_6_2</t>
+  </si>
+  <si>
+    <t>lingling_6_1</t>
+  </si>
+  <si>
+    <t>lingling_6_2</t>
+  </si>
+  <si>
+    <t>maosong_6_1</t>
+  </si>
+  <si>
+    <t>maosong_6_2</t>
+  </si>
+  <si>
+    <t>bailong_6_1</t>
+  </si>
+  <si>
+    <t>bailong_6_2</t>
+  </si>
+  <si>
+    <t>S_</t>
+  </si>
+  <si>
+    <t>tsingtao_6</t>
+  </si>
+  <si>
+    <t>lingling_6</t>
+  </si>
+  <si>
+    <t>maosong_6</t>
+  </si>
+  <si>
+    <t>bailong_6</t>
   </si>
 </sst>
 </file>
@@ -3322,10 +3454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE258"/>
+  <dimension ref="A1:AE270"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A1:A1048576"/>
+    <sheetView topLeftCell="F251" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T263" sqref="T263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -4680,6 +4812,15 @@
       <c r="M34" t="s">
         <v>205</v>
       </c>
+      <c r="N34" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="O34" t="s">
+        <v>96</v>
+      </c>
+      <c r="P34">
+        <v>100</v>
+      </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -7703,34 +7844,16 @@
         <v>200</v>
       </c>
       <c r="G120">
-        <v>180</v>
+        <v>350</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="I120" t="s">
         <v>200</v>
       </c>
-      <c r="J120">
-        <v>80</v>
-      </c>
-      <c r="K120" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L120" t="s">
-        <v>200</v>
-      </c>
-      <c r="M120">
-        <v>2</v>
-      </c>
-      <c r="N120" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="O120" t="s">
-        <v>200</v>
-      </c>
-      <c r="P120" t="s">
-        <v>120</v>
+      <c r="J120" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="121" spans="1:22" x14ac:dyDescent="0.25">
@@ -7750,16 +7873,16 @@
         <v>119</v>
       </c>
       <c r="F121" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="G121">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H121" s="1" t="s">
         <v>42</v>
       </c>
       <c r="I121" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="J121">
         <v>50</v>
@@ -7768,7 +7891,7 @@
         <v>43</v>
       </c>
       <c r="L121" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="M121" t="s">
         <v>120</v>
@@ -7777,7 +7900,7 @@
         <v>44</v>
       </c>
       <c r="O121" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="P121">
         <v>2</v>
@@ -7794,13 +7917,31 @@
         <v>445</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>446</v>
+        <v>66</v>
       </c>
       <c r="F122" t="s">
         <v>99</v>
       </c>
       <c r="G122">
-        <v>50</v>
+        <v>40</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I122" t="s">
+        <v>99</v>
+      </c>
+      <c r="J122">
+        <v>2</v>
+      </c>
+      <c r="K122" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L122" t="s">
+        <v>96</v>
+      </c>
+      <c r="M122">
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="1:22" x14ac:dyDescent="0.25">
@@ -12268,7 +12409,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="257" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>789</v>
       </c>
@@ -12318,7 +12459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="258" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>790</v>
       </c>
@@ -12336,6 +12477,522 @@
       </c>
       <c r="G258">
         <v>3</v>
+      </c>
+    </row>
+    <row r="259" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>986</v>
+      </c>
+      <c r="B259" t="s">
+        <v>987</v>
+      </c>
+      <c r="C259" t="s">
+        <v>988</v>
+      </c>
+      <c r="D259">
+        <v>84</v>
+      </c>
+      <c r="E259" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F259" t="s">
+        <v>101</v>
+      </c>
+      <c r="G259">
+        <v>140</v>
+      </c>
+      <c r="H259" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I259" t="s">
+        <v>101</v>
+      </c>
+      <c r="J259" t="s">
+        <v>120</v>
+      </c>
+      <c r="K259" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L259" t="s">
+        <v>101</v>
+      </c>
+      <c r="M259">
+        <v>2</v>
+      </c>
+      <c r="N259" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O259" t="s">
+        <v>101</v>
+      </c>
+      <c r="P259">
+        <v>2</v>
+      </c>
+      <c r="Q259" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="R259" t="s">
+        <v>101</v>
+      </c>
+      <c r="S259">
+        <v>50</v>
+      </c>
+      <c r="T259" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U259" t="s">
+        <v>101</v>
+      </c>
+      <c r="V259" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="260" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B260" t="s">
+        <v>987</v>
+      </c>
+      <c r="C260" t="s">
+        <v>989</v>
+      </c>
+      <c r="D260">
+        <v>110</v>
+      </c>
+      <c r="E260" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F260" t="s">
+        <v>96</v>
+      </c>
+      <c r="G260">
+        <v>50</v>
+      </c>
+      <c r="H260" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="I260" t="s">
+        <v>96</v>
+      </c>
+      <c r="J260">
+        <v>2</v>
+      </c>
+      <c r="K260" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="L260" t="s">
+        <v>96</v>
+      </c>
+      <c r="M260">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="261" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B261" t="s">
+        <v>987</v>
+      </c>
+      <c r="C261" t="s">
+        <v>990</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F261" t="s">
+        <v>96</v>
+      </c>
+      <c r="G261">
+        <v>40</v>
+      </c>
+      <c r="H261" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="I261" t="s">
+        <v>200</v>
+      </c>
+      <c r="J261" t="s">
+        <v>120</v>
+      </c>
+      <c r="K261" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="L261" t="s">
+        <v>200</v>
+      </c>
+      <c r="M261">
+        <v>2</v>
+      </c>
+      <c r="N261" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="O261" t="s">
+        <v>200</v>
+      </c>
+      <c r="P261" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q261" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="R261" t="s">
+        <v>200</v>
+      </c>
+      <c r="S261">
+        <v>2</v>
+      </c>
+      <c r="T261" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="U261" t="s">
+        <v>200</v>
+      </c>
+      <c r="V261" t="s">
+        <v>120</v>
+      </c>
+      <c r="W261" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="X261" t="s">
+        <v>200</v>
+      </c>
+      <c r="Y261">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="262" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>995</v>
+      </c>
+      <c r="B262" t="s">
+        <v>996</v>
+      </c>
+      <c r="C262" t="s">
+        <v>997</v>
+      </c>
+      <c r="D262">
+        <v>120</v>
+      </c>
+      <c r="E262" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F262" t="s">
+        <v>200</v>
+      </c>
+      <c r="G262">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="263" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B263" t="s">
+        <v>996</v>
+      </c>
+      <c r="C263" t="s">
+        <v>998</v>
+      </c>
+      <c r="D263">
+        <v>76</v>
+      </c>
+      <c r="E263" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F263" t="s">
+        <v>101</v>
+      </c>
+      <c r="G263">
+        <v>140</v>
+      </c>
+      <c r="H263" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="I263" t="s">
+        <v>101</v>
+      </c>
+      <c r="J263">
+        <v>2</v>
+      </c>
+      <c r="K263" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="L263" t="s">
+        <v>101</v>
+      </c>
+      <c r="M263">
+        <v>40</v>
+      </c>
+      <c r="N263" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="O263" t="s">
+        <v>101</v>
+      </c>
+      <c r="P263" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q263" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R263" t="s">
+        <v>101</v>
+      </c>
+      <c r="S263">
+        <v>2</v>
+      </c>
+      <c r="T263" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U263" t="s">
+        <v>101</v>
+      </c>
+      <c r="V263">
+        <v>40</v>
+      </c>
+      <c r="W263" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="X263" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y263" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="264" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B264" t="s">
+        <v>996</v>
+      </c>
+      <c r="C264" t="s">
+        <v>1002</v>
+      </c>
+      <c r="E264" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F264" t="s">
+        <v>99</v>
+      </c>
+      <c r="G264">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="265" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B265" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C265" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D265">
+        <v>70</v>
+      </c>
+      <c r="E265" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F265" t="s">
+        <v>200</v>
+      </c>
+      <c r="G265">
+        <v>200</v>
+      </c>
+      <c r="H265" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="I265" t="s">
+        <v>200</v>
+      </c>
+      <c r="J265" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="266" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B266" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C266" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D266">
+        <v>120</v>
+      </c>
+      <c r="E266" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F266" t="s">
+        <v>145</v>
+      </c>
+      <c r="G266">
+        <v>140</v>
+      </c>
+      <c r="H266" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I266" t="s">
+        <v>145</v>
+      </c>
+      <c r="J266" t="s">
+        <v>120</v>
+      </c>
+      <c r="K266" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L266" t="s">
+        <v>145</v>
+      </c>
+      <c r="M266">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="267" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B267" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C267" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E267" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F267" t="s">
+        <v>96</v>
+      </c>
+      <c r="G267">
+        <v>2</v>
+      </c>
+      <c r="H267" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I267" t="s">
+        <v>96</v>
+      </c>
+      <c r="J267">
+        <v>10</v>
+      </c>
+      <c r="K267" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="L267" t="s">
+        <v>96</v>
+      </c>
+      <c r="M267">
+        <v>10</v>
+      </c>
+      <c r="N267" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="O267" t="s">
+        <v>96</v>
+      </c>
+      <c r="P267">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="268" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B268" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C268" t="s">
+        <v>1011</v>
+      </c>
+      <c r="D268">
+        <v>120</v>
+      </c>
+      <c r="E268" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F268" t="s">
+        <v>200</v>
+      </c>
+      <c r="G268">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="269" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B269" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C269" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D269">
+        <v>125</v>
+      </c>
+      <c r="E269" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F269" t="s">
+        <v>145</v>
+      </c>
+      <c r="G269">
+        <v>140</v>
+      </c>
+      <c r="H269" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I269" t="s">
+        <v>145</v>
+      </c>
+      <c r="J269" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="270" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B270" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C270" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E270" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="F270" t="s">
+        <v>96</v>
+      </c>
+      <c r="G270">
+        <v>2</v>
+      </c>
+      <c r="H270" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="I270" t="s">
+        <v>96</v>
+      </c>
+      <c r="J270" t="s">
+        <v>240</v>
+      </c>
+      <c r="K270" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="L270" t="s">
+        <v>96</v>
+      </c>
+      <c r="M270" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -12343,240 +13000,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="39">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>LUT!$C:$C</xm:f>
           </x14:formula1>
-          <xm:sqref>X2:X1048576 O2:O69 U2:U1048576 O71:O1048576 I2:I1048576 R2:R1048576 F2:F1048576 M47 L2:L1048576</xm:sqref>
+          <xm:sqref>O2:O69 M47 X2:X1048576 O271:O1048576 U2:U1048576 L2:L266 O71:O266 F2:F1048576 I2:I1048576 O268:O269 R121:R1048576 R2:R119 L268:L1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>attributes!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>W90:W1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>AC87</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>T2:T240</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>T242:T1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>N9:N69</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>N2:N7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>Q2:Q240</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>Q242:Q1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>W2:W87</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>Z87</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>N71:N240</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>N242:N247</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>N249:N256</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>N258:N1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>K2:K240</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>K242:K247</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>K249:K256</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>K258:K1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H239</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>H242</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>H244:H245</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>H247:H250</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>H252:H1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>K257</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>N257</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>K248</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>N248</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>H243</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>H240:H241</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>E240</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>K241</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>N241</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>Q241</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>T241</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E239</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>E241:E1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>H251</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>H246</xm:sqref>
+          <xm:sqref>E274:E1048576 H266:H1048576 E2:E270 K264:K1048576 N271:N1048576 N264:N269 H263 T264:T1048576 AC87 K2:K262 Z87 W2:W87 N2:N7 N9:N69 N71:N262 Q2:Q119 Q121:Q1048576 T2:T262 W90:W262 W264:W1048576 H2:H261</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -12586,13 +13021,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z96"/>
+  <dimension ref="A1:Z100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="14" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="14" ySplit="1" topLeftCell="Q74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="O1" sqref="O1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S1" sqref="S1"/>
+      <selection pane="bottomRight" activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -18518,6 +18953,287 @@
       </c>
       <c r="Y96" t="s">
         <v>950</v>
+      </c>
+    </row>
+    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B97" t="s">
+        <v>910</v>
+      </c>
+      <c r="C97">
+        <v>16</v>
+      </c>
+      <c r="D97" s="2">
+        <v>1258</v>
+      </c>
+      <c r="E97" s="2">
+        <v>525</v>
+      </c>
+      <c r="F97" s="2">
+        <v>296</v>
+      </c>
+      <c r="G97" s="2">
+        <v>3298</v>
+      </c>
+      <c r="H97" s="2">
+        <v>1335</v>
+      </c>
+      <c r="I97" s="2">
+        <v>746</v>
+      </c>
+      <c r="J97" s="2">
+        <v>3953</v>
+      </c>
+      <c r="K97" s="2">
+        <v>1530</v>
+      </c>
+      <c r="L97" s="2">
+        <v>881</v>
+      </c>
+      <c r="M97" t="s">
+        <v>927</v>
+      </c>
+      <c r="N97" t="s">
+        <v>929</v>
+      </c>
+      <c r="T97" t="s">
+        <v>955</v>
+      </c>
+      <c r="U97" t="s">
+        <v>953</v>
+      </c>
+      <c r="W97" t="s">
+        <v>955</v>
+      </c>
+      <c r="X97" t="s">
+        <v>953</v>
+      </c>
+      <c r="Y97" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B98" t="s">
+        <v>910</v>
+      </c>
+      <c r="C98">
+        <v>27</v>
+      </c>
+      <c r="D98" s="2">
+        <v>937</v>
+      </c>
+      <c r="E98" s="2">
+        <v>567</v>
+      </c>
+      <c r="F98" s="2">
+        <v>253</v>
+      </c>
+      <c r="G98" s="2">
+        <v>2437</v>
+      </c>
+      <c r="H98" s="2">
+        <v>1407</v>
+      </c>
+      <c r="I98" s="2">
+        <v>685</v>
+      </c>
+      <c r="J98" s="2">
+        <v>2912</v>
+      </c>
+      <c r="K98" s="2">
+        <v>1637</v>
+      </c>
+      <c r="L98" s="2">
+        <v>790</v>
+      </c>
+      <c r="M98" t="s">
+        <v>927</v>
+      </c>
+      <c r="N98" t="s">
+        <v>931</v>
+      </c>
+      <c r="O98" t="s">
+        <v>964</v>
+      </c>
+      <c r="P98" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>966</v>
+      </c>
+      <c r="R98" t="s">
+        <v>969</v>
+      </c>
+      <c r="S98" t="s">
+        <v>967</v>
+      </c>
+      <c r="T98" t="s">
+        <v>949</v>
+      </c>
+      <c r="U98" t="s">
+        <v>951</v>
+      </c>
+      <c r="W98" t="s">
+        <v>957</v>
+      </c>
+      <c r="X98" t="s">
+        <v>959</v>
+      </c>
+      <c r="Y98" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B99" t="s">
+        <v>909</v>
+      </c>
+      <c r="C99">
+        <v>27</v>
+      </c>
+      <c r="D99" s="2">
+        <v>966</v>
+      </c>
+      <c r="E99" s="2">
+        <v>567</v>
+      </c>
+      <c r="F99" s="2">
+        <v>239</v>
+      </c>
+      <c r="G99" s="2">
+        <v>2526</v>
+      </c>
+      <c r="H99" s="2">
+        <v>1407</v>
+      </c>
+      <c r="I99" s="2">
+        <v>641</v>
+      </c>
+      <c r="J99" s="2">
+        <v>3001</v>
+      </c>
+      <c r="K99" s="2">
+        <v>1637</v>
+      </c>
+      <c r="L99" s="2">
+        <v>746</v>
+      </c>
+      <c r="M99" t="s">
+        <v>927</v>
+      </c>
+      <c r="N99" t="s">
+        <v>930</v>
+      </c>
+      <c r="O99" t="s">
+        <v>964</v>
+      </c>
+      <c r="P99" t="s">
+        <v>965</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>966</v>
+      </c>
+      <c r="R99" t="s">
+        <v>969</v>
+      </c>
+      <c r="S99" t="s">
+        <v>967</v>
+      </c>
+      <c r="T99" t="s">
+        <v>955</v>
+      </c>
+      <c r="U99" t="s">
+        <v>953</v>
+      </c>
+      <c r="W99" t="s">
+        <v>955</v>
+      </c>
+      <c r="X99" t="s">
+        <v>955</v>
+      </c>
+      <c r="Y99" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B100" t="s">
+        <v>909</v>
+      </c>
+      <c r="C100">
+        <v>29</v>
+      </c>
+      <c r="D100" s="2">
+        <v>947</v>
+      </c>
+      <c r="E100" s="2">
+        <v>569</v>
+      </c>
+      <c r="F100" s="2">
+        <v>244</v>
+      </c>
+      <c r="G100" s="2">
+        <v>2453</v>
+      </c>
+      <c r="H100" s="2">
+        <v>1415</v>
+      </c>
+      <c r="I100" s="2">
+        <v>652</v>
+      </c>
+      <c r="J100" s="2">
+        <v>2928</v>
+      </c>
+      <c r="K100" s="2">
+        <v>1645</v>
+      </c>
+      <c r="L100" s="2">
+        <v>757</v>
+      </c>
+      <c r="M100" t="s">
+        <v>927</v>
+      </c>
+      <c r="N100" t="s">
+        <v>930</v>
+      </c>
+      <c r="O100" t="s">
+        <v>964</v>
+      </c>
+      <c r="P100" t="s">
+        <v>975</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>966</v>
+      </c>
+      <c r="R100" t="s">
+        <v>969</v>
+      </c>
+      <c r="S100" t="s">
+        <v>967</v>
+      </c>
+      <c r="T100" t="s">
+        <v>1025</v>
+      </c>
+      <c r="U100" t="s">
+        <v>953</v>
+      </c>
+      <c r="W100" t="s">
+        <v>950</v>
+      </c>
+      <c r="X100" t="s">
+        <v>959</v>
+      </c>
+      <c r="Y100" t="s">
+        <v>953</v>
       </c>
     </row>
   </sheetData>
@@ -18990,11 +19706,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B146"/>
+  <dimension ref="A1:B157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -19237,7 +19953,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>802</v>
+        <v>1003</v>
       </c>
       <c r="B30" t="s">
         <v>133</v>
@@ -19245,7 +19961,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>802</v>
       </c>
       <c r="B31" t="s">
         <v>133</v>
@@ -19253,7 +19969,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
         <v>133</v>
@@ -19261,7 +19977,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
         <v>133</v>
@@ -19269,7 +19985,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s">
         <v>133</v>
@@ -19277,7 +19993,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B35" t="s">
         <v>133</v>
@@ -19285,7 +20001,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B36" t="s">
         <v>133</v>
@@ -19293,7 +20009,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B37" t="s">
         <v>133</v>
@@ -19301,31 +20017,31 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B38" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B39" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>408</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>23</v>
+        <v>408</v>
       </c>
       <c r="B41" t="s">
         <v>134</v>
@@ -19333,7 +20049,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B42" t="s">
         <v>134</v>
@@ -19341,7 +20057,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B43" t="s">
         <v>134</v>
@@ -19349,7 +20065,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B44" t="s">
         <v>134</v>
@@ -19357,7 +20073,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B45" t="s">
         <v>134</v>
@@ -19365,7 +20081,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B46" t="s">
         <v>134</v>
@@ -19373,7 +20089,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>285</v>
+        <v>26</v>
       </c>
       <c r="B47" t="s">
         <v>134</v>
@@ -19381,7 +20097,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B48" t="s">
         <v>134</v>
@@ -19389,7 +20105,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>27</v>
+        <v>284</v>
       </c>
       <c r="B49" t="s">
         <v>134</v>
@@ -19397,7 +20113,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B50" t="s">
         <v>134</v>
@@ -19405,7 +20121,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>287</v>
+        <v>28</v>
       </c>
       <c r="B51" t="s">
         <v>134</v>
@@ -19413,7 +20129,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B52" t="s">
         <v>134</v>
@@ -19421,7 +20137,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>29</v>
+        <v>286</v>
       </c>
       <c r="B53" t="s">
         <v>134</v>
@@ -19429,7 +20145,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B54" t="s">
         <v>134</v>
@@ -19437,7 +20153,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B55" t="s">
         <v>134</v>
@@ -19445,7 +20161,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B56" t="s">
         <v>134</v>
@@ -19453,7 +20169,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B57" t="s">
         <v>134</v>
@@ -19461,7 +20177,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="B58" t="s">
         <v>134</v>
@@ -19469,7 +20185,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B59" t="s">
         <v>134</v>
@@ -19477,7 +20193,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B60" t="s">
         <v>134</v>
@@ -19485,7 +20201,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" t="s">
         <v>134</v>
@@ -19493,7 +20209,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B62" t="s">
         <v>134</v>
@@ -19501,7 +20217,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B63" t="s">
         <v>134</v>
@@ -19509,7 +20225,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B64" t="s">
         <v>134</v>
@@ -19517,7 +20233,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B65" t="s">
         <v>134</v>
@@ -19525,7 +20241,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B66" t="s">
         <v>134</v>
@@ -19533,7 +20249,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>409</v>
+        <v>77</v>
       </c>
       <c r="B67" t="s">
         <v>134</v>
@@ -19541,7 +20257,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>409</v>
       </c>
       <c r="B68" t="s">
         <v>134</v>
@@ -19549,7 +20265,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B69" t="s">
         <v>134</v>
@@ -19557,7 +20273,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B70" t="s">
         <v>134</v>
@@ -19565,7 +20281,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B71" t="s">
         <v>134</v>
@@ -19573,7 +20289,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>302</v>
+        <v>81</v>
       </c>
       <c r="B72" t="s">
         <v>134</v>
@@ -19581,7 +20297,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B73" t="s">
         <v>134</v>
@@ -19589,7 +20305,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>82</v>
+        <v>301</v>
       </c>
       <c r="B74" t="s">
         <v>134</v>
@@ -19597,7 +20313,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>83</v>
+        <v>991</v>
       </c>
       <c r="B75" t="s">
         <v>134</v>
@@ -19605,79 +20321,79 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>3</v>
+        <v>992</v>
       </c>
       <c r="B76" t="s">
-        <v>174</v>
+        <v>134</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>173</v>
+        <v>993</v>
       </c>
       <c r="B77" t="s">
-        <v>174</v>
+        <v>134</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>206</v>
+        <v>994</v>
       </c>
       <c r="B78" t="s">
-        <v>174</v>
+        <v>134</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>207</v>
+        <v>82</v>
       </c>
       <c r="B79" t="s">
-        <v>174</v>
+        <v>134</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>356</v>
+        <v>83</v>
       </c>
       <c r="B80" t="s">
-        <v>2</v>
+        <v>134</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>355</v>
+        <v>3</v>
       </c>
       <c r="B81" t="s">
-        <v>2</v>
+        <v>174</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>138</v>
+        <v>173</v>
       </c>
       <c r="B82" t="s">
-        <v>2</v>
+        <v>174</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>563</v>
+        <v>206</v>
       </c>
       <c r="B83" t="s">
-        <v>2</v>
+        <v>174</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>5</v>
+        <v>207</v>
       </c>
       <c r="B84" t="s">
-        <v>2</v>
+        <v>174</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>4</v>
+        <v>356</v>
       </c>
       <c r="B85" t="s">
         <v>2</v>
@@ -19685,31 +20401,31 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>150</v>
+        <v>355</v>
       </c>
       <c r="B86" t="s">
-        <v>174</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>763</v>
+        <v>138</v>
       </c>
       <c r="B87" t="s">
-        <v>137</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>764</v>
+        <v>1014</v>
       </c>
       <c r="B88" t="s">
-        <v>137</v>
+        <v>174</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>765</v>
+        <v>1015</v>
       </c>
       <c r="B89" t="s">
         <v>137</v>
@@ -19717,7 +20433,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>41</v>
+        <v>1016</v>
       </c>
       <c r="B90" t="s">
         <v>137</v>
@@ -19725,39 +20441,39 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>367</v>
+        <v>563</v>
       </c>
       <c r="B91" t="s">
-        <v>137</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>246</v>
+        <v>5</v>
       </c>
       <c r="B92" t="s">
-        <v>137</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="B93" t="s">
-        <v>137</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>247</v>
+        <v>150</v>
       </c>
       <c r="B94" t="s">
-        <v>137</v>
+        <v>174</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>39</v>
+        <v>763</v>
       </c>
       <c r="B95" t="s">
         <v>137</v>
@@ -19765,7 +20481,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>331</v>
+        <v>764</v>
       </c>
       <c r="B96" t="s">
         <v>137</v>
@@ -19773,7 +20489,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>333</v>
+        <v>765</v>
       </c>
       <c r="B97" t="s">
         <v>137</v>
@@ -19781,7 +20497,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B98" t="s">
         <v>137</v>
@@ -19789,7 +20505,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>332</v>
+        <v>367</v>
       </c>
       <c r="B99" t="s">
         <v>137</v>
@@ -19797,7 +20513,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>42</v>
+        <v>246</v>
       </c>
       <c r="B100" t="s">
         <v>137</v>
@@ -19805,7 +20521,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B101" t="s">
         <v>137</v>
@@ -19813,7 +20529,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>44</v>
+        <v>247</v>
       </c>
       <c r="B102" t="s">
         <v>137</v>
@@ -19821,7 +20537,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B103" t="s">
         <v>137</v>
@@ -19829,7 +20545,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>60</v>
+        <v>331</v>
       </c>
       <c r="B104" t="s">
         <v>137</v>
@@ -19837,7 +20553,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>45</v>
+        <v>333</v>
       </c>
       <c r="B105" t="s">
         <v>137</v>
@@ -19845,7 +20561,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B106" t="s">
         <v>137</v>
@@ -19853,7 +20569,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>47</v>
+        <v>332</v>
       </c>
       <c r="B107" t="s">
         <v>137</v>
@@ -19861,7 +20577,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="B108" t="s">
         <v>137</v>
@@ -19869,7 +20585,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="B109" t="s">
         <v>137</v>
@@ -19877,7 +20593,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B110" t="s">
         <v>137</v>
@@ -19885,7 +20601,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B111" t="s">
         <v>137</v>
@@ -19893,7 +20609,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B112" t="s">
         <v>137</v>
@@ -19901,7 +20617,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B113" t="s">
         <v>137</v>
@@ -19909,7 +20625,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B114" t="s">
         <v>137</v>
@@ -19917,7 +20633,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B115" t="s">
         <v>137</v>
@@ -19925,7 +20641,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B116" t="s">
         <v>137</v>
@@ -19933,15 +20649,15 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>140</v>
+        <v>225</v>
       </c>
       <c r="B117" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="B118" t="s">
         <v>137</v>
@@ -19949,7 +20665,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>446</v>
+        <v>49</v>
       </c>
       <c r="B119" t="s">
         <v>137</v>
@@ -19957,7 +20673,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="B120" t="s">
         <v>137</v>
@@ -19965,7 +20681,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="B121" t="s">
         <v>137</v>
@@ -19973,7 +20689,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>142</v>
+        <v>63</v>
       </c>
       <c r="B122" t="s">
         <v>137</v>
@@ -19981,7 +20697,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>357</v>
+        <v>51</v>
       </c>
       <c r="B123" t="s">
         <v>137</v>
@@ -19989,7 +20705,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>141</v>
+        <v>52</v>
       </c>
       <c r="B124" t="s">
         <v>137</v>
@@ -19997,15 +20713,15 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="B125" t="s">
-        <v>137</v>
+        <v>174</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B126" t="s">
         <v>137</v>
@@ -20013,7 +20729,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>89</v>
+        <v>446</v>
       </c>
       <c r="B127" t="s">
         <v>137</v>
@@ -20021,7 +20737,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B128" t="s">
         <v>137</v>
@@ -20029,7 +20745,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="B129" t="s">
         <v>137</v>
@@ -20037,7 +20753,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>65</v>
+        <v>142</v>
       </c>
       <c r="B130" t="s">
         <v>137</v>
@@ -20045,7 +20761,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>66</v>
+        <v>357</v>
       </c>
       <c r="B131" t="s">
         <v>137</v>
@@ -20053,7 +20769,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>67</v>
+        <v>141</v>
       </c>
       <c r="B132" t="s">
         <v>137</v>
@@ -20061,7 +20777,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="B133" t="s">
         <v>137</v>
@@ -20069,7 +20785,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="B134" t="s">
         <v>137</v>
@@ -20077,7 +20793,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="B135" t="s">
         <v>137</v>
@@ -20085,7 +20801,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="B136" t="s">
         <v>137</v>
@@ -20093,7 +20809,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B137" t="s">
         <v>137</v>
@@ -20101,7 +20817,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B138" t="s">
         <v>137</v>
@@ -20109,7 +20825,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>431</v>
+        <v>66</v>
       </c>
       <c r="B139" t="s">
         <v>137</v>
@@ -20117,7 +20833,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B140" t="s">
         <v>137</v>
@@ -20125,7 +20841,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B141" t="s">
         <v>137</v>
@@ -20133,46 +20849,134 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>575</v>
+        <v>69</v>
       </c>
       <c r="B142" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>577</v>
+        <v>1000</v>
       </c>
       <c r="B143" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>576</v>
+        <v>999</v>
       </c>
       <c r="B144" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>15</v>
+        <v>1001</v>
       </c>
       <c r="B145" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
+        <v>53</v>
+      </c>
+      <c r="B146" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>54</v>
+      </c>
+      <c r="B147" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>55</v>
+      </c>
+      <c r="B148" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>70</v>
+      </c>
+      <c r="B149" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>431</v>
+      </c>
+      <c r="B150" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>71</v>
+      </c>
+      <c r="B151" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>72</v>
+      </c>
+      <c r="B152" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>575</v>
+      </c>
+      <c r="B153" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>577</v>
+      </c>
+      <c r="B154" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>576</v>
+      </c>
+      <c r="B155" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>15</v>
+      </c>
+      <c r="B156" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>12</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B157" t="s">
         <v>174</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B137">
+  <autoFilter ref="A1:B148">
     <sortState ref="A2:B139">
       <sortCondition ref="A1:A130"/>
     </sortState>

</xml_diff>

<commit_message>
Fixed Daisy's second active skill.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11479" windowHeight="10610" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11479" windowHeight="10610"/>
   </bookViews>
   <sheets>
     <sheet name="skills" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3630" uniqueCount="1030">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3630" uniqueCount="1029">
   <si>
     <t>attributes</t>
   </si>
@@ -3108,9 +3108,6 @@
   </si>
   <si>
     <t>bailong_6_2</t>
-  </si>
-  <si>
-    <t>S_</t>
   </si>
   <si>
     <t>tsingtao_6</t>
@@ -3456,8 +3453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE270"/>
   <sheetViews>
-    <sheetView topLeftCell="F251" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T263" sqref="T263"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N122" sqref="N122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -7879,7 +7876,7 @@
         <v>100</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="I121" t="s">
         <v>201</v>
@@ -7888,7 +7885,7 @@
         <v>50</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="L121" t="s">
         <v>201</v>
@@ -7897,7 +7894,7 @@
         <v>120</v>
       </c>
       <c r="N121" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="O121" t="s">
         <v>201</v>
@@ -13023,11 +13020,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="14" ySplit="1" topLeftCell="Q74" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="14" ySplit="1" topLeftCell="O74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="O1" sqref="O1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A101" sqref="A101"/>
+      <selection pane="bottomRight" activeCell="T100" sqref="T100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -18957,7 +18954,7 @@
     </row>
     <row r="97" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B97" t="s">
         <v>910</v>
@@ -19016,7 +19013,7 @@
     </row>
     <row r="98" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B98" t="s">
         <v>910</v>
@@ -19090,7 +19087,7 @@
     </row>
     <row r="99" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B99" t="s">
         <v>909</v>
@@ -19164,7 +19161,7 @@
     </row>
     <row r="100" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="B100" t="s">
         <v>909</v>
@@ -19221,7 +19218,7 @@
         <v>967</v>
       </c>
       <c r="T100" t="s">
-        <v>1025</v>
+        <v>950</v>
       </c>
       <c r="U100" t="s">
         <v>953</v>

</xml_diff>

<commit_message>
Fixed Rachel and Eileene element.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -13021,10 +13021,10 @@
   <dimension ref="A1:Z100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y5" sqref="Y5"/>
+      <selection pane="bottomRight" activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -13220,45 +13220,45 @@
       </c>
       <c r="D3">
         <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M3,"_",$N3),stats_base!$C:$C,0))</f>
-        <v>1086</v>
+        <v>1486</v>
       </c>
       <c r="E3">
         <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M3,"_",$N3),stats_base!$C:$C,0))</f>
-        <v>696</v>
+        <v>637</v>
       </c>
       <c r="F3">
         <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M3,"_",$N3),stats_base!$C:$C,0))</f>
-        <v>328</v>
+        <v>415</v>
       </c>
       <c r="G3">
         <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M3,"_",$N3),stats_base!$C:$C,0))</f>
-        <v>2730</v>
+        <v>3688</v>
       </c>
       <c r="H3">
         <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M3,"_",$N3),stats_base!$C:$C,0))</f>
-        <v>1680</v>
+        <v>1555</v>
       </c>
       <c r="I3">
         <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M3,"_",$N3),stats_base!$C:$C,0))</f>
-        <v>874</v>
+        <v>1039</v>
       </c>
       <c r="J3">
         <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M3,"_",$N3),stats_base!$C:$C,0))</f>
-        <v>3205</v>
+        <v>4343</v>
       </c>
       <c r="K3">
         <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M3,"_",$N3),stats_base!$C:$C,0))</f>
-        <v>1910</v>
+        <v>1750</v>
       </c>
       <c r="L3">
         <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M3,"_",$N3),stats_base!$C:$C,0))</f>
-        <v>979</v>
+        <v>1174</v>
       </c>
       <c r="M3" t="s">
         <v>923</v>
       </c>
       <c r="N3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="O3" t="s">
         <v>964</v>
@@ -13309,45 +13309,45 @@
       </c>
       <c r="D4">
         <f>INDEX(stats_base!D:D,MATCH(CONCATENATE($M4,"_",$N4),stats_base!$C:$C,0))</f>
-        <v>1086</v>
+        <v>1486</v>
       </c>
       <c r="E4">
         <f>INDEX(stats_base!E:E,MATCH(CONCATENATE($M4,"_",$N4),stats_base!$C:$C,0))</f>
-        <v>696</v>
+        <v>637</v>
       </c>
       <c r="F4">
         <f>INDEX(stats_base!F:F,MATCH(CONCATENATE($M4,"_",$N4),stats_base!$C:$C,0))</f>
-        <v>328</v>
+        <v>415</v>
       </c>
       <c r="G4">
         <f>INDEX(stats_base!G:G,MATCH(CONCATENATE($M4,"_",$N4),stats_base!$C:$C,0))</f>
-        <v>2730</v>
+        <v>3688</v>
       </c>
       <c r="H4">
         <f>INDEX(stats_base!H:H,MATCH(CONCATENATE($M4,"_",$N4),stats_base!$C:$C,0))</f>
-        <v>1680</v>
+        <v>1555</v>
       </c>
       <c r="I4">
         <f>INDEX(stats_base!I:I,MATCH(CONCATENATE($M4,"_",$N4),stats_base!$C:$C,0))</f>
-        <v>874</v>
+        <v>1039</v>
       </c>
       <c r="J4">
         <f>INDEX(stats_base!J:J,MATCH(CONCATENATE($M4,"_",$N4),stats_base!$C:$C,0))</f>
-        <v>3205</v>
+        <v>4343</v>
       </c>
       <c r="K4">
         <f>INDEX(stats_base!K:K,MATCH(CONCATENATE($M4,"_",$N4),stats_base!$C:$C,0))</f>
-        <v>1910</v>
+        <v>1750</v>
       </c>
       <c r="L4">
         <f>INDEX(stats_base!L:L,MATCH(CONCATENATE($M4,"_",$N4),stats_base!$C:$C,0))</f>
-        <v>979</v>
+        <v>1174</v>
       </c>
       <c r="M4" t="s">
         <v>923</v>
       </c>
       <c r="N4" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="O4" t="s">
         <v>964</v>

</xml_diff>

<commit_message>
Changed Daisy's recommended equipment.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -13021,10 +13021,10 @@
   <dimension ref="A1:Z100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N4" sqref="N4"/>
+      <selection pane="bottomRight" activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -16378,13 +16378,13 @@
         <v>977</v>
       </c>
       <c r="P42" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="Q42" t="s">
         <v>966</v>
       </c>
       <c r="R42" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="S42" t="s">
         <v>967</v>
@@ -19377,7 +19377,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="D16:L16"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Completed Masteries, Friendship Quests, and Guide Quests
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11479" windowHeight="10610" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11479" windowHeight="10610"/>
   </bookViews>
   <sheets>
     <sheet name="skills" sheetId="1" r:id="rId1"/>
@@ -3456,8 +3456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE270"/>
   <sheetViews>
-    <sheetView topLeftCell="D79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M98" sqref="M98"/>
+    <sheetView tabSelected="1" topLeftCell="I79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P87" sqref="P87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -6684,6 +6684,9 @@
       </c>
       <c r="F87" t="s">
         <v>98</v>
+      </c>
+      <c r="G87">
+        <v>25</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>224</v>
@@ -20002,8 +20005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed Lania's attack type.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -13199,10 +13199,10 @@
   <dimension ref="A1:AA100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA101" sqref="AA101"/>
+      <selection pane="bottomRight" activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -16567,7 +16567,7 @@
         <v>890</v>
       </c>
       <c r="B55" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="C55">
         <v>16</v>

</xml_diff>

<commit_message>
Updated to 3/23 new heros.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -19,7 +19,7 @@
     <sheet name="LUT" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">attributes!$A$1:$B$158</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">attributes!$A$1:$B$160</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">skills!$A$1:$AE$246</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">stats!$A$1:$Z$100</definedName>
   </definedNames>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3712" uniqueCount="1033">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3948" uniqueCount="1077">
   <si>
     <t>attributes</t>
   </si>
@@ -3132,6 +3132,138 @@
   </si>
   <si>
     <t>S+ (Fri)</t>
+  </si>
+  <si>
+    <t>lubu_6_0</t>
+  </si>
+  <si>
+    <t>Invincible LuBu</t>
+  </si>
+  <si>
+    <t>Cosmic Dimension Slash</t>
+  </si>
+  <si>
+    <t>attack_physical_with_piercing_probability</t>
+  </si>
+  <si>
+    <t>Crimson Gale Slam</t>
+  </si>
+  <si>
+    <t>Super Power</t>
+  </si>
+  <si>
+    <t>immunity_to_all_damage_hit_count</t>
+  </si>
+  <si>
+    <t>zhaoyun_6_0</t>
+  </si>
+  <si>
+    <t>Tornado Thrust</t>
+  </si>
+  <si>
+    <t>Tornado Spears Thrust</t>
+  </si>
+  <si>
+    <t>Protection Aura</t>
+  </si>
+  <si>
+    <t>Chancellor ZhaoYun</t>
+  </si>
+  <si>
+    <t>diaochan_6_0</t>
+  </si>
+  <si>
+    <t>Hidden Moon Diaochan</t>
+  </si>
+  <si>
+    <t>March Forward</t>
+  </si>
+  <si>
+    <t>Song of Protection</t>
+  </si>
+  <si>
+    <t>Crescent Andante</t>
+  </si>
+  <si>
+    <t>zhugeliang_6_0</t>
+  </si>
+  <si>
+    <t>Great Strategist ZhugeLiang</t>
+  </si>
+  <si>
+    <t>The Eight Trigram</t>
+  </si>
+  <si>
+    <t>Rain of Flame Arrows</t>
+  </si>
+  <si>
+    <t>War Tactics</t>
+  </si>
+  <si>
+    <t>guanyu_6</t>
+  </si>
+  <si>
+    <t>guanyu_6_0</t>
+  </si>
+  <si>
+    <t>Virtuous King GuanYu</t>
+  </si>
+  <si>
+    <t>Dragon Burst Slash</t>
+  </si>
+  <si>
+    <t>Hold Your Position!</t>
+  </si>
+  <si>
+    <t>Figure of Brilliance</t>
+  </si>
+  <si>
+    <t>lubu_6_1</t>
+  </si>
+  <si>
+    <t>lubu_6_2</t>
+  </si>
+  <si>
+    <t>zhaoyun_6_1</t>
+  </si>
+  <si>
+    <t>zhaoyun_6_2</t>
+  </si>
+  <si>
+    <t>diaochan_6_1</t>
+  </si>
+  <si>
+    <t>diaochan_6_2</t>
+  </si>
+  <si>
+    <t>zhugeliang_6_1</t>
+  </si>
+  <si>
+    <t>zhugeliang_6_2</t>
+  </si>
+  <si>
+    <t>guanyu_6_1</t>
+  </si>
+  <si>
+    <t>guanyu_6_2</t>
+  </si>
+  <si>
+    <t>lubu_6</t>
+  </si>
+  <si>
+    <t>zhaoyun_6</t>
+  </si>
+  <si>
+    <t>diaochan_6</t>
+  </si>
+  <si>
+    <t>zhugeliang_6</t>
+  </si>
+  <si>
+    <t>Double HP / Double block</t>
+  </si>
+  <si>
+    <t>Life Steal</t>
   </si>
 </sst>
 </file>
@@ -3463,10 +3595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE270"/>
+  <dimension ref="A1:AE285"/>
   <sheetViews>
-    <sheetView topLeftCell="I79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P87" sqref="P87"/>
+    <sheetView topLeftCell="H262" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H281" sqref="H281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -13049,143 +13181,632 @@
         <v>239</v>
       </c>
     </row>
+    <row r="271" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B271" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C271" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D271">
+        <v>76</v>
+      </c>
+      <c r="E271" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F271" t="s">
+        <v>200</v>
+      </c>
+      <c r="G271">
+        <v>150</v>
+      </c>
+      <c r="H271" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="I271" t="s">
+        <v>200</v>
+      </c>
+      <c r="J271" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="272" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B272" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C272" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D272">
+        <v>100</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F272" t="s">
+        <v>200</v>
+      </c>
+      <c r="G272">
+        <v>100</v>
+      </c>
+      <c r="H272" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I272" t="s">
+        <v>200</v>
+      </c>
+      <c r="J272" t="s">
+        <v>142</v>
+      </c>
+      <c r="K272" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="L272" t="s">
+        <v>200</v>
+      </c>
+      <c r="M272">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="273" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B273" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C273" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E273" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F273" t="s">
+        <v>95</v>
+      </c>
+      <c r="G273">
+        <v>50</v>
+      </c>
+      <c r="H273" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="I273" t="s">
+        <v>95</v>
+      </c>
+      <c r="J273">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="274" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B274" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C274" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D274">
+        <v>74</v>
+      </c>
+      <c r="E274" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F274" t="s">
+        <v>199</v>
+      </c>
+      <c r="G274">
+        <v>190</v>
+      </c>
+      <c r="H274" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="I274" t="s">
+        <v>199</v>
+      </c>
+      <c r="J274">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="275" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B275" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C275" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D275">
+        <v>70</v>
+      </c>
+      <c r="E275" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F275" t="s">
+        <v>100</v>
+      </c>
+      <c r="G275">
+        <v>100</v>
+      </c>
+      <c r="H275" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="I275" t="s">
+        <v>100</v>
+      </c>
+      <c r="J275">
+        <v>50</v>
+      </c>
+      <c r="K275" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L275" t="s">
+        <v>100</v>
+      </c>
+      <c r="M275" t="s">
+        <v>119</v>
+      </c>
+      <c r="N275" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O275" t="s">
+        <v>100</v>
+      </c>
+      <c r="P275">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="276" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B276" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C276" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E276" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F276" t="s">
+        <v>95</v>
+      </c>
+      <c r="G276">
+        <v>60</v>
+      </c>
+      <c r="H276" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I276" t="s">
+        <v>95</v>
+      </c>
+      <c r="J276">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="277" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B277" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C277" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D277">
+        <v>100</v>
+      </c>
+      <c r="E277" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="F277" t="s">
+        <v>98</v>
+      </c>
+      <c r="G277">
+        <v>60</v>
+      </c>
+      <c r="H277" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="I277" t="s">
+        <v>98</v>
+      </c>
+      <c r="J277">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="278" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B278" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C278" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D278">
+        <v>80</v>
+      </c>
+      <c r="E278" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F278" t="s">
+        <v>98</v>
+      </c>
+      <c r="G278">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B279" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C279" t="s">
+        <v>1049</v>
+      </c>
+      <c r="E279" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F279" t="s">
+        <v>98</v>
+      </c>
+      <c r="G279">
+        <v>40</v>
+      </c>
+      <c r="H279" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I279" t="s">
+        <v>98</v>
+      </c>
+      <c r="J279" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="280" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B280" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C280" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D280">
+        <v>76</v>
+      </c>
+      <c r="E280" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F280" t="s">
+        <v>100</v>
+      </c>
+      <c r="G280">
+        <v>140</v>
+      </c>
+      <c r="H280" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I280" t="s">
+        <v>100</v>
+      </c>
+      <c r="J280">
+        <v>40</v>
+      </c>
+      <c r="K280" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L280" t="s">
+        <v>100</v>
+      </c>
+      <c r="M280" t="s">
+        <v>119</v>
+      </c>
+      <c r="N280" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O280" t="s">
+        <v>100</v>
+      </c>
+      <c r="P280">
+        <v>2</v>
+      </c>
+      <c r="Q280" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="R280" t="s">
+        <v>100</v>
+      </c>
+      <c r="S280">
+        <v>40</v>
+      </c>
+      <c r="T280" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="U280" t="s">
+        <v>100</v>
+      </c>
+      <c r="V280" t="s">
+        <v>119</v>
+      </c>
+      <c r="W280" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="X280" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y280">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="281" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B281" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C281" t="s">
+        <v>1053</v>
+      </c>
+      <c r="D281">
+        <v>76</v>
+      </c>
+      <c r="E281" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F281" t="s">
+        <v>100</v>
+      </c>
+      <c r="G281">
+        <v>140</v>
+      </c>
+      <c r="H281" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="I281" t="s">
+        <v>100</v>
+      </c>
+      <c r="J281">
+        <v>2</v>
+      </c>
+      <c r="K281" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="L281" t="s">
+        <v>100</v>
+      </c>
+      <c r="M281" t="s">
+        <v>119</v>
+      </c>
+      <c r="N281" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O281" t="s">
+        <v>100</v>
+      </c>
+      <c r="P281">
+        <v>40</v>
+      </c>
+      <c r="Q281" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="R281" t="s">
+        <v>100</v>
+      </c>
+      <c r="S281">
+        <v>2</v>
+      </c>
+      <c r="T281" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="U281" t="s">
+        <v>100</v>
+      </c>
+      <c r="V281" t="s">
+        <v>119</v>
+      </c>
+      <c r="W281" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X281" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y281">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="282" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B282" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C282" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E282" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F282" t="s">
+        <v>98</v>
+      </c>
+      <c r="G282">
+        <v>40</v>
+      </c>
+      <c r="H282" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I282" t="s">
+        <v>98</v>
+      </c>
+      <c r="J282">
+        <v>6</v>
+      </c>
+      <c r="K282" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="L282" t="s">
+        <v>95</v>
+      </c>
+      <c r="M282" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="283" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B283" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C283" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D283">
+        <v>140</v>
+      </c>
+      <c r="E283" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F283" t="s">
+        <v>199</v>
+      </c>
+      <c r="G283">
+        <v>500</v>
+      </c>
+      <c r="H283" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="I283" t="s">
+        <v>199</v>
+      </c>
+      <c r="J283" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="284" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B284" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C284" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D284">
+        <v>80</v>
+      </c>
+      <c r="E284" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F284" t="s">
+        <v>98</v>
+      </c>
+      <c r="G284">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="285" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B285" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C285" t="s">
+        <v>1060</v>
+      </c>
+      <c r="E285" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F285" t="s">
+        <v>144</v>
+      </c>
+      <c r="G285">
+        <v>40</v>
+      </c>
+      <c r="H285" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I285" t="s">
+        <v>144</v>
+      </c>
+      <c r="J285" t="s">
+        <v>142</v>
+      </c>
+      <c r="K285" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L285" t="s">
+        <v>144</v>
+      </c>
+      <c r="M285" t="s">
+        <v>204</v>
+      </c>
+      <c r="N285" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="O285" t="s">
+        <v>144</v>
+      </c>
+      <c r="P285">
+        <v>40</v>
+      </c>
+      <c r="Q285" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="R285" t="s">
+        <v>144</v>
+      </c>
+      <c r="S285" t="s">
+        <v>142</v>
+      </c>
+      <c r="T285" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="U285" t="s">
+        <v>144</v>
+      </c>
+      <c r="V285" t="s">
+        <v>204</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AE246"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="22">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>LUT!$C:$C</xm:f>
           </x14:formula1>
-          <xm:sqref>O2:O69 M47 X2:X1048576 O271:O1048576 U2:U1048576 L268:L1048576 O71:O266 F2:F1048576 I2:I1048576 O268:O269 R121:R1048576 R2:R119 L2:L266</xm:sqref>
+          <xm:sqref>O2:O69 M47 O71:O266 L2:L266 O268:O269 R2:R119 O271:O1048576 F2:F1048576 I2:I1048576 L268:L280 L282:L1048576 R121:R1048576 X2:X1048576 U2:U280 U282:U1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>attributes!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>E274:E1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>H266:H1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E270</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>K264:K1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>N271:N1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>N264:N269</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>H263</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>T264:T1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>AC87</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>K2:K262</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>Z87</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>W2:W87</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>N2:N7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>N9:N69</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>N71:N262</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>Q2:Q119</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>Q121:Q1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>T2:T262</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>W90:W262</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>W264:W1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>attributes!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H261</xm:sqref>
+          <xm:sqref>H2:H261 W90:W262 T2:T262 Q2:Q119 N71:N262 N9:N69 N2:N7 W2:W87 Z87 K2:K262 AC87 H263 N264:N269 E2:E270 E274:E1048576 H266:H1048576 K264:K1048576 N271:N1048576 Q121:Q1048576 W264:W1048576 T264:T1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -13196,13 +13817,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AA100"/>
+  <dimension ref="A1:AA105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B56" sqref="B56"/>
+      <selection pane="bottomRight" activeCell="O106" sqref="O106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -19619,6 +20240,409 @@
       </c>
       <c r="AA100" t="s">
         <v>1032</v>
+      </c>
+    </row>
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B101" t="s">
+        <v>908</v>
+      </c>
+      <c r="C101">
+        <v>20</v>
+      </c>
+      <c r="D101">
+        <v>1478</v>
+      </c>
+      <c r="E101">
+        <v>627</v>
+      </c>
+      <c r="F101">
+        <v>380</v>
+      </c>
+      <c r="G101">
+        <v>3668</v>
+      </c>
+      <c r="H101">
+        <v>1533</v>
+      </c>
+      <c r="I101">
+        <v>950</v>
+      </c>
+      <c r="J101">
+        <v>4323</v>
+      </c>
+      <c r="K101">
+        <v>1728</v>
+      </c>
+      <c r="L101">
+        <v>1085</v>
+      </c>
+      <c r="M101" t="s">
+        <v>923</v>
+      </c>
+      <c r="N101" t="s">
+        <v>928</v>
+      </c>
+      <c r="O101" t="s">
+        <v>976</v>
+      </c>
+      <c r="P101" t="s">
+        <v>974</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>967</v>
+      </c>
+      <c r="R101" t="s">
+        <v>970</v>
+      </c>
+      <c r="S101" t="s">
+        <v>966</v>
+      </c>
+      <c r="T101" t="s">
+        <v>944</v>
+      </c>
+      <c r="U101" t="s">
+        <v>953</v>
+      </c>
+      <c r="V101" t="s">
+        <v>952</v>
+      </c>
+      <c r="W101" t="s">
+        <v>947</v>
+      </c>
+      <c r="X101" t="s">
+        <v>956</v>
+      </c>
+      <c r="Y101" t="s">
+        <v>952</v>
+      </c>
+      <c r="Z101" t="s">
+        <v>952</v>
+      </c>
+      <c r="AA101" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B102" t="s">
+        <v>908</v>
+      </c>
+      <c r="C102">
+        <v>16</v>
+      </c>
+      <c r="D102">
+        <v>1345</v>
+      </c>
+      <c r="E102">
+        <v>530</v>
+      </c>
+      <c r="F102">
+        <v>303</v>
+      </c>
+      <c r="G102">
+        <v>3445</v>
+      </c>
+      <c r="H102">
+        <v>1430</v>
+      </c>
+      <c r="I102">
+        <v>723</v>
+      </c>
+      <c r="J102">
+        <v>4240</v>
+      </c>
+      <c r="K102">
+        <v>1565</v>
+      </c>
+      <c r="L102">
+        <v>868</v>
+      </c>
+      <c r="M102" t="s">
+        <v>926</v>
+      </c>
+      <c r="N102" t="s">
+        <v>927</v>
+      </c>
+      <c r="O102" t="s">
+        <v>976</v>
+      </c>
+      <c r="P102" t="s">
+        <v>974</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>970</v>
+      </c>
+      <c r="R102" t="s">
+        <v>967</v>
+      </c>
+      <c r="S102" t="s">
+        <v>1076</v>
+      </c>
+      <c r="T102" t="s">
+        <v>949</v>
+      </c>
+      <c r="U102" t="s">
+        <v>949</v>
+      </c>
+      <c r="V102" t="s">
+        <v>949</v>
+      </c>
+      <c r="W102" t="s">
+        <v>948</v>
+      </c>
+      <c r="X102" t="s">
+        <v>948</v>
+      </c>
+      <c r="Y102" t="s">
+        <v>948</v>
+      </c>
+      <c r="AA102" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B103" t="s">
+        <v>909</v>
+      </c>
+      <c r="C103">
+        <v>12</v>
+      </c>
+      <c r="D103">
+        <v>1119</v>
+      </c>
+      <c r="E103">
+        <v>405</v>
+      </c>
+      <c r="F103">
+        <v>259</v>
+      </c>
+      <c r="G103">
+        <v>2841</v>
+      </c>
+      <c r="H103">
+        <v>1047</v>
+      </c>
+      <c r="I103">
+        <v>691</v>
+      </c>
+      <c r="J103">
+        <v>3381</v>
+      </c>
+      <c r="K103">
+        <v>1192</v>
+      </c>
+      <c r="L103">
+        <v>801</v>
+      </c>
+      <c r="M103" t="s">
+        <v>926</v>
+      </c>
+      <c r="N103" t="s">
+        <v>931</v>
+      </c>
+      <c r="O103" t="s">
+        <v>981</v>
+      </c>
+      <c r="P103" t="s">
+        <v>973</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>970</v>
+      </c>
+      <c r="R103" t="s">
+        <v>968</v>
+      </c>
+      <c r="S103" t="s">
+        <v>969</v>
+      </c>
+      <c r="T103" t="s">
+        <v>949</v>
+      </c>
+      <c r="U103" t="s">
+        <v>949</v>
+      </c>
+      <c r="V103" t="s">
+        <v>949</v>
+      </c>
+      <c r="W103" t="s">
+        <v>944</v>
+      </c>
+      <c r="X103" t="s">
+        <v>949</v>
+      </c>
+      <c r="Y103" t="s">
+        <v>949</v>
+      </c>
+      <c r="AA103" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B104" t="s">
+        <v>909</v>
+      </c>
+      <c r="C104">
+        <v>29</v>
+      </c>
+      <c r="D104">
+        <v>947</v>
+      </c>
+      <c r="E104">
+        <v>569</v>
+      </c>
+      <c r="F104">
+        <v>244</v>
+      </c>
+      <c r="G104">
+        <v>2453</v>
+      </c>
+      <c r="H104">
+        <v>1415</v>
+      </c>
+      <c r="I104">
+        <v>652</v>
+      </c>
+      <c r="J104">
+        <v>2928</v>
+      </c>
+      <c r="K104">
+        <v>1645</v>
+      </c>
+      <c r="L104">
+        <v>757</v>
+      </c>
+      <c r="M104" t="s">
+        <v>926</v>
+      </c>
+      <c r="N104" t="s">
+        <v>930</v>
+      </c>
+      <c r="O104" t="s">
+        <v>976</v>
+      </c>
+      <c r="P104" t="s">
+        <v>979</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>968</v>
+      </c>
+      <c r="R104" t="s">
+        <v>970</v>
+      </c>
+      <c r="S104" t="s">
+        <v>966</v>
+      </c>
+      <c r="T104" t="s">
+        <v>948</v>
+      </c>
+      <c r="U104" t="s">
+        <v>947</v>
+      </c>
+      <c r="V104" t="s">
+        <v>947</v>
+      </c>
+      <c r="W104" t="s">
+        <v>944</v>
+      </c>
+      <c r="X104" t="s">
+        <v>949</v>
+      </c>
+      <c r="Y104" t="s">
+        <v>952</v>
+      </c>
+      <c r="AA104" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B105" t="s">
+        <v>908</v>
+      </c>
+      <c r="C105">
+        <v>16</v>
+      </c>
+      <c r="D105">
+        <v>1655</v>
+      </c>
+      <c r="E105">
+        <v>467</v>
+      </c>
+      <c r="F105">
+        <v>264</v>
+      </c>
+      <c r="G105">
+        <v>4355</v>
+      </c>
+      <c r="H105">
+        <v>1247</v>
+      </c>
+      <c r="I105">
+        <v>624</v>
+      </c>
+      <c r="J105">
+        <v>5150</v>
+      </c>
+      <c r="K105">
+        <v>1382</v>
+      </c>
+      <c r="L105">
+        <v>769</v>
+      </c>
+      <c r="M105" t="s">
+        <v>926</v>
+      </c>
+      <c r="N105" t="s">
+        <v>927</v>
+      </c>
+      <c r="O105" t="s">
+        <v>963</v>
+      </c>
+      <c r="P105" t="s">
+        <v>1075</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>968</v>
+      </c>
+      <c r="R105" t="s">
+        <v>970</v>
+      </c>
+      <c r="S105" t="s">
+        <v>967</v>
+      </c>
+      <c r="T105" t="s">
+        <v>948</v>
+      </c>
+      <c r="U105" t="s">
+        <v>954</v>
+      </c>
+      <c r="V105" t="s">
+        <v>954</v>
+      </c>
+      <c r="W105" t="s">
+        <v>947</v>
+      </c>
+      <c r="X105" t="s">
+        <v>948</v>
+      </c>
+      <c r="Y105" t="s">
+        <v>952</v>
+      </c>
+      <c r="AA105" t="s">
+        <v>950</v>
       </c>
     </row>
   </sheetData>
@@ -20100,11 +21124,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B158"/>
+  <dimension ref="A1:B160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A50" activeCellId="2" sqref="A46 A49 A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -20211,15 +21235,15 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1015</v>
+        <v>1036</v>
       </c>
       <c r="B13" t="s">
-        <v>173</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="B14" t="s">
         <v>173</v>
@@ -20227,23 +21251,23 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="B15" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>1013</v>
       </c>
       <c r="B16" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>201</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
         <v>173</v>
@@ -20251,7 +21275,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="B18" t="s">
         <v>173</v>
@@ -20259,7 +21283,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B19" t="s">
         <v>173</v>
@@ -20267,7 +21291,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B20" t="s">
         <v>173</v>
@@ -20275,15 +21299,15 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>707</v>
+        <v>209</v>
       </c>
       <c r="B21" t="s">
-        <v>135</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>719</v>
+        <v>707</v>
       </c>
       <c r="B22" t="s">
         <v>135</v>
@@ -20291,7 +21315,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>566</v>
+        <v>719</v>
       </c>
       <c r="B23" t="s">
         <v>135</v>
@@ -20299,7 +21323,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>406</v>
+        <v>566</v>
       </c>
       <c r="B24" t="s">
         <v>135</v>
@@ -20307,23 +21331,23 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>567</v>
+        <v>406</v>
       </c>
       <c r="B25" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="B26" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>708</v>
+        <v>565</v>
       </c>
       <c r="B27" t="s">
         <v>135</v>
@@ -20331,7 +21355,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>718</v>
+        <v>708</v>
       </c>
       <c r="B28" t="s">
         <v>135</v>
@@ -20339,23 +21363,23 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>170</v>
+        <v>718</v>
       </c>
       <c r="B29" t="s">
-        <v>173</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>170</v>
       </c>
       <c r="B30" t="s">
-        <v>132</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
         <v>132</v>
@@ -20363,7 +21387,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1002</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s">
         <v>132</v>
@@ -20371,7 +21395,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>171</v>
+        <v>1039</v>
       </c>
       <c r="B33" t="s">
         <v>132</v>
@@ -20379,7 +21403,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>801</v>
+        <v>1002</v>
       </c>
       <c r="B34" t="s">
         <v>132</v>
@@ -20387,7 +21411,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>171</v>
       </c>
       <c r="B35" t="s">
         <v>132</v>
@@ -20395,7 +21419,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>801</v>
       </c>
       <c r="B36" t="s">
         <v>132</v>
@@ -20403,7 +21427,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B37" t="s">
         <v>132</v>
@@ -20411,7 +21435,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B38" t="s">
         <v>132</v>
@@ -20419,15 +21443,15 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B40" t="s">
         <v>132</v>
@@ -20435,15 +21459,15 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B41" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B42" t="s">
         <v>132</v>
@@ -20451,7 +21475,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B43" t="s">
         <v>132</v>
@@ -20459,23 +21483,23 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>407</v>
+        <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>31</v>
+        <v>407</v>
       </c>
       <c r="B46" t="s">
         <v>133</v>
@@ -20483,7 +21507,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B47" t="s">
         <v>133</v>
@@ -20491,7 +21515,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B48" t="s">
         <v>133</v>
@@ -20499,7 +21523,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B49" t="s">
         <v>133</v>
@@ -20507,7 +21531,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B50" t="s">
         <v>133</v>
@@ -20515,7 +21539,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>284</v>
+        <v>24</v>
       </c>
       <c r="B51" t="s">
         <v>133</v>
@@ -20523,7 +21547,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>283</v>
+        <v>25</v>
       </c>
       <c r="B52" t="s">
         <v>133</v>
@@ -20531,7 +21555,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>26</v>
+        <v>284</v>
       </c>
       <c r="B53" t="s">
         <v>133</v>
@@ -20539,7 +21563,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>27</v>
+        <v>283</v>
       </c>
       <c r="B54" t="s">
         <v>133</v>
@@ -20547,7 +21571,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>286</v>
+        <v>26</v>
       </c>
       <c r="B55" t="s">
         <v>133</v>
@@ -20555,7 +21579,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>285</v>
+        <v>27</v>
       </c>
       <c r="B56" t="s">
         <v>133</v>
@@ -20563,7 +21587,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>28</v>
+        <v>286</v>
       </c>
       <c r="B57" t="s">
         <v>133</v>
@@ -20571,7 +21595,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>29</v>
+        <v>285</v>
       </c>
       <c r="B58" t="s">
         <v>133</v>
@@ -20579,7 +21603,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B59" t="s">
         <v>133</v>
@@ -20587,7 +21611,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B60" t="s">
         <v>133</v>
@@ -20595,7 +21619,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B61" t="s">
         <v>133</v>
@@ -20603,7 +21627,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1029</v>
+        <v>30</v>
       </c>
       <c r="B62" t="s">
         <v>133</v>
@@ -20611,7 +21635,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="B63" t="s">
         <v>133</v>
@@ -20619,7 +21643,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>55</v>
+        <v>1029</v>
       </c>
       <c r="B64" t="s">
         <v>133</v>
@@ -20627,7 +21651,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B65" t="s">
         <v>133</v>
@@ -20635,7 +21659,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B66" t="s">
         <v>133</v>
@@ -20643,7 +21667,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B67" t="s">
         <v>133</v>
@@ -20651,7 +21675,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B68" t="s">
         <v>133</v>
@@ -20659,7 +21683,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B69" t="s">
         <v>133</v>
@@ -20667,7 +21691,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B70" t="s">
         <v>133</v>
@@ -20675,7 +21699,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B71" t="s">
         <v>133</v>
@@ -20683,7 +21707,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>408</v>
+        <v>75</v>
       </c>
       <c r="B72" t="s">
         <v>133</v>
@@ -20691,7 +21715,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B73" t="s">
         <v>133</v>
@@ -20699,7 +21723,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>78</v>
+        <v>408</v>
       </c>
       <c r="B74" t="s">
         <v>133</v>
@@ -20707,7 +21731,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B75" t="s">
         <v>133</v>
@@ -20715,7 +21739,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B76" t="s">
         <v>133</v>
@@ -20723,7 +21747,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>990</v>
+        <v>79</v>
       </c>
       <c r="B77" t="s">
         <v>133</v>
@@ -20731,7 +21755,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>991</v>
+        <v>80</v>
       </c>
       <c r="B78" t="s">
         <v>133</v>
@@ -20739,7 +21763,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>301</v>
+        <v>990</v>
       </c>
       <c r="B79" t="s">
         <v>133</v>
@@ -20747,7 +21771,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>300</v>
+        <v>991</v>
       </c>
       <c r="B80" t="s">
         <v>133</v>
@@ -20755,7 +21779,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>992</v>
+        <v>301</v>
       </c>
       <c r="B81" t="s">
         <v>133</v>
@@ -20763,7 +21787,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>993</v>
+        <v>300</v>
       </c>
       <c r="B82" t="s">
         <v>133</v>
@@ -20771,7 +21795,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>992</v>
       </c>
       <c r="B83" t="s">
         <v>133</v>
@@ -20779,7 +21803,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>993</v>
       </c>
       <c r="B84" t="s">
         <v>133</v>
@@ -20787,23 +21811,23 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>2</v>
+        <v>81</v>
       </c>
       <c r="B85" t="s">
-        <v>173</v>
+        <v>133</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>172</v>
+        <v>82</v>
       </c>
       <c r="B86" t="s">
-        <v>173</v>
+        <v>133</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>205</v>
+        <v>2</v>
       </c>
       <c r="B87" t="s">
         <v>173</v>
@@ -20811,7 +21835,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
       <c r="B88" t="s">
         <v>173</v>
@@ -20819,23 +21843,23 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>355</v>
+        <v>205</v>
       </c>
       <c r="B89" t="s">
-        <v>1028</v>
+        <v>173</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>354</v>
+        <v>206</v>
       </c>
       <c r="B90" t="s">
-        <v>1028</v>
+        <v>173</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>137</v>
+        <v>355</v>
       </c>
       <c r="B91" t="s">
         <v>1028</v>
@@ -20843,7 +21867,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>562</v>
+        <v>354</v>
       </c>
       <c r="B92" t="s">
         <v>1028</v>
@@ -20851,7 +21875,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>4</v>
+        <v>137</v>
       </c>
       <c r="B93" t="s">
         <v>1028</v>
@@ -20859,7 +21883,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>3</v>
+        <v>562</v>
       </c>
       <c r="B94" t="s">
         <v>1028</v>
@@ -20867,31 +21891,31 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>149</v>
+        <v>4</v>
       </c>
       <c r="B95" t="s">
-        <v>173</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="B96" t="s">
-        <v>136</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>366</v>
+        <v>149</v>
       </c>
       <c r="B97" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>245</v>
+        <v>40</v>
       </c>
       <c r="B98" t="s">
         <v>136</v>
@@ -20899,7 +21923,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>37</v>
+        <v>366</v>
       </c>
       <c r="B99" t="s">
         <v>136</v>
@@ -20907,7 +21931,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B100" t="s">
         <v>136</v>
@@ -20915,7 +21939,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B101" t="s">
         <v>136</v>
@@ -20923,7 +21947,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>330</v>
+        <v>246</v>
       </c>
       <c r="B102" t="s">
         <v>136</v>
@@ -20931,7 +21955,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>332</v>
+        <v>38</v>
       </c>
       <c r="B103" t="s">
         <v>136</v>
@@ -20939,7 +21963,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>36</v>
+        <v>330</v>
       </c>
       <c r="B104" t="s">
         <v>136</v>
@@ -20947,7 +21971,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B105" t="s">
         <v>136</v>
@@ -20955,7 +21979,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B106" t="s">
         <v>136</v>
@@ -20963,7 +21987,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>42</v>
+        <v>331</v>
       </c>
       <c r="B107" t="s">
         <v>136</v>
@@ -20971,7 +21995,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B108" t="s">
         <v>136</v>
@@ -20979,7 +22003,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B109" t="s">
         <v>136</v>
@@ -20987,7 +22011,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="B110" t="s">
         <v>136</v>
@@ -20995,7 +22019,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B111" t="s">
         <v>136</v>
@@ -21003,7 +22027,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B112" t="s">
         <v>136</v>
@@ -21011,7 +22035,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B113" t="s">
         <v>136</v>
@@ -21019,7 +22043,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B114" t="s">
         <v>136</v>
@@ -21027,7 +22051,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>224</v>
+        <v>46</v>
       </c>
       <c r="B115" t="s">
         <v>136</v>
@@ -21035,7 +22059,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B116" t="s">
         <v>136</v>
@@ -21043,7 +22067,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>48</v>
+        <v>224</v>
       </c>
       <c r="B117" t="s">
         <v>136</v>
@@ -21051,7 +22075,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B118" t="s">
         <v>136</v>
@@ -21059,7 +22083,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B119" t="s">
         <v>136</v>
@@ -21067,7 +22091,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B120" t="s">
         <v>136</v>
@@ -21075,7 +22099,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B121" t="s">
         <v>136</v>
@@ -21083,7 +22107,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B122" t="s">
         <v>136</v>
@@ -21091,15 +22115,15 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>139</v>
+        <v>50</v>
       </c>
       <c r="B123" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="B124" t="s">
         <v>136</v>
@@ -21107,15 +22131,15 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>445</v>
+        <v>139</v>
       </c>
       <c r="B125" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B126" t="s">
         <v>136</v>
@@ -21123,7 +22147,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>85</v>
+        <v>445</v>
       </c>
       <c r="B127" t="s">
         <v>136</v>
@@ -21131,7 +22155,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>141</v>
+        <v>84</v>
       </c>
       <c r="B128" t="s">
         <v>136</v>
@@ -21139,7 +22163,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>356</v>
+        <v>85</v>
       </c>
       <c r="B129" t="s">
         <v>136</v>
@@ -21147,7 +22171,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B130" t="s">
         <v>136</v>
@@ -21155,7 +22179,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>86</v>
+        <v>356</v>
       </c>
       <c r="B131" t="s">
         <v>136</v>
@@ -21163,7 +22187,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="B132" t="s">
         <v>136</v>
@@ -21171,7 +22195,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B133" t="s">
         <v>136</v>
@@ -21179,7 +22203,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B134" t="s">
         <v>136</v>
@@ -21187,7 +22211,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="B135" t="s">
         <v>136</v>
@@ -21195,7 +22219,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="B136" t="s">
         <v>136</v>
@@ -21203,7 +22227,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>998</v>
+        <v>63</v>
       </c>
       <c r="B137" t="s">
         <v>136</v>
@@ -21211,7 +22235,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>1000</v>
+        <v>64</v>
       </c>
       <c r="B138" t="s">
         <v>136</v>
@@ -21219,7 +22243,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="B139" t="s">
         <v>136</v>
@@ -21227,7 +22251,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>65</v>
+        <v>1000</v>
       </c>
       <c r="B140" t="s">
         <v>136</v>
@@ -21235,7 +22259,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>66</v>
+        <v>999</v>
       </c>
       <c r="B141" t="s">
         <v>136</v>
@@ -21243,7 +22267,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B142" t="s">
         <v>136</v>
@@ -21251,7 +22275,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B143" t="s">
         <v>136</v>
@@ -21259,7 +22283,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B144" t="s">
         <v>136</v>
@@ -21267,7 +22291,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B145" t="s">
         <v>136</v>
@@ -21275,7 +22299,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B146" t="s">
         <v>136</v>
@@ -21283,7 +22307,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B147" t="s">
         <v>136</v>
@@ -21291,7 +22315,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>430</v>
+        <v>54</v>
       </c>
       <c r="B148" t="s">
         <v>136</v>
@@ -21299,7 +22323,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B149" t="s">
         <v>136</v>
@@ -21307,7 +22331,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>71</v>
+        <v>430</v>
       </c>
       <c r="B150" t="s">
         <v>136</v>
@@ -21315,7 +22339,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>762</v>
+        <v>70</v>
       </c>
       <c r="B151" t="s">
         <v>136</v>
@@ -21323,7 +22347,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>763</v>
+        <v>71</v>
       </c>
       <c r="B152" t="s">
         <v>136</v>
@@ -21331,7 +22355,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="B153" t="s">
         <v>136</v>
@@ -21339,23 +22363,23 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>574</v>
+        <v>763</v>
       </c>
       <c r="B154" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>576</v>
+        <v>764</v>
       </c>
       <c r="B155" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B156" t="s">
         <v>173</v>
@@ -21363,7 +22387,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>14</v>
+        <v>576</v>
       </c>
       <c r="B157" t="s">
         <v>173</v>
@@ -21371,14 +22395,30 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>11</v>
+        <v>575</v>
       </c>
       <c r="B158" t="s">
         <v>173</v>
       </c>
     </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>14</v>
+      </c>
+      <c r="B159" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>11</v>
+      </c>
+      <c r="B160" t="s">
+        <v>173</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B158">
+  <autoFilter ref="A1:B160">
     <sortState ref="A2:B157">
       <sortCondition ref="A1:A148"/>
     </sortState>

</xml_diff>

<commit_message>
Corrected Zhuge Liang's passive.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11479" windowHeight="10610" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11479" windowHeight="10610"/>
   </bookViews>
   <sheets>
     <sheet name="skills" sheetId="1" r:id="rId1"/>
@@ -3597,8 +3597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE285"/>
   <sheetViews>
-    <sheetView topLeftCell="H262" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H281" sqref="H281"/>
+    <sheetView tabSelected="1" topLeftCell="A262" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L282" sqref="L282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -13657,8 +13657,8 @@
       <c r="I282" t="s">
         <v>98</v>
       </c>
-      <c r="J282">
-        <v>6</v>
+      <c r="J282" t="s">
+        <v>204</v>
       </c>
       <c r="K282" s="1" t="s">
         <v>171</v>
@@ -13666,8 +13666,8 @@
       <c r="L282" t="s">
         <v>95</v>
       </c>
-      <c r="M282" t="s">
-        <v>204</v>
+      <c r="M282">
+        <v>6</v>
       </c>
     </row>
     <row r="283" spans="1:25" x14ac:dyDescent="0.25">
@@ -13819,11 +13819,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AA105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O106" sqref="O106"/>
+      <selection pane="bottomRight" activeCell="N106" sqref="N106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed Zhuge Liang's passive skill.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -19,7 +19,7 @@
     <sheet name="LUT" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">attributes!$A$1:$B$160</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">attributes!$A$1:$B$161</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">skills!$A$1:$AE$246</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">stats!$A$1:$Z$100</definedName>
   </definedNames>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3948" uniqueCount="1077">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3950" uniqueCount="1078">
   <si>
     <t>attributes</t>
   </si>
@@ -3264,6 +3264,9 @@
   </si>
   <si>
     <t>Life Steal</t>
+  </si>
+  <si>
+    <t>immunity_to_stat_attrition_debuffs_turns</t>
   </si>
 </sst>
 </file>
@@ -3597,8 +3600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A262" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L282" sqref="L282"/>
+    <sheetView tabSelected="1" topLeftCell="D262" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N273" sqref="N273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -13661,7 +13664,7 @@
         <v>204</v>
       </c>
       <c r="K282" s="1" t="s">
-        <v>171</v>
+        <v>1077</v>
       </c>
       <c r="L282" t="s">
         <v>95</v>
@@ -13795,7 +13798,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="22">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>LUT!$C:$C</xm:f>
@@ -13806,7 +13809,127 @@
           <x14:formula1>
             <xm:f>attributes!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H261 W90:W262 T2:T262 Q2:Q119 N71:N262 N9:N69 N2:N7 W2:W87 Z87 K2:K262 AC87 H263 N264:N269 E2:E270 E274:E1048576 H266:H1048576 K264:K1048576 N271:N1048576 Q121:Q1048576 W264:W1048576 T264:T1048576</xm:sqref>
+          <xm:sqref>H2:H261</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>W90:W262</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>T2:T262</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q2:Q119</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>N71:N262</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>N9:N69</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>N2:N7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>W2:W87</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>Z87</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>K2:K262</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>AC87</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>H263</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>N264:N269</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E270</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>E274:E1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>H266:H1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>K264:K1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>N271:N1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q121:Q1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>W264:W1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>T264:T1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -21124,11 +21247,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B160"/>
+  <dimension ref="A1:B161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A50" activeCellId="2" sqref="A46 A49 A50"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -21491,7 +21614,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>7</v>
+        <v>1077</v>
       </c>
       <c r="B45" t="s">
         <v>132</v>
@@ -21499,15 +21622,15 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>407</v>
+        <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>22</v>
+        <v>407</v>
       </c>
       <c r="B47" t="s">
         <v>133</v>
@@ -21515,7 +21638,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B48" t="s">
         <v>133</v>
@@ -21523,7 +21646,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B49" t="s">
         <v>133</v>
@@ -21531,7 +21654,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B50" t="s">
         <v>133</v>
@@ -21539,7 +21662,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B51" t="s">
         <v>133</v>
@@ -21547,7 +21670,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B52" t="s">
         <v>133</v>
@@ -21555,7 +21678,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>284</v>
+        <v>25</v>
       </c>
       <c r="B53" t="s">
         <v>133</v>
@@ -21563,7 +21686,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B54" t="s">
         <v>133</v>
@@ -21571,7 +21694,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>26</v>
+        <v>283</v>
       </c>
       <c r="B55" t="s">
         <v>133</v>
@@ -21579,7 +21702,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B56" t="s">
         <v>133</v>
@@ -21587,7 +21710,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>286</v>
+        <v>27</v>
       </c>
       <c r="B57" t="s">
         <v>133</v>
@@ -21595,7 +21718,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B58" t="s">
         <v>133</v>
@@ -21603,7 +21726,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>28</v>
+        <v>285</v>
       </c>
       <c r="B59" t="s">
         <v>133</v>
@@ -21611,7 +21734,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B60" t="s">
         <v>133</v>
@@ -21619,7 +21742,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B61" t="s">
         <v>133</v>
@@ -21627,7 +21750,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B62" t="s">
         <v>133</v>
@@ -21635,7 +21758,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B63" t="s">
         <v>133</v>
@@ -21643,7 +21766,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>1029</v>
+        <v>35</v>
       </c>
       <c r="B64" t="s">
         <v>133</v>
@@ -21651,7 +21774,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>56</v>
+        <v>1029</v>
       </c>
       <c r="B65" t="s">
         <v>133</v>
@@ -21659,7 +21782,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B66" t="s">
         <v>133</v>
@@ -21667,7 +21790,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B67" t="s">
         <v>133</v>
@@ -21675,7 +21798,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B68" t="s">
         <v>133</v>
@@ -21683,7 +21806,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B69" t="s">
         <v>133</v>
@@ -21691,7 +21814,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B70" t="s">
         <v>133</v>
@@ -21699,7 +21822,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B71" t="s">
         <v>133</v>
@@ -21707,7 +21830,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B72" t="s">
         <v>133</v>
@@ -21715,7 +21838,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B73" t="s">
         <v>133</v>
@@ -21723,7 +21846,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>408</v>
+        <v>76</v>
       </c>
       <c r="B74" t="s">
         <v>133</v>
@@ -21731,7 +21854,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>408</v>
       </c>
       <c r="B75" t="s">
         <v>133</v>
@@ -21739,7 +21862,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B76" t="s">
         <v>133</v>
@@ -21747,7 +21870,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B77" t="s">
         <v>133</v>
@@ -21755,7 +21878,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B78" t="s">
         <v>133</v>
@@ -21763,7 +21886,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>990</v>
+        <v>80</v>
       </c>
       <c r="B79" t="s">
         <v>133</v>
@@ -21771,7 +21894,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B80" t="s">
         <v>133</v>
@@ -21779,7 +21902,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>301</v>
+        <v>991</v>
       </c>
       <c r="B81" t="s">
         <v>133</v>
@@ -21787,7 +21910,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B82" t="s">
         <v>133</v>
@@ -21795,7 +21918,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>992</v>
+        <v>300</v>
       </c>
       <c r="B83" t="s">
         <v>133</v>
@@ -21803,7 +21926,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="B84" t="s">
         <v>133</v>
@@ -21811,7 +21934,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>81</v>
+        <v>993</v>
       </c>
       <c r="B85" t="s">
         <v>133</v>
@@ -21819,7 +21942,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B86" t="s">
         <v>133</v>
@@ -21827,15 +21950,15 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="B87" t="s">
-        <v>173</v>
+        <v>133</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>172</v>
+        <v>2</v>
       </c>
       <c r="B88" t="s">
         <v>173</v>
@@ -21843,7 +21966,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>205</v>
+        <v>172</v>
       </c>
       <c r="B89" t="s">
         <v>173</v>
@@ -21851,7 +21974,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B90" t="s">
         <v>173</v>
@@ -21859,15 +21982,15 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>355</v>
+        <v>206</v>
       </c>
       <c r="B91" t="s">
-        <v>1028</v>
+        <v>173</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B92" t="s">
         <v>1028</v>
@@ -21875,7 +21998,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>137</v>
+        <v>354</v>
       </c>
       <c r="B93" t="s">
         <v>1028</v>
@@ -21883,7 +22006,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>562</v>
+        <v>137</v>
       </c>
       <c r="B94" t="s">
         <v>1028</v>
@@ -21891,7 +22014,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>4</v>
+        <v>562</v>
       </c>
       <c r="B95" t="s">
         <v>1028</v>
@@ -21899,7 +22022,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B96" t="s">
         <v>1028</v>
@@ -21907,23 +22030,23 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>149</v>
+        <v>3</v>
       </c>
       <c r="B97" t="s">
-        <v>173</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>40</v>
+        <v>149</v>
       </c>
       <c r="B98" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>366</v>
+        <v>40</v>
       </c>
       <c r="B99" t="s">
         <v>136</v>
@@ -21931,7 +22054,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>245</v>
+        <v>366</v>
       </c>
       <c r="B100" t="s">
         <v>136</v>
@@ -21939,7 +22062,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>37</v>
+        <v>245</v>
       </c>
       <c r="B101" t="s">
         <v>136</v>
@@ -21947,7 +22070,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>246</v>
+        <v>37</v>
       </c>
       <c r="B102" t="s">
         <v>136</v>
@@ -21955,7 +22078,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>38</v>
+        <v>246</v>
       </c>
       <c r="B103" t="s">
         <v>136</v>
@@ -21963,7 +22086,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>330</v>
+        <v>38</v>
       </c>
       <c r="B104" t="s">
         <v>136</v>
@@ -21971,7 +22094,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B105" t="s">
         <v>136</v>
@@ -21979,7 +22102,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>36</v>
+        <v>332</v>
       </c>
       <c r="B106" t="s">
         <v>136</v>
@@ -21987,7 +22110,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>331</v>
+        <v>36</v>
       </c>
       <c r="B107" t="s">
         <v>136</v>
@@ -21995,7 +22118,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>41</v>
+        <v>331</v>
       </c>
       <c r="B108" t="s">
         <v>136</v>
@@ -22003,7 +22126,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B109" t="s">
         <v>136</v>
@@ -22011,7 +22134,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B110" t="s">
         <v>136</v>
@@ -22019,7 +22142,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B111" t="s">
         <v>136</v>
@@ -22027,7 +22150,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="B112" t="s">
         <v>136</v>
@@ -22035,7 +22158,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B113" t="s">
         <v>136</v>
@@ -22043,7 +22166,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B114" t="s">
         <v>136</v>
@@ -22051,7 +22174,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B115" t="s">
         <v>136</v>
@@ -22059,7 +22182,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B116" t="s">
         <v>136</v>
@@ -22067,7 +22190,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>224</v>
+        <v>60</v>
       </c>
       <c r="B117" t="s">
         <v>136</v>
@@ -22075,7 +22198,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>47</v>
+        <v>224</v>
       </c>
       <c r="B118" t="s">
         <v>136</v>
@@ -22083,7 +22206,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B119" t="s">
         <v>136</v>
@@ -22091,7 +22214,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B120" t="s">
         <v>136</v>
@@ -22099,7 +22222,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B121" t="s">
         <v>136</v>
@@ -22107,7 +22230,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B122" t="s">
         <v>136</v>
@@ -22115,7 +22238,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B123" t="s">
         <v>136</v>
@@ -22123,7 +22246,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B124" t="s">
         <v>136</v>
@@ -22131,23 +22254,23 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>139</v>
+        <v>51</v>
       </c>
       <c r="B125" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>83</v>
+        <v>139</v>
       </c>
       <c r="B126" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>445</v>
+        <v>83</v>
       </c>
       <c r="B127" t="s">
         <v>136</v>
@@ -22155,7 +22278,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>84</v>
+        <v>445</v>
       </c>
       <c r="B128" t="s">
         <v>136</v>
@@ -22163,7 +22286,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B129" t="s">
         <v>136</v>
@@ -22171,7 +22294,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
       <c r="B130" t="s">
         <v>136</v>
@@ -22179,7 +22302,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>356</v>
+        <v>141</v>
       </c>
       <c r="B131" t="s">
         <v>136</v>
@@ -22187,7 +22310,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>140</v>
+        <v>356</v>
       </c>
       <c r="B132" t="s">
         <v>136</v>
@@ -22195,7 +22318,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>86</v>
+        <v>140</v>
       </c>
       <c r="B133" t="s">
         <v>136</v>
@@ -22203,7 +22326,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B134" t="s">
         <v>136</v>
@@ -22211,7 +22334,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B135" t="s">
         <v>136</v>
@@ -22219,7 +22342,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B136" t="s">
         <v>136</v>
@@ -22227,7 +22350,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="B137" t="s">
         <v>136</v>
@@ -22235,7 +22358,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B138" t="s">
         <v>136</v>
@@ -22243,7 +22366,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>998</v>
+        <v>64</v>
       </c>
       <c r="B139" t="s">
         <v>136</v>
@@ -22251,7 +22374,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="B140" t="s">
         <v>136</v>
@@ -22259,7 +22382,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="B141" t="s">
         <v>136</v>
@@ -22267,7 +22390,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>65</v>
+        <v>999</v>
       </c>
       <c r="B142" t="s">
         <v>136</v>
@@ -22275,7 +22398,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B143" t="s">
         <v>136</v>
@@ -22283,7 +22406,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B144" t="s">
         <v>136</v>
@@ -22291,7 +22414,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B145" t="s">
         <v>136</v>
@@ -22299,7 +22422,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B146" t="s">
         <v>136</v>
@@ -22307,7 +22430,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B147" t="s">
         <v>136</v>
@@ -22315,7 +22438,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B148" t="s">
         <v>136</v>
@@ -22323,7 +22446,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B149" t="s">
         <v>136</v>
@@ -22331,7 +22454,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>430</v>
+        <v>69</v>
       </c>
       <c r="B150" t="s">
         <v>136</v>
@@ -22339,7 +22462,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>70</v>
+        <v>430</v>
       </c>
       <c r="B151" t="s">
         <v>136</v>
@@ -22347,7 +22470,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B152" t="s">
         <v>136</v>
@@ -22355,7 +22478,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>762</v>
+        <v>71</v>
       </c>
       <c r="B153" t="s">
         <v>136</v>
@@ -22363,7 +22486,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B154" t="s">
         <v>136</v>
@@ -22371,7 +22494,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B155" t="s">
         <v>136</v>
@@ -22379,15 +22502,15 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>574</v>
+        <v>764</v>
       </c>
       <c r="B156" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B157" t="s">
         <v>173</v>
@@ -22395,7 +22518,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B158" t="s">
         <v>173</v>
@@ -22403,7 +22526,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>14</v>
+        <v>575</v>
       </c>
       <c r="B159" t="s">
         <v>173</v>
@@ -22411,14 +22534,22 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B160" t="s">
         <v>173</v>
       </c>
     </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>11</v>
+      </c>
+      <c r="B161" t="s">
+        <v>173</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B160">
+  <autoFilter ref="A1:B161">
     <sortState ref="A2:B157">
       <sortCondition ref="A1:A148"/>
     </sortState>

</xml_diff>

<commit_message>
Hit count fully integrated into mechanics.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11479" windowHeight="10610" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11479" windowHeight="10610"/>
   </bookViews>
   <sheets>
     <sheet name="skills" sheetId="1" r:id="rId1"/>
@@ -3618,8 +3618,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AF285"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+    <sheetView tabSelected="1" topLeftCell="A263" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C280" sqref="C280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -14325,7 +14325,7 @@
       </c>
       <c r="E280">
         <f>IF(ISBLANK(VLOOKUP(A280,_ext_hit_count!A:B,2,FALSE)), -1, VLOOKUP(A280,_ext_hit_count!A:B,2,FALSE))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F280" s="1" t="s">
         <v>118</v>
@@ -14406,7 +14406,7 @@
       </c>
       <c r="E281">
         <f>IF(ISBLANK(VLOOKUP(A281,_ext_hit_count!A:B,2,FALSE)), -1, VLOOKUP(A281,_ext_hit_count!A:B,2,FALSE))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F281" s="1" t="s">
         <v>118</v>
@@ -14672,7 +14672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -21930,7 +21930,7 @@
   <dimension ref="A1:B208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -23076,8 +23076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B208"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1001"/>
+    <sheetView topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -24431,7 +24431,7 @@
         <v>1049</v>
       </c>
       <c r="B205">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
@@ -24439,7 +24439,7 @@
         <v>1066</v>
       </c>
       <c r="B206">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Corrected flipped Joker's skills.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -3618,8 +3618,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AF285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A263" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C280" sqref="C280"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -6684,7 +6684,7 @@
       </c>
       <c r="E77">
         <f>IF(ISBLANK(VLOOKUP(A77,_ext_hit_count!A:B,2,FALSE)), -1, VLOOKUP(A77,_ext_hit_count!A:B,2,FALSE))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>118</v>
@@ -6729,7 +6729,7 @@
       </c>
       <c r="E78">
         <f>IF(ISBLANK(VLOOKUP(A78,_ext_hit_count!A:B,2,FALSE)), -1, VLOOKUP(A78,_ext_hit_count!A:B,2,FALSE))</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>118</v>
@@ -23076,8 +23076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B208"/>
   <sheetViews>
-    <sheetView topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B208"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -23506,7 +23506,7 @@
         <v>339</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -23514,7 +23514,7 @@
         <v>341</v>
       </c>
       <c r="B54">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed Berserk to Zombie, Lubu's invincibility to Void Shield. Accomodates both types of Void Shield.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11479" windowHeight="10610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11479" windowHeight="10610" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="skills" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4371" uniqueCount="1083">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4375" uniqueCount="1085">
   <si>
     <t>attributes</t>
   </si>
@@ -3284,6 +3284,12 @@
   </si>
   <si>
     <t>Green Shield</t>
+  </si>
+  <si>
+    <t>void_shield_attack_based_attack_count</t>
+  </si>
+  <si>
+    <t>void_shield_hit_based_hit_count</t>
   </si>
 </sst>
 </file>
@@ -3615,11 +3621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AF285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView topLeftCell="F265" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I270" sqref="I270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3838,7 +3843,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>176</v>
       </c>
@@ -3957,7 +3962,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>179</v>
       </c>
@@ -4121,7 +4126,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>192</v>
       </c>
@@ -4249,7 +4254,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>182</v>
       </c>
@@ -4377,7 +4382,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>184</v>
       </c>
@@ -4514,7 +4519,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>186</v>
       </c>
@@ -4624,7 +4629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>188</v>
       </c>
@@ -4743,7 +4748,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>190</v>
       </c>
@@ -4853,7 +4858,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>264</v>
       </c>
@@ -4936,7 +4941,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>266</v>
       </c>
@@ -5046,7 +5051,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>268</v>
       </c>
@@ -5165,7 +5170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>270</v>
       </c>
@@ -5257,7 +5262,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>272</v>
       </c>
@@ -5367,7 +5372,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>274</v>
       </c>
@@ -5477,7 +5482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>276</v>
       </c>
@@ -5596,7 +5601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>278</v>
       </c>
@@ -5706,7 +5711,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>280</v>
       </c>
@@ -5816,7 +5821,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>282</v>
       </c>
@@ -5899,7 +5904,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>289</v>
       </c>
@@ -6018,7 +6023,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>295</v>
       </c>
@@ -6110,7 +6115,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>305</v>
       </c>
@@ -6229,7 +6234,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>312</v>
       </c>
@@ -6366,7 +6371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>319</v>
       </c>
@@ -6485,7 +6490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>325</v>
       </c>
@@ -6631,7 +6636,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="76" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>335</v>
       </c>
@@ -6750,7 +6755,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="79" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>342</v>
       </c>
@@ -6869,7 +6874,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="82" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>349</v>
       </c>
@@ -6979,7 +6984,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="85" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>358</v>
       </c>
@@ -7062,7 +7067,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="87" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>361</v>
       </c>
@@ -7229,7 +7234,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="90" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>903</v>
       </c>
@@ -7351,7 +7356,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="93" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>372</v>
       </c>
@@ -7473,7 +7478,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="96" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>376</v>
       </c>
@@ -7583,7 +7588,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="99" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>382</v>
       </c>
@@ -7639,7 +7644,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="101" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>388</v>
       </c>
@@ -7731,7 +7736,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="104" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>394</v>
       </c>
@@ -7832,7 +7837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>400</v>
       </c>
@@ -7924,7 +7929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>414</v>
       </c>
@@ -8037,7 +8042,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>418</v>
       </c>
@@ -8147,7 +8152,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="116" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>425</v>
       </c>
@@ -8266,7 +8271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>434</v>
       </c>
@@ -8421,7 +8426,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>441</v>
       </c>
@@ -8549,7 +8554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>448</v>
       </c>
@@ -8821,7 +8826,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="134" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>468</v>
       </c>
@@ -9021,7 +9026,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>484</v>
       </c>
@@ -9599,7 +9604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>525</v>
       </c>
@@ -10141,7 +10146,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="169" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>556</v>
       </c>
@@ -10242,7 +10247,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="172" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>577</v>
       </c>
@@ -10604,7 +10609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>598</v>
       </c>
@@ -10702,7 +10707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>604</v>
       </c>
@@ -10785,7 +10790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>610</v>
       </c>
@@ -10895,7 +10900,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="190" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>617</v>
       </c>
@@ -11302,7 +11307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>726</v>
       </c>
@@ -11412,7 +11417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="204" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>728</v>
       </c>
@@ -11531,7 +11536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="207" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>730</v>
       </c>
@@ -11776,7 +11781,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="214" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>734</v>
       </c>
@@ -11913,7 +11918,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>736</v>
       </c>
@@ -12023,7 +12028,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>738</v>
       </c>
@@ -12124,7 +12129,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="223" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>740</v>
       </c>
@@ -12234,7 +12239,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="226" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>742</v>
       </c>
@@ -12425,7 +12430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="231" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>745</v>
       </c>
@@ -12535,7 +12540,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="234" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>747</v>
       </c>
@@ -12663,7 +12668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="237" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>749</v>
       </c>
@@ -12770,7 +12775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="240" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>751</v>
       </c>
@@ -12898,7 +12903,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="243" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>753</v>
       </c>
@@ -12999,7 +13004,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="246" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>755</v>
       </c>
@@ -13127,7 +13132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="249" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>782</v>
       </c>
@@ -13228,7 +13233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="252" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>784</v>
       </c>
@@ -13320,7 +13325,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="255" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>786</v>
       </c>
@@ -13421,7 +13426,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="258" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>788</v>
       </c>
@@ -13558,7 +13563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="261" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>1016</v>
       </c>
@@ -13740,7 +13745,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="264" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>1018</v>
       </c>
@@ -13841,7 +13846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="267" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>1020</v>
       </c>
@@ -13951,7 +13956,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="270" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>1022</v>
       </c>
@@ -14070,7 +14075,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="273" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>1061</v>
       </c>
@@ -14090,7 +14095,7 @@
         <v>50</v>
       </c>
       <c r="I273" s="1" t="s">
-        <v>1038</v>
+        <v>1083</v>
       </c>
       <c r="J273" t="s">
         <v>95</v>
@@ -14189,7 +14194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="276" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>1063</v>
       </c>
@@ -14272,7 +14277,7 @@
         <v>0</v>
       </c>
       <c r="F278" s="1" t="s">
-        <v>1038</v>
+        <v>1083</v>
       </c>
       <c r="G278" t="s">
         <v>98</v>
@@ -14281,7 +14286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>1065</v>
       </c>
@@ -14472,7 +14477,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="282" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>1067</v>
       </c>
@@ -14564,7 +14569,7 @@
         <v>0</v>
       </c>
       <c r="F284" s="1" t="s">
-        <v>1038</v>
+        <v>1083</v>
       </c>
       <c r="G284" t="s">
         <v>98</v>
@@ -14573,7 +14578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>1069</v>
       </c>
@@ -14639,13 +14644,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AF285">
-    <filterColumn colId="3">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AF285"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -14660,7 +14659,7 @@
           <x14:formula1>
             <xm:f>attributes!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I261 U264:U1048576 X264:X1048576 R121:R1048576 O271:O1048576 L264:L1048576 I266:I1048576 F274:F1048576 F2:F270 O264:O269 I263 AD87 L2:L262 AA87 X2:X87 O2:O7 O9:O69 O71:O262 R2:R119 U2:U262 X90:X262</xm:sqref>
+          <xm:sqref>I2:I261 U264:U1048576 X264:X1048576 R121:R1048576 O271:O1048576 L264:L1048576 I266:I1048576 X90:X262 F2:F270 O264:O269 I263 AD87 L2:L262 AA87 X2:X87 O2:O7 O9:O69 O71:O262 R2:R119 U2:U262 F274:F1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -14673,7 +14672,7 @@
   <dimension ref="A1:AB105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="AB48" sqref="AB48"/>
@@ -24927,11 +24926,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B161"/>
+  <dimension ref="A1:B163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -26226,6 +26225,22 @@
       </c>
       <c r="B161" t="s">
         <v>173</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B162" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B163" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pre-emptive update for 7K revamp.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11479" windowHeight="10610" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11479" windowHeight="10610"/>
   </bookViews>
   <sheets>
     <sheet name="skills" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4375" uniqueCount="1085">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4388" uniqueCount="1085">
   <si>
     <t>attributes</t>
   </si>
@@ -3623,8 +3623,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF285"/>
   <sheetViews>
-    <sheetView topLeftCell="F265" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I270" sqref="I270"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3804,7 +3807,7 @@
         <v>199</v>
       </c>
       <c r="Q2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
@@ -3916,6 +3919,15 @@
       <c r="N5" t="s">
         <v>119</v>
       </c>
+      <c r="O5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P5" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -3990,6 +4002,15 @@
       <c r="K7" t="s">
         <v>204</v>
       </c>
+      <c r="L7" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="M7" t="s">
+        <v>95</v>
+      </c>
+      <c r="N7">
+        <v>100</v>
+      </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -4018,7 +4039,7 @@
         <v>230</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="J8" t="s">
         <v>199</v>
@@ -4027,49 +4048,22 @@
         <v>2</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>44</v>
+        <v>283</v>
       </c>
       <c r="M8" t="s">
         <v>199</v>
       </c>
       <c r="N8">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="P8" t="s">
         <v>199</v>
       </c>
-      <c r="Q8">
-        <v>2</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="S8" t="s">
-        <v>199</v>
-      </c>
-      <c r="T8">
-        <v>80</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="V8" t="s">
-        <v>199</v>
-      </c>
-      <c r="W8" t="s">
-        <v>142</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>199</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>142</v>
+      <c r="Q8" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
@@ -4099,7 +4093,7 @@
         <v>160</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="J9" t="s">
         <v>100</v>
@@ -4108,22 +4102,49 @@
         <v>2</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>283</v>
+        <v>44</v>
       </c>
       <c r="M9" t="s">
         <v>100</v>
       </c>
       <c r="N9">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="P9" t="s">
         <v>100</v>
       </c>
-      <c r="Q9" t="s">
-        <v>119</v>
+      <c r="Q9">
+        <v>2</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S9" t="s">
+        <v>100</v>
+      </c>
+      <c r="T9">
+        <v>80</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V9" t="s">
+        <v>100</v>
+      </c>
+      <c r="W9" t="s">
+        <v>142</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
@@ -4161,7 +4182,7 @@
         <v>95</v>
       </c>
       <c r="Q10">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>149</v>
@@ -4200,7 +4221,7 @@
         <v>230</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="J11" t="s">
         <v>199</v>
@@ -4230,16 +4251,16 @@
         <v>117</v>
       </c>
       <c r="G12" t="s">
-        <v>144</v>
+        <v>100</v>
       </c>
       <c r="H12">
-        <v>90</v>
+        <v>160</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>80</v>
       </c>
       <c r="J12" t="s">
-        <v>144</v>
+        <v>100</v>
       </c>
       <c r="K12">
         <v>2</v>
@@ -4248,7 +4269,7 @@
         <v>79</v>
       </c>
       <c r="M12" t="s">
-        <v>144</v>
+        <v>100</v>
       </c>
       <c r="N12" t="s">
         <v>119</v>
@@ -4280,7 +4301,7 @@
         <v>98</v>
       </c>
       <c r="K13">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>224</v>
@@ -4316,7 +4337,7 @@
         <v>144</v>
       </c>
       <c r="H14">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>19</v>
@@ -4352,34 +4373,16 @@
         <v>144</v>
       </c>
       <c r="H15">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="J15" t="s">
         <v>144</v>
       </c>
-      <c r="K15">
-        <v>2</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="M15" t="s">
-        <v>144</v>
-      </c>
-      <c r="N15">
-        <v>60</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P15" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>119</v>
+      <c r="K15" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
@@ -4538,6 +4541,33 @@
       <c r="H19">
         <v>2</v>
       </c>
+      <c r="I19" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="J19" t="s">
+        <v>95</v>
+      </c>
+      <c r="K19" t="s">
+        <v>204</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M19" t="s">
+        <v>98</v>
+      </c>
+      <c r="N19">
+        <v>40</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P19" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -4608,7 +4638,7 @@
         <v>144</v>
       </c>
       <c r="H21">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>35</v>
@@ -4647,6 +4677,24 @@
       </c>
       <c r="H22">
         <v>30</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="J22" t="s">
+        <v>95</v>
+      </c>
+      <c r="K22">
+        <v>3</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>1013</v>
+      </c>
+      <c r="M22" t="s">
+        <v>95</v>
+      </c>
+      <c r="N22">
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -14648,18 +14696,30 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>LUT!$C:$C</xm:f>
           </x14:formula1>
-          <xm:sqref>P2:P69 N47 P71:P266 M2:M266 P268:P269 S2:S119 P271:P1048576 G2:G1048576 J2:J1048576 M268:M280 M282:M1048576 S121:S1048576 Y2:Y1048576 V2:V280 V282:V1048576</xm:sqref>
+          <xm:sqref>N47 P71:P266 V282:V1048576 P268:P269 P271:P1048576 G2:G1048576 M268:M280 M282:M1048576 S121:S1048576 J2:J1048576 V2:V7 V9:V280 Y2:Y7 Y9:Y1048576 M2:M266 S2:S7 S9:S119 P2:P69</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>attributes!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I261 U264:U1048576 X264:X1048576 R121:R1048576 O271:O1048576 L264:L1048576 I266:I1048576 X90:X262 F2:F270 O264:O269 I263 AD87 L2:L262 AA87 X2:X87 O2:O7 O9:O69 O71:O262 R2:R119 U2:U262 F274:F1048576</xm:sqref>
+          <xm:sqref>U264:U1048576 X264:X1048576 R121:R1048576 O271:O1048576 L264:L1048576 I266:I1048576 X90:X262 F2:F270 O264:O269 I263 AD87 F274:F1048576 AA87 O2:O7 O71:O262 L2:L7 L10:L262 U2:U7 U10:U262 R2:R7 R10:R119 I10:I261 X2:X7 X10:X87 I2:I7 O10:O69</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>LUT!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>Y8 V8 S8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>I8:I9 X8:X9 O8 R8:R9 U8:U9 L8:L9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -24928,7 +24988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>

</xml_diff>

<commit_message>
Sync GA 1.0.51. Add Xiao. Add Void Shield and Cooldown Modifier on stack table.
</commit_message>
<xml_diff>
--- a/db/seed.xlsx
+++ b/db/seed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11479" windowHeight="10610" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11479" windowHeight="10610"/>
   </bookViews>
   <sheets>
     <sheet name="skills" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="LUT" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">attributes!$A$1:$B$161</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">attributes!$A$1:$B$162</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">skills!$A$1:$AF$285</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">stats!$A$1:$AB$105</definedName>
   </definedNames>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4375" uniqueCount="1085">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4416" uniqueCount="1094">
   <si>
     <t>attributes</t>
   </si>
@@ -3290,6 +3290,33 @@
   </si>
   <si>
     <t>void_shield_hit_based_hit_count</t>
+  </si>
+  <si>
+    <t>xiao_6_0</t>
+  </si>
+  <si>
+    <t>Ownerless Xiao</t>
+  </si>
+  <si>
+    <t>Energy Drain</t>
+  </si>
+  <si>
+    <t>cooldown_increase_amount</t>
+  </si>
+  <si>
+    <t>Arise, Zombie!</t>
+  </si>
+  <si>
+    <t>Zombie's Charm</t>
+  </si>
+  <si>
+    <t>xiao_6_1</t>
+  </si>
+  <si>
+    <t>xiao_6_2</t>
+  </si>
+  <si>
+    <t>xiao_6</t>
   </si>
 </sst>
 </file>
@@ -3621,10 +3648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF285"/>
+  <dimension ref="A1:AF288"/>
   <sheetViews>
-    <sheetView topLeftCell="F265" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I270" sqref="I270"/>
+    <sheetView tabSelected="1" topLeftCell="A255" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G287" sqref="G287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -5702,7 +5729,7 @@
         <v>150</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>76</v>
+        <v>1035</v>
       </c>
       <c r="J51" t="s">
         <v>99</v>
@@ -8363,7 +8390,7 @@
         <v>350</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>76</v>
+        <v>570</v>
       </c>
       <c r="J120" t="s">
         <v>199</v>
@@ -8491,7 +8518,7 @@
         <v>80</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>76</v>
+        <v>1035</v>
       </c>
       <c r="J123" t="s">
         <v>144</v>
@@ -14641,6 +14668,98 @@
       </c>
       <c r="W285" t="s">
         <v>204</v>
+      </c>
+    </row>
+    <row r="286" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B286" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C286" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D286">
+        <v>70</v>
+      </c>
+      <c r="E286">
+        <f>IF(ISBLANK(VLOOKUP(A286,_ext_hit_count!A:B,2,FALSE)), -1, VLOOKUP(A286,_ext_hit_count!A:B,2,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="F286" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G286" t="s">
+        <v>199</v>
+      </c>
+      <c r="H286">
+        <v>190</v>
+      </c>
+      <c r="I286" s="1" t="s">
+        <v>1088</v>
+      </c>
+      <c r="J286" t="s">
+        <v>199</v>
+      </c>
+      <c r="K286">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="287" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B287" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C287" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D287">
+        <v>90</v>
+      </c>
+      <c r="E287">
+        <f>IF(ISBLANK(VLOOKUP(A287,_ext_hit_count!A:B,2,FALSE)), -1, VLOOKUP(A287,_ext_hit_count!A:B,2,FALSE))</f>
+        <v>1</v>
+      </c>
+      <c r="F287" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G287" t="s">
+        <v>144</v>
+      </c>
+      <c r="H287">
+        <v>85</v>
+      </c>
+      <c r="I287" s="1" t="s">
+        <v>1088</v>
+      </c>
+      <c r="J287" t="s">
+        <v>144</v>
+      </c>
+      <c r="K287">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="288" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B288" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C288" t="s">
+        <v>1090</v>
+      </c>
+      <c r="F288" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G288" t="s">
+        <v>95</v>
+      </c>
+      <c r="H288">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -14648,7 +14767,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="22">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>LUT!$C:$C</xm:f>
@@ -14659,7 +14778,127 @@
           <x14:formula1>
             <xm:f>attributes!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I261 U264:U1048576 X264:X1048576 R121:R1048576 O271:O1048576 L264:L1048576 I266:I1048576 X90:X262 F2:F270 O264:O269 I263 AD87 L2:L262 AA87 X2:X87 O2:O7 O9:O69 O71:O262 R2:R119 U2:U262 F274:F1048576</xm:sqref>
+          <xm:sqref>I2:I261</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>U264:U1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>X264:X1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>R121:R1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>O271:O1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>L264:L1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>I266:I1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>X90:X262</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F270</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>O264:O269</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>I263</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>AD87</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>L2:L262</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>AA87</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>X2:X87</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>O2:O7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>O9:O69</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>O71:O262</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>R2:R119</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>U2:U262</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>attributes!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>F274:F1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -14669,13 +14908,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB105"/>
+  <dimension ref="A1:AB106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M89" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB48" sqref="AB48"/>
+      <selection pane="bottomRight" activeCell="S107" sqref="S107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -21917,6 +22156,90 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="106" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B106" t="s">
+        <v>907</v>
+      </c>
+      <c r="C106">
+        <v>29</v>
+      </c>
+      <c r="D106">
+        <v>947</v>
+      </c>
+      <c r="E106">
+        <v>569</v>
+      </c>
+      <c r="F106">
+        <v>244</v>
+      </c>
+      <c r="G106">
+        <v>2453</v>
+      </c>
+      <c r="H106">
+        <v>1415</v>
+      </c>
+      <c r="I106">
+        <v>652</v>
+      </c>
+      <c r="J106">
+        <v>2928</v>
+      </c>
+      <c r="K106">
+        <v>1645</v>
+      </c>
+      <c r="L106">
+        <v>757</v>
+      </c>
+      <c r="M106" t="s">
+        <v>923</v>
+      </c>
+      <c r="N106" t="s">
+        <v>928</v>
+      </c>
+      <c r="O106" t="s">
+        <v>962</v>
+      </c>
+      <c r="P106" t="s">
+        <v>973</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>969</v>
+      </c>
+      <c r="R106" t="s">
+        <v>964</v>
+      </c>
+      <c r="S106" t="s">
+        <v>966</v>
+      </c>
+      <c r="T106" t="s">
+        <v>956</v>
+      </c>
+      <c r="U106" t="s">
+        <v>956</v>
+      </c>
+      <c r="V106" t="s">
+        <v>956</v>
+      </c>
+      <c r="W106" t="s">
+        <v>955</v>
+      </c>
+      <c r="X106" t="s">
+        <v>956</v>
+      </c>
+      <c r="Y106" t="s">
+        <v>951</v>
+      </c>
+      <c r="AA106" t="s">
+        <v>952</v>
+      </c>
+      <c r="AB106">
+        <f>IF(ISBLANK(VLOOKUP(CONCATENATE(A106, "_0"),_ext_crit_hit!A:B,2,FALSE)),-1,VLOOKUP(CONCATENATE(A106, "_0"),_ext_crit_hit!A:B,2,FALSE))</f>
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AB105"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21926,10 +22249,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B208"/>
+  <dimension ref="A1:B210"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="B209" sqref="B209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -23065,6 +23388,19 @@
         <v>1068</v>
       </c>
     </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B209">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>1091</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -23073,10 +23409,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B208"/>
+  <dimension ref="A1:B210"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView topLeftCell="A195" workbookViewId="0">
+      <selection activeCell="B209" sqref="B209:B210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -24455,6 +24791,22 @@
       </c>
       <c r="B208">
         <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B210">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -24926,11 +25278,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B163"/>
+  <dimension ref="A1:B164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -25109,15 +25461,15 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>706</v>
+        <v>1088</v>
       </c>
       <c r="B22" t="s">
-        <v>135</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>718</v>
+        <v>706</v>
       </c>
       <c r="B23" t="s">
         <v>135</v>
@@ -25125,7 +25477,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>565</v>
+        <v>718</v>
       </c>
       <c r="B24" t="s">
         <v>135</v>
@@ -25133,7 +25485,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>406</v>
+        <v>565</v>
       </c>
       <c r="B25" t="s">
         <v>135</v>
@@ -25141,23 +25493,23 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>566</v>
+        <v>406</v>
       </c>
       <c r="B26" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="B27" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>707</v>
+        <v>564</v>
       </c>
       <c r="B28" t="s">
         <v>135</v>
@@ -25165,7 +25517,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>717</v>
+        <v>707</v>
       </c>
       <c r="B29" t="s">
         <v>135</v>
@@ -25173,23 +25525,23 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>170</v>
+        <v>717</v>
       </c>
       <c r="B30" t="s">
-        <v>173</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>170</v>
       </c>
       <c r="B31" t="s">
-        <v>132</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
         <v>132</v>
@@ -25197,7 +25549,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1038</v>
+        <v>15</v>
       </c>
       <c r="B33" t="s">
         <v>132</v>
@@ -25205,7 +25557,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1001</v>
+        <v>1038</v>
       </c>
       <c r="B34" t="s">
         <v>132</v>
@@ -25213,7 +25565,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>171</v>
+        <v>1001</v>
       </c>
       <c r="B35" t="s">
         <v>132</v>
@@ -25221,7 +25573,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>800</v>
+        <v>171</v>
       </c>
       <c r="B36" t="s">
         <v>132</v>
@@ -25229,7 +25581,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>800</v>
       </c>
       <c r="B37" t="s">
         <v>132</v>
@@ -25237,7 +25589,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B38" t="s">
         <v>132</v>
@@ -25245,7 +25597,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="B39" t="s">
         <v>132</v>
@@ -25253,7 +25605,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
         <v>132</v>
@@ -25261,23 +25613,23 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B42" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B43" t="s">
         <v>132</v>
@@ -25285,7 +25637,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B44" t="s">
         <v>132</v>
@@ -25293,7 +25645,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>1076</v>
+        <v>5</v>
       </c>
       <c r="B45" t="s">
         <v>132</v>
@@ -25301,7 +25653,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>7</v>
+        <v>1076</v>
       </c>
       <c r="B46" t="s">
         <v>132</v>
@@ -25309,15 +25661,15 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>407</v>
+        <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>22</v>
+        <v>407</v>
       </c>
       <c r="B48" t="s">
         <v>133</v>
@@ -25325,7 +25677,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B49" t="s">
         <v>133</v>
@@ -25333,7 +25685,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B50" t="s">
         <v>133</v>
@@ -25341,7 +25693,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B51" t="s">
         <v>133</v>
@@ -25349,7 +25701,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B52" t="s">
         <v>133</v>
@@ -25357,7 +25709,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B53" t="s">
         <v>133</v>
@@ -25365,7 +25717,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>284</v>
+        <v>25</v>
       </c>
       <c r="B54" t="s">
         <v>133</v>
@@ -25373,7 +25725,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B55" t="s">
         <v>133</v>
@@ -25381,7 +25733,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>26</v>
+        <v>283</v>
       </c>
       <c r="B56" t="s">
         <v>133</v>
@@ -25389,7 +25741,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B57" t="s">
         <v>133</v>
@@ -25397,7 +25749,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>286</v>
+        <v>27</v>
       </c>
       <c r="B58" t="s">
         <v>133</v>
@@ -25405,7 +25757,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B59" t="s">
         <v>133</v>
@@ -25413,7 +25765,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>28</v>
+        <v>285</v>
       </c>
       <c r="B60" t="s">
         <v>133</v>
@@ -25421,7 +25773,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B61" t="s">
         <v>133</v>
@@ -25429,7 +25781,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B62" t="s">
         <v>133</v>
@@ -25437,7 +25789,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B63" t="s">
         <v>133</v>
@@ -25445,7 +25797,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B64" t="s">
         <v>133</v>
@@ -25453,7 +25805,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>1028</v>
+        <v>35</v>
       </c>
       <c r="B65" t="s">
         <v>133</v>
@@ -25461,7 +25813,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>56</v>
+        <v>1028</v>
       </c>
       <c r="B66" t="s">
         <v>133</v>
@@ -25469,7 +25821,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B67" t="s">
         <v>133</v>
@@ -25477,7 +25829,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B68" t="s">
         <v>133</v>
@@ -25485,7 +25837,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B69" t="s">
         <v>133</v>
@@ -25493,7 +25845,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B70" t="s">
         <v>133</v>
@@ -25501,7 +25853,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B71" t="s">
         <v>133</v>
@@ -25509,7 +25861,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B72" t="s">
         <v>133</v>
@@ -25517,7 +25869,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B73" t="s">
         <v>133</v>
@@ -25525,7 +25877,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B74" t="s">
         <v>133</v>
@@ -25533,7 +25885,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>408</v>
+        <v>76</v>
       </c>
       <c r="B75" t="s">
         <v>133</v>
@@ -25541,7 +25893,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>77</v>
+        <v>408</v>
       </c>
       <c r="B76" t="s">
         <v>133</v>
@@ -25549,7 +25901,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B77" t="s">
         <v>133</v>
@@ -25557,7 +25909,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B78" t="s">
         <v>133</v>
@@ -25565,7 +25917,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B79" t="s">
         <v>133</v>
@@ -25573,7 +25925,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>989</v>
+        <v>80</v>
       </c>
       <c r="B80" t="s">
         <v>133</v>
@@ -25581,7 +25933,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B81" t="s">
         <v>133</v>
@@ -25589,7 +25941,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>301</v>
+        <v>990</v>
       </c>
       <c r="B82" t="s">
         <v>133</v>
@@ -25597,7 +25949,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B83" t="s">
         <v>133</v>
@@ -25605,7 +25957,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>991</v>
+        <v>300</v>
       </c>
       <c r="B84" t="s">
         <v>133</v>
@@ -25613,7 +25965,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B85" t="s">
         <v>133</v>
@@ -25621,7 +25973,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>81</v>
+        <v>992</v>
       </c>
       <c r="B86" t="s">
         <v>133</v>
@@ -25629,7 +25981,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B87" t="s">
         <v>133</v>
@@ -25637,15 +25989,15 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="B88" t="s">
-        <v>173</v>
+        <v>133</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>172</v>
+        <v>2</v>
       </c>
       <c r="B89" t="s">
         <v>173</v>
@@ -25653,7 +26005,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>205</v>
+        <v>172</v>
       </c>
       <c r="B90" t="s">
         <v>173</v>
@@ -25661,7 +26013,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B91" t="s">
         <v>173</v>
@@ -25669,15 +26021,15 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>355</v>
+        <v>206</v>
       </c>
       <c r="B92" t="s">
-        <v>1027</v>
+        <v>173</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B93" t="s">
         <v>1027</v>
@@ -25685,7 +26037,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>137</v>
+        <v>354</v>
       </c>
       <c r="B94" t="s">
         <v>1027</v>
@@ -25693,7 +26045,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>561</v>
+        <v>137</v>
       </c>
       <c r="B95" t="s">
         <v>1027</v>
@@ -25701,7 +26053,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>4</v>
+        <v>561</v>
       </c>
       <c r="B96" t="s">
         <v>1027</v>
@@ -25709,7 +26061,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B97" t="s">
         <v>1027</v>
@@ -25717,23 +26069,23 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>149</v>
+        <v>3</v>
       </c>
       <c r="B98" t="s">
-        <v>173</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>40</v>
+        <v>149</v>
       </c>
       <c r="B99" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>366</v>
+        <v>40</v>
       </c>
       <c r="B100" t="s">
         <v>136</v>
@@ -25741,7 +26093,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>245</v>
+        <v>366</v>
       </c>
       <c r="B101" t="s">
         <v>136</v>
@@ -25749,7 +26101,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>37</v>
+        <v>245</v>
       </c>
       <c r="B102" t="s">
         <v>136</v>
@@ -25757,7 +26109,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>246</v>
+        <v>37</v>
       </c>
       <c r="B103" t="s">
         <v>136</v>
@@ -25765,7 +26117,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>38</v>
+        <v>246</v>
       </c>
       <c r="B104" t="s">
         <v>136</v>
@@ -25773,7 +26125,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>330</v>
+        <v>38</v>
       </c>
       <c r="B105" t="s">
         <v>136</v>
@@ -25781,7 +26133,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B106" t="s">
         <v>136</v>
@@ -25789,7 +26141,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>36</v>
+        <v>332</v>
       </c>
       <c r="B107" t="s">
         <v>136</v>
@@ -25797,7 +26149,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>331</v>
+        <v>36</v>
       </c>
       <c r="B108" t="s">
         <v>136</v>
@@ -25805,7 +26157,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>41</v>
+        <v>331</v>
       </c>
       <c r="B109" t="s">
         <v>136</v>
@@ -25813,7 +26165,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B110" t="s">
         <v>136</v>
@@ -25821,7 +26173,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B111" t="s">
         <v>136</v>
@@ -25829,7 +26181,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B112" t="s">
         <v>136</v>
@@ -25837,7 +26189,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="B113" t="s">
         <v>136</v>
@@ -25845,7 +26197,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B114" t="s">
         <v>136</v>
@@ -25853,7 +26205,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B115" t="s">
         <v>136</v>
@@ -25861,7 +26213,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B116" t="s">
         <v>136</v>
@@ -25869,7 +26221,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B117" t="s">
         <v>136</v>
@@ -25877,7 +26229,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>224</v>
+        <v>60</v>
       </c>
       <c r="B118" t="s">
         <v>136</v>
@@ -25885,7 +26237,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>47</v>
+        <v>224</v>
       </c>
       <c r="B119" t="s">
         <v>136</v>
@@ -25893,7 +26245,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B120" t="s">
         <v>136</v>
@@ -25901,7 +26253,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B121" t="s">
         <v>136</v>
@@ -25909,7 +26261,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B122" t="s">
         <v>136</v>
@@ -25917,7 +26269,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B123" t="s">
         <v>136</v>
@@ -25925,7 +26277,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B124" t="s">
         <v>136</v>
@@ -25933,7 +26285,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B125" t="s">
         <v>136</v>
@@ -25941,23 +26293,23 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>139</v>
+        <v>51</v>
       </c>
       <c r="B126" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>83</v>
+        <v>139</v>
       </c>
       <c r="B127" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>445</v>
+        <v>83</v>
       </c>
       <c r="B128" t="s">
         <v>136</v>
@@ -25965,7 +26317,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>84</v>
+        <v>445</v>
       </c>
       <c r="B129" t="s">
         <v>136</v>
@@ -25973,7 +26325,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B130" t="s">
         <v>136</v>
@@ -25981,7 +26333,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
       <c r="B131" t="s">
         <v>136</v>
@@ -25989,7 +26341,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>356</v>
+        <v>141</v>
       </c>
       <c r="B132" t="s">
         <v>136</v>
@@ -25997,7 +26349,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>140</v>
+        <v>356</v>
       </c>
       <c r="B133" t="s">
         <v>136</v>
@@ -26005,7 +26357,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>86</v>
+        <v>140</v>
       </c>
       <c r="B134" t="s">
         <v>136</v>
@@ -26013,7 +26365,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B135" t="s">
         <v>136</v>
@@ -26021,7 +26373,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B136" t="s">
         <v>136</v>
@@ -26029,7 +26381,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B137" t="s">
         <v>136</v>
@@ -26037,7 +26389,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="B138" t="s">
         <v>136</v>
@@ -26045,7 +26397,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B139" t="s">
         <v>136</v>
@@ -26053,7 +26405,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>997</v>
+        <v>64</v>
       </c>
       <c r="B140" t="s">
         <v>136</v>
@@ -26061,7 +26413,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="B141" t="s">
         <v>136</v>
@@ -26069,7 +26421,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B142" t="s">
         <v>136</v>
@@ -26077,7 +26429,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>65</v>
+        <v>998</v>
       </c>
       <c r="B143" t="s">
         <v>136</v>
@@ -26085,7 +26437,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B144" t="s">
         <v>136</v>
@@ -26093,7 +26445,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B145" t="s">
         <v>136</v>
@@ -26101,7 +26453,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B146" t="s">
         <v>136</v>
@@ -26109,7 +26461,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B147" t="s">
         <v>136</v>
@@ -26117,7 +26469,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B148" t="s">
         <v>136</v>
@@ -26125,7 +26477,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B149" t="s">
         <v>136</v>
@@ -26133,7 +26485,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B150" t="s">
         <v>136</v>
@@ -26141,7 +26493,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>430</v>
+        <v>69</v>
       </c>
       <c r="B151" t="s">
         <v>136</v>
@@ -26149,7 +26501,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>70</v>
+        <v>430</v>
       </c>
       <c r="B152" t="s">
         <v>136</v>
@@ -26157,7 +26509,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B153" t="s">
         <v>136</v>
@@ -26165,7 +26517,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>761</v>
+        <v>71</v>
       </c>
       <c r="B154" t="s">
         <v>136</v>
@@ -26173,7 +26525,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B155" t="s">
         <v>136</v>
@@ -26181,7 +26533,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B156" t="s">
         <v>136</v>
@@ -26189,15 +26541,15 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>573</v>
+        <v>763</v>
       </c>
       <c r="B157" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B158" t="s">
         <v>173</v>
@@ -26205,7 +26557,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B159" t="s">
         <v>173</v>
@@ -26213,7 +26565,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>14</v>
+        <v>574</v>
       </c>
       <c r="B160" t="s">
         <v>173</v>
@@ -26221,7 +26573,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B161" t="s">
         <v>173</v>
@@ -26229,22 +26581,30 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>1083</v>
+        <v>11</v>
       </c>
       <c r="B162" t="s">
-        <v>132</v>
+        <v>173</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B163" t="s">
         <v>132</v>
       </c>
     </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B164" t="s">
+        <v>132</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B161">
+  <autoFilter ref="A1:B162">
     <sortState ref="A2:B157">
       <sortCondition ref="A1:A148"/>
     </sortState>

</xml_diff>